<commit_message>
+ Update sql scripts
</commit_message>
<xml_diff>
--- a/面试高频题.xlsx
+++ b/面试高频题.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F9909A-B4DD-4B8A-8C44-9E5B393B629D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="2475" windowWidth="23760" windowHeight="10500" tabRatio="539"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$225</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
@@ -1888,562 +1889,564 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>树，递归，深搜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树，递归，深搜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/flatten-binary-tree-to-linked-list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/pascals-triangle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/pascals-triangle-ii</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树，深搜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/flatten-binary-tree-to-linked-list/solution/er-cha-shu-zhan-kai-wei-lian-biao-by-leetcode-solu/</t>
+  </si>
+  <si>
+    <t>数组，动态规划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/pascals-triangle/solution/yang-hui-san-jiao-by-leetcode/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/pascals-triangle-ii/solution/119yang-hui-san-jiao-ii-dong-tai-gui-hua-by-ceng-j/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/best-time-to-buy-and-sell-stock</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/best-time-to-buy-and-sell-stock-ii</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/valid-palindrome</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/best-time-to-buy-and-sell-stock/solution/121-mai-mai-gu-piao-de-zui-jia-shi-ji-by-leetcode-/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/best-time-to-buy-and-sell-stock-ii/solution/mai-mai-gu-piao-de-zui-jia-shi-ji-ii-by-leetcode/</t>
+  </si>
+  <si>
+    <t>数组，贪心，动态规划，单调栈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串，双指针</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/valid-palindrome/solution/yan-zheng-hui-wen-chuan-by-leetcode-solution/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/single-number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/single-number-ii</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/word-break</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/single-number/solution/zhi-chu-xian-yi-ci-de-shu-zi-by-leetcode-solution/</t>
+  </si>
+  <si>
+    <t>数组，集合，哈希表，位运算</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/single-number-ii/solution/luo-ji-dian-lu-jiao-du-xiang-xi-fen-xi-gai-ti-si-l/</t>
+  </si>
+  <si>
+    <t>数组，位运算，数学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数组，动态规划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/word-break/solution/dong-tai-gui-hua-ji-yi-hua-hui-su-zhu-xing-jie-shi/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/linked-list-cycle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/linked-list-cycle-ii</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/reorder-list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/linked-list-cycle/solution/huan-xing-lian-biao-by-leetcode/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/linked-list-cycle-ii/solution/linked-list-cycle-ii-kuai-man-zhi-zhen-shuang-zhi-/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/reorder-list/solution/3ge-bu-zou-jian-dan-yi-dong-by-wang_dong/</t>
+  </si>
+  <si>
+    <t>链表，双指针</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/binary-tree-preorder-traversal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/lru-cache</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/sort-list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树，递归</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/binary-tree-preorder-traversal/solution/leetcodesuan-fa-xiu-lian-dong-hua-yan-shi-xbian-2/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/lru-cache/solution/lruhuan-cun-ji-zhi-by-leetcode-solution/</t>
+  </si>
+  <si>
+    <t>设计，哈希表，链表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/evaluate-reverse-polish-notation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/maximum-product-subarray</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>链表，排序，归并</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/sort-list/solution/148-pai-xu-lian-biao-bottom-to-up-o1-kong-jian-by-/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/sort-list/solution/lioney-cgui-bing-pai-xu-lian-biao-by-lioney/</t>
+  </si>
+  <si>
+    <t>栈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/evaluate-reverse-polish-notation/solution/hou-zhui-biao-da-shi-de-ji-suan-by-yi-wen-statisti/</t>
+  </si>
+  <si>
+    <t>数组，动态规划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/maximum-product-subarray/solution/hua-jie-suan-fa-152-cheng-ji-zui-da-zi-xu-lie-by-g/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/min-stack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/min-stack/solution/zui-xiao-zhan-by-leetcode-solution/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/intersection-of-two-linked-lists</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/find-peak-element</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/majority-element</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>栈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/intersection-of-two-linked-lists/solution/intersection-of-two-linked-lists-shuang-zhi-zhen-l/</t>
+  </si>
+  <si>
+    <t>数组，二分查找</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/find-peak-element/solution/xun-zhao-feng-zhi-by-leetcode/</t>
+  </si>
+  <si>
+    <t>39</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/shu-zu-zhong-chu-xian-ci-shu-chao-guo-yi-ban-de-shu-zi-lcof/solution/mian-shi-ti-39-shu-zu-zhong-chu-xian-ci-shu-chao-3/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/excel-sheet-column-number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/factorial-trailing-zeroes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/largest-number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数组，摩尔投票法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串，数学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/excel-sheet-column-number/solution/hua-jie-suan-fa-171-excelbiao-lie-xu-hao-by-guanpe/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/factorial-trailing-zeroes/solution/xiang-xi-tong-su-de-si-lu-fen-xi-by-windliang-3/</t>
+  </si>
+  <si>
+    <t>字符串，排序，数学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/largest-number/solution/zui-da-shu-by-leetcode/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/largest-number/solution/zui-da-shu-bi-jiao-gui-ze-chuan-di-xing-yi-ji-suan/344160</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/repeated-dna-sequences</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/rotate-array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/house-robber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串，哈希表，位运算</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/repeated-dna-sequences/solution/liang-ge-ji-he-by-tuotuoli/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/rotate-array/solution/san-ci-fan-zhuan-fu-yi-xie-pythonicde-jie-fa-pytho/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/house-robber/solution/da-jia-jie-she-by-leetcode-solution/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/binary-tree-right-side-view</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/number-of-islands</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/happy-number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树，深搜，广搜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图，深搜，广搜，并查集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/binary-tree-right-side-view/solution/jian-dan-bfsdfs-bi-xu-miao-dong-by-sweetiee/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/happy-number/solution/kuai-le-shu-by-leetcode-solution/</t>
+  </si>
+  <si>
+    <t>数学，哈希表，双指针</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/remove-linked-list-elements</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/reverse-linked-list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/kth-largest-element-in-an-array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/remove-linked-list-elements/solution/yi-chu-lian-biao-yuan-su-by-leetcode/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/reverse-linked-list/solution/dong-hua-yan-shi-206-fan-zhuan-lian-biao-by-user74/</t>
+  </si>
+  <si>
+    <t>链表，双指针，递归</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/kth-largest-element-in-an-array/solution/partitionfen-er-zhi-zhi-you-xian-dui-lie-java-dai-/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/contains-duplicate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/maximal-square</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/implement-stack-using-queues</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/shu-zu-zhong-zhong-fu-de-shu-zi-lcof/solution/yuan-di-zhi-huan-shi-jian-kong-jian-100-by-derrick/</t>
+  </si>
+  <si>
+    <t>数组，哈希表，原地</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/contains-duplicate/solution/cun-zai-zhong-fu-yuan-su-by-leetcode/</t>
+  </si>
+  <si>
+    <t>数组，动态规划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数组，分治，快排</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/maximal-square/solution/zui-da-zheng-fang-xing-by-leetcode-solution/</t>
+  </si>
+  <si>
+    <t>栈，队列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/implement-stack-using-queues/solution/c-shi-yong-queueshi-xian-by-panini/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/invert-binary-tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/basic-calculator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/basic-calculator-ii</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/er-cha-sou-suo-shu-de-di-kda-jie-dian-lcof/solution/mian-shi-ti-54-er-cha-sou-suo-shu-de-di-k-da-jie-d/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/kth-smallest-element-in-a-bst</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/kth-smallest-element-in-a-bst/solution/er-cha-sou-suo-shu-zhong-di-kxiao-de-yuan-su-by-le/</t>
+  </si>
+  <si>
+    <t>树，中序遍历</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树，递归，广搜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/invert-binary-tree/solution/fan-zhuan-er-cha-shu-by-leetcode/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/er-cha-shu-de-jing-xiang-lcof</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/er-cha-shu-de-jing-xiang-lcof/solution/mian-shi-ti-27-er-cha-shu-de-jing-xiang-di-gui-fu-/</t>
+  </si>
+  <si>
+    <t>基本计算器II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基本计算器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/basic-calculator-ii/solution/chai-jie-fu-za-wen-ti-shi-xian-yi-ge-wan-zheng-ji-/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/implement-queue-using-stacks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/palindrome-linked-list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/lowest-common-ancestor-of-a-binary-search-tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/lowest-common-ancestor-of-a-binary-tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/implement-queue-using-stacks/solution/yong-zhan-shi-xian-dui-lie-by-leetcode/</t>
+  </si>
+  <si>
+    <t>栈，队列，设计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/yong-liang-ge-zhan-shi-xian-dui-lie-lcof/solution/mian-shi-ti-09-yong-liang-ge-zhan-shi-xian-dui-l-2/</t>
+  </si>
+  <si>
+    <t>栈，队列，设计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/palindrome-linked-list/solution/hui-wen-lian-biao-1zhan-2kuai-man-zhi-zhen-fan-zhu/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/valid-anagram</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>68-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>68-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/er-cha-sou-suo-shu-de-zui-jin-gong-gong-zu-xian-lcof/solution/mian-shi-ti-68-i-er-cha-sou-suo-shu-de-zui-jin-g-7/</t>
+  </si>
+  <si>
+    <t>树，递归，迭代</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树，递归，迭代</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/er-cha-shu-de-zui-jin-gong-gong-zu-xian-lcof/solution/mian-shi-ti-68-ii-er-cha-shu-de-zui-jin-gong-gon-7/</t>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/chou-shu-lcof</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数学，动态规划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/chou-shu-lcof/solution/mian-shi-ti-49-chou-shu-dong-tai-gui-hua-qing-xi-t/</t>
+  </si>
+  <si>
+    <t>栈，数学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>栈，数学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/delete-node-in-a-linked-list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>链表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/delete-node-in-a-linked-list/solution/shan-chu-lian-biao-zhong-de-jie-dian-by-leetcode/</t>
+  </si>
+  <si>
+    <t>岛屿数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/number-of-islands/solution/number-of-islands-shen-du-you-xian-bian-li-dfs-or-/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已刷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/longest-substring-without-repeating-characters/solution/hua-jie-suan-fa-3-wu-zhong-fu-zi-fu-de-zui-chang-z/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/container-with-most-water/solution/container-with-most-water-shuang-zhi-zhen-fa-yi-do/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/3sum/solution/3sumpai-xu-shuang-zhi-zhen-yi-dong-by-jyd/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>https://leetcode-cn.com/problems/path-sum/solution/lu-jing-zong-he-by-leetcode-solution/</t>
-  </si>
-  <si>
-    <t>树，递归，深搜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>树，递归，深搜</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>https://leetcode-cn.com/problems/path-sum-ii/solution/dfsfei-di-gui-python3-by-baiyizhe/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/flatten-binary-tree-to-linked-list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/pascals-triangle</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/pascals-triangle-ii</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>树，深搜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/flatten-binary-tree-to-linked-list/solution/er-cha-shu-zhan-kai-wei-lian-biao-by-leetcode-solu/</t>
-  </si>
-  <si>
-    <t>数组，动态规划</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/pascals-triangle/solution/yang-hui-san-jiao-by-leetcode/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/pascals-triangle-ii/solution/119yang-hui-san-jiao-ii-dong-tai-gui-hua-by-ceng-j/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/best-time-to-buy-and-sell-stock</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/best-time-to-buy-and-sell-stock-ii</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/valid-palindrome</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/best-time-to-buy-and-sell-stock/solution/121-mai-mai-gu-piao-de-zui-jia-shi-ji-by-leetcode-/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/best-time-to-buy-and-sell-stock-ii/solution/mai-mai-gu-piao-de-zui-jia-shi-ji-ii-by-leetcode/</t>
-  </si>
-  <si>
-    <t>数组，贪心，动态规划，单调栈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>字符串，双指针</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/valid-palindrome/solution/yan-zheng-hui-wen-chuan-by-leetcode-solution/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/single-number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/single-number-ii</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/word-break</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/single-number/solution/zhi-chu-xian-yi-ci-de-shu-zi-by-leetcode-solution/</t>
-  </si>
-  <si>
-    <t>数组，集合，哈希表，位运算</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/single-number-ii/solution/luo-ji-dian-lu-jiao-du-xiang-xi-fen-xi-gai-ti-si-l/</t>
-  </si>
-  <si>
-    <t>数组，位运算，数学</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数组，动态规划</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/word-break/solution/dong-tai-gui-hua-ji-yi-hua-hui-su-zhu-xing-jie-shi/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/linked-list-cycle</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/linked-list-cycle-ii</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/reorder-list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/linked-list-cycle/solution/huan-xing-lian-biao-by-leetcode/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/linked-list-cycle-ii/solution/linked-list-cycle-ii-kuai-man-zhi-zhen-shuang-zhi-/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/reorder-list/solution/3ge-bu-zou-jian-dan-yi-dong-by-wang_dong/</t>
-  </si>
-  <si>
-    <t>链表，双指针</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/binary-tree-preorder-traversal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/lru-cache</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/sort-list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>树，递归</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/binary-tree-preorder-traversal/solution/leetcodesuan-fa-xiu-lian-dong-hua-yan-shi-xbian-2/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/lru-cache/solution/lruhuan-cun-ji-zhi-by-leetcode-solution/</t>
-  </si>
-  <si>
-    <t>设计，哈希表，链表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/evaluate-reverse-polish-notation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/maximum-product-subarray</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>链表，排序，归并</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/sort-list/solution/148-pai-xu-lian-biao-bottom-to-up-o1-kong-jian-by-/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/sort-list/solution/lioney-cgui-bing-pai-xu-lian-biao-by-lioney/</t>
-  </si>
-  <si>
-    <t>栈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/evaluate-reverse-polish-notation/solution/hou-zhui-biao-da-shi-de-ji-suan-by-yi-wen-statisti/</t>
-  </si>
-  <si>
-    <t>数组，动态规划</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/maximum-product-subarray/solution/hua-jie-suan-fa-152-cheng-ji-zui-da-zi-xu-lie-by-g/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/min-stack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/min-stack/solution/zui-xiao-zhan-by-leetcode-solution/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/intersection-of-two-linked-lists</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/find-peak-element</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/majority-element</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>栈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/intersection-of-two-linked-lists/solution/intersection-of-two-linked-lists-shuang-zhi-zhen-l/</t>
-  </si>
-  <si>
-    <t>数组，二分查找</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/find-peak-element/solution/xun-zhao-feng-zhi-by-leetcode/</t>
-  </si>
-  <si>
-    <t>39</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/shu-zu-zhong-chu-xian-ci-shu-chao-guo-yi-ban-de-shu-zi-lcof/solution/mian-shi-ti-39-shu-zu-zhong-chu-xian-ci-shu-chao-3/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/excel-sheet-column-number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/factorial-trailing-zeroes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/largest-number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数组，摩尔投票法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>字符串，数学</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/excel-sheet-column-number/solution/hua-jie-suan-fa-171-excelbiao-lie-xu-hao-by-guanpe/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/factorial-trailing-zeroes/solution/xiang-xi-tong-su-de-si-lu-fen-xi-by-windliang-3/</t>
-  </si>
-  <si>
-    <t>字符串，排序，数学</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/largest-number/solution/zui-da-shu-by-leetcode/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/largest-number/solution/zui-da-shu-bi-jiao-gui-ze-chuan-di-xing-yi-ji-suan/344160</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/repeated-dna-sequences</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/rotate-array</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/house-robber</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>字符串，哈希表，位运算</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/repeated-dna-sequences/solution/liang-ge-ji-he-by-tuotuoli/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/rotate-array/solution/san-ci-fan-zhuan-fu-yi-xie-pythonicde-jie-fa-pytho/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/house-robber/solution/da-jia-jie-she-by-leetcode-solution/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/binary-tree-right-side-view</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/number-of-islands</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/happy-number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>树，深搜，广搜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>图，深搜，广搜，并查集</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/binary-tree-right-side-view/solution/jian-dan-bfsdfs-bi-xu-miao-dong-by-sweetiee/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/happy-number/solution/kuai-le-shu-by-leetcode-solution/</t>
-  </si>
-  <si>
-    <t>数学，哈希表，双指针</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/remove-linked-list-elements</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/reverse-linked-list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/kth-largest-element-in-an-array</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/remove-linked-list-elements/solution/yi-chu-lian-biao-yuan-su-by-leetcode/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/reverse-linked-list/solution/dong-hua-yan-shi-206-fan-zhuan-lian-biao-by-user74/</t>
-  </si>
-  <si>
-    <t>链表，双指针，递归</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/kth-largest-element-in-an-array/solution/partitionfen-er-zhi-zhi-you-xian-dui-lie-java-dai-/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/contains-duplicate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/maximal-square</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/implement-stack-using-queues</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/shu-zu-zhong-zhong-fu-de-shu-zi-lcof/solution/yuan-di-zhi-huan-shi-jian-kong-jian-100-by-derrick/</t>
-  </si>
-  <si>
-    <t>数组，哈希表，原地</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/contains-duplicate/solution/cun-zai-zhong-fu-yuan-su-by-leetcode/</t>
-  </si>
-  <si>
-    <t>数组，动态规划</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数组，分治，快排</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/maximal-square/solution/zui-da-zheng-fang-xing-by-leetcode-solution/</t>
-  </si>
-  <si>
-    <t>栈，队列</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/implement-stack-using-queues/solution/c-shi-yong-queueshi-xian-by-panini/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/invert-binary-tree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/basic-calculator</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/basic-calculator-ii</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/er-cha-sou-suo-shu-de-di-kda-jie-dian-lcof/solution/mian-shi-ti-54-er-cha-sou-suo-shu-de-di-k-da-jie-d/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/kth-smallest-element-in-a-bst</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/kth-smallest-element-in-a-bst/solution/er-cha-sou-suo-shu-zhong-di-kxiao-de-yuan-su-by-le/</t>
-  </si>
-  <si>
-    <t>树，中序遍历</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>树，递归，广搜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/invert-binary-tree/solution/fan-zhuan-er-cha-shu-by-leetcode/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/er-cha-shu-de-jing-xiang-lcof</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/er-cha-shu-de-jing-xiang-lcof/solution/mian-shi-ti-27-er-cha-shu-de-jing-xiang-di-gui-fu-/</t>
-  </si>
-  <si>
-    <t>基本计算器II</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>基本计算器</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/basic-calculator-ii/solution/chai-jie-fu-za-wen-ti-shi-xian-yi-ge-wan-zheng-ji-/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/implement-queue-using-stacks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/palindrome-linked-list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/lowest-common-ancestor-of-a-binary-search-tree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/lowest-common-ancestor-of-a-binary-tree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/implement-queue-using-stacks/solution/yong-zhan-shi-xian-dui-lie-by-leetcode/</t>
-  </si>
-  <si>
-    <t>栈，队列，设计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/yong-liang-ge-zhan-shi-xian-dui-lie-lcof/solution/mian-shi-ti-09-yong-liang-ge-zhan-shi-xian-dui-l-2/</t>
-  </si>
-  <si>
-    <t>栈，队列，设计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/palindrome-linked-list/solution/hui-wen-lian-biao-1zhan-2kuai-man-zhi-zhen-fan-zhu/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/valid-anagram</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>68-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>68-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/er-cha-sou-suo-shu-de-zui-jin-gong-gong-zu-xian-lcof/solution/mian-shi-ti-68-i-er-cha-sou-suo-shu-de-zui-jin-g-7/</t>
-  </si>
-  <si>
-    <t>树，递归，迭代</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>树，递归，迭代</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/er-cha-shu-de-zui-jin-gong-gong-zu-xian-lcof/solution/mian-shi-ti-68-ii-er-cha-shu-de-zui-jin-gong-gon-7/</t>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/chou-shu-lcof</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数学，动态规划</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/chou-shu-lcof/solution/mian-shi-ti-49-chou-shu-dong-tai-gui-hua-qing-xi-t/</t>
-  </si>
-  <si>
-    <t>栈，数学</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>栈，数学</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/delete-node-in-a-linked-list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>链表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/delete-node-in-a-linked-list/solution/shan-chu-lian-biao-zhong-de-jie-dian-by-leetcode/</t>
-  </si>
-  <si>
-    <t>岛屿数量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/number-of-islands/solution/number-of-islands-shen-du-you-xian-bian-li-dfs-or-/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>已刷</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/longest-substring-without-repeating-characters/solution/hua-jie-suan-fa-3-wu-zhong-fu-zi-fu-de-zui-chang-z/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/container-with-most-water/solution/container-with-most-water-shuang-zhi-zhen-fa-yi-do/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode-cn.com/problems/3sum/solution/3sumpai-xu-shuang-zhi-zhen-yi-dong-by-jyd/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2503,7 +2506,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2581,6 +2584,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2594,9 +2603,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2623,7 +2629,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2698,6 +2704,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2733,6 +2756,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2908,12 +2948,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I225"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2940,7 +2980,7 @@
         <v>556</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>312</v>
@@ -3005,7 +3045,7 @@
       <c r="B4" s="7">
         <v>3</v>
       </c>
-      <c r="D4" s="32"/>
+      <c r="D4" s="28"/>
       <c r="E4" s="4" t="s">
         <v>2</v>
       </c>
@@ -3016,7 +3056,7 @@
         <v>324</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
@@ -3106,7 +3146,7 @@
       <c r="B9" s="7">
         <v>11</v>
       </c>
-      <c r="D9" s="32"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="4" t="s">
         <v>8</v>
       </c>
@@ -3117,7 +3157,7 @@
         <v>338</v>
       </c>
       <c r="H9" s="26" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
@@ -3147,7 +3187,7 @@
       <c r="B11" s="7">
         <v>15</v>
       </c>
-      <c r="D11" s="32"/>
+      <c r="D11" s="28"/>
       <c r="E11" s="4" t="s">
         <v>10</v>
       </c>
@@ -3158,7 +3198,7 @@
         <v>344</v>
       </c>
       <c r="H11" s="26" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
@@ -3482,19 +3522,19 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A28" s="27">
+      <c r="A28" s="29">
         <v>26</v>
       </c>
-      <c r="B28" s="27">
+      <c r="B28" s="29">
         <v>46</v>
       </c>
-      <c r="E28" s="28" t="s">
+      <c r="E28" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="F28" s="29" t="s">
+      <c r="F28" s="31" t="s">
         <v>390</v>
       </c>
-      <c r="G28" s="30" t="s">
+      <c r="G28" s="32" t="s">
         <v>392</v>
       </c>
       <c r="H28" s="3" t="s">
@@ -3502,17 +3542,17 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A29" s="27"/>
-      <c r="B29" s="27"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="30"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="29"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="32"/>
       <c r="H29" s="3" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A30" s="27"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="7">
         <v>47</v>
       </c>
@@ -3686,7 +3726,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A39" s="27">
+      <c r="A39" s="29">
         <v>35</v>
       </c>
       <c r="B39" s="7">
@@ -3706,7 +3746,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A40" s="27"/>
+      <c r="A40" s="29"/>
       <c r="B40" s="7">
         <v>63</v>
       </c>
@@ -3860,7 +3900,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A48" s="27">
+      <c r="A48" s="29">
         <v>43</v>
       </c>
       <c r="B48" s="7">
@@ -3876,7 +3916,7 @@
       <c r="H48" s="10"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A49" s="27"/>
+      <c r="A49" s="29"/>
       <c r="B49" s="7">
         <v>83</v>
       </c>
@@ -3894,7 +3934,7 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A50" s="27">
+      <c r="A50" s="29">
         <v>44</v>
       </c>
       <c r="B50" s="7">
@@ -3914,7 +3954,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A51" s="27"/>
+      <c r="A51" s="29"/>
       <c r="B51" s="7">
         <v>725</v>
       </c>
@@ -3952,19 +3992,19 @@
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A53" s="27">
+      <c r="A53" s="29">
         <v>46</v>
       </c>
-      <c r="B53" s="27">
+      <c r="B53" s="29">
         <v>90</v>
       </c>
-      <c r="E53" s="28" t="s">
+      <c r="E53" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="F53" s="29" t="s">
+      <c r="F53" s="31" t="s">
         <v>450</v>
       </c>
-      <c r="G53" s="30" t="s">
+      <c r="G53" s="32" t="s">
         <v>453</v>
       </c>
       <c r="H53" s="10" t="s">
@@ -3972,11 +4012,11 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A54" s="27"/>
-      <c r="B54" s="27"/>
-      <c r="E54" s="28"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="30"/>
+      <c r="A54" s="29"/>
+      <c r="B54" s="29"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="32"/>
       <c r="H54" s="10" t="s">
         <v>454</v>
       </c>
@@ -4003,16 +4043,16 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A56" s="7"/>
-      <c r="B56" s="27">
+      <c r="B56" s="29">
         <v>92</v>
       </c>
-      <c r="E56" s="28" t="s">
+      <c r="E56" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="F56" s="29" t="s">
+      <c r="F56" s="31" t="s">
         <v>452</v>
       </c>
-      <c r="G56" s="30" t="s">
+      <c r="G56" s="32" t="s">
         <v>458</v>
       </c>
       <c r="H56" s="10" t="s">
@@ -4023,10 +4063,10 @@
       <c r="A57" s="2">
         <v>48</v>
       </c>
-      <c r="B57" s="27"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="29"/>
-      <c r="G57" s="30"/>
+      <c r="B57" s="29"/>
+      <c r="E57" s="30"/>
+      <c r="F57" s="31"/>
+      <c r="G57" s="32"/>
       <c r="H57" s="10" t="s">
         <v>459</v>
       </c>
@@ -4134,19 +4174,19 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A63" s="27">
+      <c r="A63" s="29">
         <v>54</v>
       </c>
-      <c r="B63" s="27">
+      <c r="B63" s="29">
         <v>102</v>
       </c>
-      <c r="E63" s="28" t="s">
+      <c r="E63" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="F63" s="29" t="s">
+      <c r="F63" s="31" t="s">
         <v>472</v>
       </c>
-      <c r="G63" s="30" t="s">
+      <c r="G63" s="32" t="s">
         <v>478</v>
       </c>
       <c r="H63" s="9" t="s">
@@ -4154,11 +4194,11 @@
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A64" s="27"/>
-      <c r="B64" s="27"/>
-      <c r="E64" s="28"/>
-      <c r="F64" s="29"/>
-      <c r="G64" s="30"/>
+      <c r="A64" s="29"/>
+      <c r="B64" s="29"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="31"/>
+      <c r="G64" s="32"/>
       <c r="H64" s="10" t="s">
         <v>477</v>
       </c>
@@ -4277,10 +4317,10 @@
         <v>491</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>562</v>
-      </c>
-      <c r="H70" s="12" t="s">
         <v>561</v>
+      </c>
+      <c r="H70" s="27" t="s">
+        <v>710</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.15">
@@ -4297,10 +4337,10 @@
         <v>492</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>563</v>
-      </c>
-      <c r="H71" s="12" t="s">
-        <v>564</v>
+        <v>562</v>
+      </c>
+      <c r="H71" s="27" t="s">
+        <v>711</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.15">
@@ -4314,17 +4354,17 @@
         <v>63</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="H72" s="12" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A73" s="27">
+      <c r="A73" s="29">
         <v>62</v>
       </c>
       <c r="B73" s="7">
@@ -4334,17 +4374,17 @@
         <v>64</v>
       </c>
       <c r="F73" s="11" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="H73" s="12" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A74" s="27"/>
+      <c r="A74" s="29"/>
       <c r="B74" s="7">
         <v>119</v>
       </c>
@@ -4352,13 +4392,13 @@
         <v>499</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="G74" s="10" t="s">
         <v>405</v>
       </c>
       <c r="H74" s="12" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.15">
@@ -4372,13 +4412,13 @@
         <v>65</v>
       </c>
       <c r="F75" s="11" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="H75" s="12" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.15">
@@ -4392,13 +4432,13 @@
         <v>66</v>
       </c>
       <c r="F76" s="11" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="G76" s="3" t="s">
         <v>410</v>
       </c>
       <c r="H76" s="12" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.15">
@@ -4412,13 +4452,13 @@
         <v>67</v>
       </c>
       <c r="F77" s="11" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="H77" s="12" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.15">
@@ -4432,13 +4472,13 @@
         <v>68</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="H78" s="12" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.15">
@@ -4452,13 +4492,13 @@
         <v>69</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="H79" s="16" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.15">
@@ -4472,13 +4512,13 @@
         <v>70</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="H80" s="16" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.15">
@@ -4492,13 +4532,13 @@
         <v>71</v>
       </c>
       <c r="F81" s="17" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="G81" s="3" t="s">
         <v>354</v>
       </c>
       <c r="H81" s="16" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.15">
@@ -4512,13 +4552,13 @@
         <v>72</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="G82" s="3" t="s">
         <v>354</v>
       </c>
       <c r="H82" s="16" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.15">
@@ -4532,13 +4572,13 @@
         <v>73</v>
       </c>
       <c r="F83" s="17" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="H83" s="16" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.15">
@@ -4552,13 +4592,13 @@
         <v>74</v>
       </c>
       <c r="F84" s="17" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="H84" s="16" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.15">
@@ -4572,43 +4612,43 @@
         <v>75</v>
       </c>
       <c r="F85" s="17" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="H85" s="16" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A86" s="27">
+      <c r="A86" s="29">
         <v>74</v>
       </c>
-      <c r="B86" s="27">
+      <c r="B86" s="29">
         <v>148</v>
       </c>
-      <c r="E86" s="28" t="s">
+      <c r="E86" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="F86" s="29" t="s">
-        <v>599</v>
-      </c>
-      <c r="G86" s="30" t="s">
+      <c r="F86" s="31" t="s">
+        <v>597</v>
+      </c>
+      <c r="G86" s="32" t="s">
+        <v>604</v>
+      </c>
+      <c r="H86" s="18" t="s">
         <v>606</v>
       </c>
-      <c r="H86" s="18" t="s">
-        <v>608</v>
-      </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A87" s="27"/>
-      <c r="B87" s="27"/>
-      <c r="E87" s="28"/>
-      <c r="F87" s="29"/>
-      <c r="G87" s="30"/>
+      <c r="A87" s="29"/>
+      <c r="B87" s="29"/>
+      <c r="E87" s="30"/>
+      <c r="F87" s="31"/>
+      <c r="G87" s="32"/>
       <c r="H87" s="18" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.15">
@@ -4622,13 +4662,13 @@
         <v>77</v>
       </c>
       <c r="F88" s="19" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="H88" s="18" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.15">
@@ -4642,13 +4682,13 @@
         <v>78</v>
       </c>
       <c r="F89" s="19" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="H89" s="18" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.15">
@@ -4665,13 +4705,13 @@
         <v>79</v>
       </c>
       <c r="F90" s="19" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="H90" s="18" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.15">
@@ -4685,13 +4725,13 @@
         <v>80</v>
       </c>
       <c r="F91" s="19" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="G91" s="3" t="s">
         <v>354</v>
       </c>
       <c r="H91" s="18" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.15">
@@ -4705,13 +4745,13 @@
         <v>81</v>
       </c>
       <c r="F92" s="19" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="H92" s="18" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.15">
@@ -4722,19 +4762,19 @@
         <v>169</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E93" s="4" t="s">
         <v>82</v>
       </c>
       <c r="F93" s="19" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="H93" s="18" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.15">
@@ -4748,13 +4788,13 @@
         <v>83</v>
       </c>
       <c r="F94" s="19" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="H94" s="18" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.15">
@@ -4768,45 +4808,45 @@
         <v>84</v>
       </c>
       <c r="F95" s="19" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="G95" s="3" t="s">
         <v>332</v>
       </c>
       <c r="H95" s="18" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A96" s="29">
+        <v>83</v>
+      </c>
+      <c r="B96" s="29">
+        <v>179</v>
+      </c>
+      <c r="C96" s="33"/>
+      <c r="E96" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="F96" s="31" t="s">
+        <v>624</v>
+      </c>
+      <c r="G96" s="32" t="s">
+        <v>629</v>
+      </c>
+      <c r="H96" s="18" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A97" s="29"/>
+      <c r="B97" s="29"/>
+      <c r="C97" s="33"/>
+      <c r="E97" s="30"/>
+      <c r="F97" s="31"/>
+      <c r="G97" s="32"/>
+      <c r="H97" s="18" t="s">
         <v>630</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A96" s="27">
-        <v>83</v>
-      </c>
-      <c r="B96" s="27">
-        <v>179</v>
-      </c>
-      <c r="C96" s="31"/>
-      <c r="E96" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="F96" s="29" t="s">
-        <v>626</v>
-      </c>
-      <c r="G96" s="30" t="s">
-        <v>631</v>
-      </c>
-      <c r="H96" s="18" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A97" s="27"/>
-      <c r="B97" s="27"/>
-      <c r="C97" s="31"/>
-      <c r="E97" s="28"/>
-      <c r="F97" s="29"/>
-      <c r="G97" s="30"/>
-      <c r="H97" s="18" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.15">
@@ -4820,13 +4860,13 @@
         <v>86</v>
       </c>
       <c r="F98" s="19" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="H98" s="18" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.15">
@@ -4840,13 +4880,13 @@
         <v>87</v>
       </c>
       <c r="F99" s="19" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="G99" s="3" t="s">
         <v>408</v>
       </c>
       <c r="H99" s="18" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.15">
@@ -4860,13 +4900,13 @@
         <v>88</v>
       </c>
       <c r="F100" s="19" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="H100" s="18" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.15">
@@ -4880,13 +4920,13 @@
         <v>89</v>
       </c>
       <c r="F101" s="19" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="G101" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="H101" s="18" t="s">
         <v>644</v>
-      </c>
-      <c r="H101" s="18" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.15">
@@ -4897,16 +4937,16 @@
         <v>200</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="F102" s="19" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="H102" s="22" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.15">
@@ -4920,13 +4960,13 @@
         <v>90</v>
       </c>
       <c r="F103" s="19" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="H103" s="18" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.15">
@@ -4940,13 +4980,13 @@
         <v>91</v>
       </c>
       <c r="F104" s="19" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="G104" s="3" t="s">
         <v>360</v>
       </c>
       <c r="H104" s="18" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.15">
@@ -4960,13 +5000,13 @@
         <v>92</v>
       </c>
       <c r="F105" s="19" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="H105" s="18" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.15">
@@ -4980,13 +5020,13 @@
         <v>93</v>
       </c>
       <c r="F106" s="19" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="H106" s="18" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.15">
@@ -5000,13 +5040,13 @@
         <v>94</v>
       </c>
       <c r="F107" s="19" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="G107" s="3" t="s">
         <v>318</v>
       </c>
       <c r="H107" s="18" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.15">
@@ -5020,13 +5060,13 @@
         <v>95</v>
       </c>
       <c r="F108" s="19" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="G108" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="H108" s="18" t="s">
         <v>662</v>
-      </c>
-      <c r="H108" s="18" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.15">
@@ -5040,13 +5080,13 @@
         <v>96</v>
       </c>
       <c r="F109" s="19" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="H109" s="18" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.15">
@@ -5063,51 +5103,51 @@
         <v>97</v>
       </c>
       <c r="F110" s="19" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="H110" s="18" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A111" s="27">
+      <c r="A111" s="29">
         <v>97</v>
       </c>
       <c r="B111" s="7">
         <v>224</v>
       </c>
       <c r="E111" s="4" t="s">
+        <v>676</v>
+      </c>
+      <c r="F111" s="19" t="s">
+        <v>667</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="H111" s="21" t="s">
         <v>678</v>
       </c>
-      <c r="F111" s="19" t="s">
-        <v>669</v>
-      </c>
-      <c r="G111" s="3" t="s">
-        <v>702</v>
-      </c>
-      <c r="H111" s="21" t="s">
-        <v>680</v>
-      </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A112" s="27"/>
+      <c r="A112" s="29"/>
       <c r="B112" s="7">
         <v>227</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="F112" s="19" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="H112" s="21" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.15">
@@ -5124,13 +5164,13 @@
         <v>98</v>
       </c>
       <c r="F113" s="19" t="s">
+        <v>669</v>
+      </c>
+      <c r="G113" s="3" t="s">
         <v>671</v>
       </c>
-      <c r="G113" s="3" t="s">
-        <v>673</v>
-      </c>
       <c r="H113" s="18" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.15">
@@ -5141,19 +5181,19 @@
         <v>232</v>
       </c>
       <c r="C114" s="13" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E114" s="4" t="s">
         <v>99</v>
       </c>
       <c r="F114" s="20" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="H114" s="21" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.15">
@@ -5167,13 +5207,13 @@
         <v>100</v>
       </c>
       <c r="F115" s="6" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="G115" s="3" t="s">
         <v>354</v>
       </c>
       <c r="H115" s="21" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.15">
@@ -5184,19 +5224,19 @@
         <v>235</v>
       </c>
       <c r="C116" s="13" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="E116" s="5" t="s">
         <v>101</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="H116" s="21" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.15">
@@ -5207,19 +5247,19 @@
         <v>236</v>
       </c>
       <c r="C117" s="13" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="E117" s="5" t="s">
         <v>102</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="H117" s="21" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.15">
@@ -5233,13 +5273,13 @@
         <v>103</v>
       </c>
       <c r="F118" s="6" t="s">
+        <v>701</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="H118" s="23" t="s">
         <v>703</v>
-      </c>
-      <c r="G118" s="3" t="s">
-        <v>704</v>
-      </c>
-      <c r="H118" s="23" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.15">
@@ -5257,7 +5297,7 @@
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A120" s="27">
+      <c r="A120" s="29">
         <v>105</v>
       </c>
       <c r="B120" s="7">
@@ -5271,7 +5311,7 @@
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A121" s="27"/>
+      <c r="A121" s="29"/>
       <c r="B121" s="7">
         <v>240</v>
       </c>
@@ -5293,7 +5333,7 @@
         <v>110</v>
       </c>
       <c r="F122" s="6" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.15">
@@ -5465,7 +5505,7 @@
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A135" s="27">
+      <c r="A135" s="29">
         <v>119</v>
       </c>
       <c r="B135" s="7">
@@ -5479,7 +5519,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A136" s="27"/>
+      <c r="A136" s="29"/>
       <c r="B136" s="7">
         <v>337</v>
       </c>
@@ -5966,10 +6006,10 @@
         <v>203</v>
       </c>
       <c r="G170" s="3" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="H170" s="24" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.15">
@@ -6000,10 +6040,10 @@
         <v>207</v>
       </c>
       <c r="G172" s="3" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="H172" s="18" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.15">
@@ -6143,13 +6183,13 @@
         <v>226</v>
       </c>
       <c r="F182" s="6" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="G182" s="3" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="H182" s="18" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.15">
@@ -6642,10 +6682,10 @@
         <v>295</v>
       </c>
       <c r="G217" s="3" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="H217" s="18" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.15">
@@ -6659,13 +6699,13 @@
         <v>296</v>
       </c>
       <c r="F218" s="6" t="s">
+        <v>696</v>
+      </c>
+      <c r="G218" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="H218" s="23" t="s">
         <v>698</v>
-      </c>
-      <c r="G218" s="3" t="s">
-        <v>699</v>
-      </c>
-      <c r="H218" s="23" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.15">
@@ -6767,19 +6807,25 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1"/>
+  <autoFilter ref="A1:I225" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="37">
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="G86:G87"/>
+    <mergeCell ref="G96:G97"/>
+    <mergeCell ref="F96:F97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A96:A97"/>
     <mergeCell ref="B56:B57"/>
     <mergeCell ref="G63:G64"/>
     <mergeCell ref="F63:F64"/>
@@ -6789,146 +6835,142 @@
     <mergeCell ref="E56:E57"/>
     <mergeCell ref="F56:F57"/>
     <mergeCell ref="G56:G57"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="E86:E87"/>
-    <mergeCell ref="F86:F87"/>
-    <mergeCell ref="G86:G87"/>
-    <mergeCell ref="G96:G97"/>
-    <mergeCell ref="F96:F97"/>
-    <mergeCell ref="E96:E97"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B53:B54"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
-    <hyperlink ref="F6" r:id="rId5"/>
-    <hyperlink ref="F7" r:id="rId6"/>
-    <hyperlink ref="F8" r:id="rId7"/>
-    <hyperlink ref="F9" r:id="rId8"/>
-    <hyperlink ref="F10" r:id="rId9"/>
-    <hyperlink ref="F11" r:id="rId10"/>
-    <hyperlink ref="F12" r:id="rId11"/>
-    <hyperlink ref="F13" r:id="rId12"/>
-    <hyperlink ref="F14" r:id="rId13"/>
-    <hyperlink ref="F15" r:id="rId14"/>
-    <hyperlink ref="F16" r:id="rId15"/>
-    <hyperlink ref="F17" r:id="rId16"/>
-    <hyperlink ref="F18" r:id="rId17"/>
-    <hyperlink ref="F19" r:id="rId18"/>
-    <hyperlink ref="F20" r:id="rId19"/>
-    <hyperlink ref="F21" r:id="rId20"/>
-    <hyperlink ref="F22" r:id="rId21"/>
-    <hyperlink ref="F23" r:id="rId22"/>
-    <hyperlink ref="F24" r:id="rId23"/>
-    <hyperlink ref="F25" r:id="rId24"/>
-    <hyperlink ref="F26" r:id="rId25"/>
-    <hyperlink ref="F27" r:id="rId26"/>
-    <hyperlink ref="F28" r:id="rId27"/>
-    <hyperlink ref="F31" r:id="rId28"/>
-    <hyperlink ref="F32" r:id="rId29"/>
-    <hyperlink ref="F33" r:id="rId30"/>
-    <hyperlink ref="F34" r:id="rId31"/>
-    <hyperlink ref="F35" r:id="rId32"/>
-    <hyperlink ref="F36" r:id="rId33"/>
-    <hyperlink ref="F37" r:id="rId34"/>
-    <hyperlink ref="F38" r:id="rId35"/>
-    <hyperlink ref="F39" r:id="rId36"/>
-    <hyperlink ref="F41" r:id="rId37"/>
-    <hyperlink ref="F42" r:id="rId38"/>
-    <hyperlink ref="F43" r:id="rId39"/>
-    <hyperlink ref="F44" r:id="rId40"/>
-    <hyperlink ref="F45" r:id="rId41"/>
-    <hyperlink ref="F46" r:id="rId42"/>
-    <hyperlink ref="F47" r:id="rId43"/>
-    <hyperlink ref="F49" r:id="rId44"/>
-    <hyperlink ref="F51" r:id="rId45"/>
-    <hyperlink ref="F50" r:id="rId46"/>
-    <hyperlink ref="F52" r:id="rId47"/>
-    <hyperlink ref="F132" r:id="rId48"/>
-    <hyperlink ref="F53" r:id="rId49"/>
-    <hyperlink ref="F55" r:id="rId50"/>
-    <hyperlink ref="F56" r:id="rId51"/>
-    <hyperlink ref="F58" r:id="rId52"/>
-    <hyperlink ref="F60" r:id="rId53"/>
-    <hyperlink ref="F59" r:id="rId54"/>
-    <hyperlink ref="F61" r:id="rId55"/>
-    <hyperlink ref="F62" r:id="rId56"/>
-    <hyperlink ref="F63" r:id="rId57"/>
-    <hyperlink ref="H62" r:id="rId58"/>
-    <hyperlink ref="F65" r:id="rId59"/>
-    <hyperlink ref="F66" r:id="rId60"/>
-    <hyperlink ref="F67" r:id="rId61"/>
-    <hyperlink ref="F68" r:id="rId62"/>
-    <hyperlink ref="F69" r:id="rId63"/>
-    <hyperlink ref="F70" r:id="rId64"/>
-    <hyperlink ref="F71" r:id="rId65"/>
-    <hyperlink ref="F72" r:id="rId66"/>
-    <hyperlink ref="F73" r:id="rId67"/>
-    <hyperlink ref="F74" r:id="rId68"/>
-    <hyperlink ref="F75" r:id="rId69"/>
-    <hyperlink ref="F76" r:id="rId70"/>
-    <hyperlink ref="F77" r:id="rId71"/>
-    <hyperlink ref="F78" r:id="rId72"/>
-    <hyperlink ref="F79" r:id="rId73"/>
-    <hyperlink ref="F80" r:id="rId74"/>
-    <hyperlink ref="F81" r:id="rId75"/>
-    <hyperlink ref="F82" r:id="rId76"/>
-    <hyperlink ref="F83" r:id="rId77"/>
-    <hyperlink ref="F84" r:id="rId78"/>
-    <hyperlink ref="F85" r:id="rId79"/>
-    <hyperlink ref="F86" r:id="rId80"/>
-    <hyperlink ref="F88" r:id="rId81"/>
-    <hyperlink ref="F89" r:id="rId82"/>
-    <hyperlink ref="F90" r:id="rId83"/>
-    <hyperlink ref="F91" r:id="rId84"/>
-    <hyperlink ref="F92" r:id="rId85"/>
-    <hyperlink ref="F93" r:id="rId86"/>
-    <hyperlink ref="F94" r:id="rId87"/>
-    <hyperlink ref="F95" r:id="rId88"/>
-    <hyperlink ref="F96" r:id="rId89"/>
-    <hyperlink ref="F98" r:id="rId90"/>
-    <hyperlink ref="F99" r:id="rId91"/>
-    <hyperlink ref="F100" r:id="rId92"/>
-    <hyperlink ref="F101" r:id="rId93"/>
-    <hyperlink ref="F102" r:id="rId94"/>
-    <hyperlink ref="F103" r:id="rId95"/>
-    <hyperlink ref="F104" r:id="rId96"/>
-    <hyperlink ref="F105" r:id="rId97"/>
-    <hyperlink ref="F106" r:id="rId98"/>
-    <hyperlink ref="F107" r:id="rId99"/>
-    <hyperlink ref="F108" r:id="rId100"/>
-    <hyperlink ref="F109" r:id="rId101"/>
-    <hyperlink ref="F110" r:id="rId102"/>
-    <hyperlink ref="F111" r:id="rId103"/>
-    <hyperlink ref="F112" r:id="rId104"/>
-    <hyperlink ref="F113" r:id="rId105"/>
-    <hyperlink ref="F182" r:id="rId106"/>
-    <hyperlink ref="F114" r:id="rId107"/>
-    <hyperlink ref="F115" r:id="rId108"/>
-    <hyperlink ref="F116" r:id="rId109"/>
-    <hyperlink ref="F117" r:id="rId110"/>
-    <hyperlink ref="H170" r:id="rId111"/>
-    <hyperlink ref="F122" r:id="rId112"/>
-    <hyperlink ref="F218" r:id="rId113"/>
-    <hyperlink ref="F118" r:id="rId114"/>
-    <hyperlink ref="H102" r:id="rId115"/>
-    <hyperlink ref="H4" r:id="rId116"/>
-    <hyperlink ref="H9" r:id="rId117"/>
-    <hyperlink ref="H11" r:id="rId118"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="F21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="F22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="F23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="F24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="F25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="F26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="F27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="F28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="F31" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="F32" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="F33" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="F34" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="F35" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="F36" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="F37" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="F38" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="F39" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="F41" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="F42" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="F43" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="F44" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="F45" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="F46" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="F47" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="F49" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="F51" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="F50" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="F52" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="F132" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="F53" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="F55" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="F56" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="F58" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="F60" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="F59" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="F61" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="F62" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="F63" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="H62" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="F65" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="F66" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="F67" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="F68" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="F69" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="F70" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="F71" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="F72" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="F73" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="F74" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="F75" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="F76" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="F77" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="F78" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="F79" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="F80" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="F81" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="F82" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="F83" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="F84" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="F85" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="F86" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="F88" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="F89" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="F90" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="F91" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="F92" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="F93" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="F94" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="F95" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="F96" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="F98" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="F99" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="F100" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="F101" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="F102" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="F103" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="F104" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="F105" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="F106" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="F107" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="F108" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="F109" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="F110" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="F111" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="F112" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="F113" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="F182" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="F114" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="F115" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="F116" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="F117" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="H170" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="F122" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="F218" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="F118" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="H102" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="H4" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="H9" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="H11" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="H70" r:id="rId119" xr:uid="{55759A4B-1148-4482-AF42-940857893685}"/>
+    <hyperlink ref="H71" r:id="rId120" xr:uid="{598AB80F-E8DD-4B20-A237-CB2351614891}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId119"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId121"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
+ Add fluent python ipynb
</commit_message>
<xml_diff>
--- a/面试高频题.xlsx
+++ b/面试高频题.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F9909A-B4DD-4B8A-8C44-9E5B393B629D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10028127-0926-4449-95B1-7E8FC182F24F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2952,8 +2952,8 @@
   <dimension ref="A1:I225"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
+ Add interview questions
</commit_message>
<xml_diff>
--- a/面试高频题.xlsx
+++ b/面试高频题.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10028127-0926-4449-95B1-7E8FC182F24F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAFE6B5-636E-40FB-BD45-8DAB5C16F0F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6015" yWindow="4065" windowWidth="19545" windowHeight="10500" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2952,8 +2952,8 @@
   <dimension ref="A1:I225"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E130" sqref="E130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2963,7 +2963,7 @@
     <col min="3" max="3" width="7.25" style="13" customWidth="1"/>
     <col min="4" max="4" width="7.625" style="25" customWidth="1"/>
     <col min="5" max="5" width="28.75" style="5" customWidth="1"/>
-    <col min="6" max="6" width="26.875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="34" style="10" customWidth="1"/>
     <col min="7" max="7" width="31.875" style="3" customWidth="1"/>
     <col min="8" max="8" width="21.875" style="3" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
@@ -6809,6 +6809,34 @@
   </sheetData>
   <autoFilter ref="A1:I225" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="37">
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="G56:G57"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A96:A97"/>
     <mergeCell ref="B86:B87"/>
     <mergeCell ref="E86:E87"/>
     <mergeCell ref="F86:F87"/>
@@ -6818,34 +6846,6 @@
     <mergeCell ref="E96:E97"/>
     <mergeCell ref="C96:C97"/>
     <mergeCell ref="B96:B97"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="G56:G57"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B53:B54"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
+ Add 0078, 0090
</commit_message>
<xml_diff>
--- a/面试高频题.xlsx
+++ b/面试高频题.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9127FF1E-D364-448E-A108-0A6FC3D2397D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C2D7FF-41AB-4AB9-B0E5-A53218CBD49F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2606,23 +2606,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2970,25 +2970,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E151" sqref="E151"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="7.25" style="13" customWidth="1"/>
-    <col min="4" max="4" width="7.625" style="25" customWidth="1"/>
-    <col min="5" max="5" width="37.375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="6.36328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.08984375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="7.26953125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="7.6328125" style="25" customWidth="1"/>
+    <col min="5" max="5" width="37.36328125" style="5" customWidth="1"/>
     <col min="6" max="6" width="34" style="10" customWidth="1"/>
-    <col min="7" max="7" width="31.875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="21.875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="31.90625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="21.90625" style="3" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>311</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3078,7 +3078,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -3199,7 +3199,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -3360,7 +3360,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -3540,45 +3540,46 @@
         <v>389</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A28" s="33">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="32">
         <v>26</v>
       </c>
-      <c r="B28" s="33">
+      <c r="B28" s="32">
         <v>46</v>
       </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="31"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="36"/>
       <c r="E28" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="F28" s="35" t="s">
+      <c r="F28" s="31" t="s">
         <v>390</v>
       </c>
-      <c r="G28" s="36" t="s">
+      <c r="G28" s="33" t="s">
         <v>391</v>
       </c>
       <c r="H28" s="29" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A29" s="33"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="31"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="36"/>
       <c r="E29" s="34"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="36"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="33"/>
       <c r="H29" s="29" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A30" s="33"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="32"/>
       <c r="B30" s="7">
         <v>47</v>
       </c>
+      <c r="D30" s="28"/>
       <c r="E30" s="8" t="s">
         <v>491</v>
       </c>
@@ -3588,7 +3589,7 @@
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>27</v>
       </c>
@@ -3608,7 +3609,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>28</v>
       </c>
@@ -3628,7 +3629,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>29</v>
       </c>
@@ -3648,7 +3649,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>30</v>
       </c>
@@ -3668,7 +3669,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>31</v>
       </c>
@@ -3688,7 +3689,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>32</v>
       </c>
@@ -3708,7 +3709,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>33</v>
       </c>
@@ -3728,7 +3729,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>34</v>
       </c>
@@ -3748,8 +3749,8 @@
         <v>415</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A39" s="33">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="32">
         <v>35</v>
       </c>
       <c r="B39" s="7">
@@ -3768,8 +3769,8 @@
         <v>417</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A40" s="33"/>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="32"/>
       <c r="B40" s="7">
         <v>63</v>
       </c>
@@ -3782,7 +3783,7 @@
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>36</v>
       </c>
@@ -3802,7 +3803,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>37</v>
       </c>
@@ -3822,7 +3823,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>38</v>
       </c>
@@ -3842,7 +3843,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>39</v>
       </c>
@@ -3862,7 +3863,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>40</v>
       </c>
@@ -3882,7 +3883,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>41</v>
       </c>
@@ -3902,7 +3903,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>42</v>
       </c>
@@ -3922,8 +3923,8 @@
         <v>440</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A48" s="33">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="32">
         <v>43</v>
       </c>
       <c r="B48" s="7">
@@ -3938,8 +3939,8 @@
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A49" s="33"/>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="32"/>
       <c r="B49" s="7">
         <v>83</v>
       </c>
@@ -3956,8 +3957,8 @@
         <v>442</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A50" s="33">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="32">
         <v>44</v>
       </c>
       <c r="B50" s="7">
@@ -3976,8 +3977,8 @@
         <v>444</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A51" s="33"/>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="32"/>
       <c r="B51" s="7">
         <v>725</v>
       </c>
@@ -3994,7 +3995,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>45</v>
       </c>
@@ -4014,37 +4015,37 @@
         <v>447</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A53" s="33">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="32">
         <v>46</v>
       </c>
-      <c r="B53" s="33">
+      <c r="B53" s="32">
         <v>90</v>
       </c>
       <c r="E53" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="F53" s="35" t="s">
+      <c r="F53" s="31" t="s">
         <v>448</v>
       </c>
-      <c r="G53" s="36" t="s">
+      <c r="G53" s="33" t="s">
         <v>451</v>
       </c>
       <c r="H53" s="10" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A54" s="33"/>
-      <c r="B54" s="33"/>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="32"/>
+      <c r="B54" s="32"/>
       <c r="E54" s="34"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="36"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="33"/>
       <c r="H54" s="10" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>47</v>
       </c>
@@ -4064,37 +4065,37 @@
         <v>455</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
-      <c r="B56" s="33">
+      <c r="B56" s="32">
         <v>92</v>
       </c>
       <c r="E56" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="F56" s="35" t="s">
+      <c r="F56" s="31" t="s">
         <v>450</v>
       </c>
-      <c r="G56" s="36" t="s">
+      <c r="G56" s="33" t="s">
         <v>456</v>
       </c>
       <c r="H56" s="10" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>48</v>
       </c>
-      <c r="B57" s="33"/>
+      <c r="B57" s="32"/>
       <c r="E57" s="34"/>
-      <c r="F57" s="35"/>
-      <c r="G57" s="36"/>
+      <c r="F57" s="31"/>
+      <c r="G57" s="33"/>
       <c r="H57" s="10" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>49</v>
       </c>
@@ -4114,7 +4115,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>50</v>
       </c>
@@ -4136,7 +4137,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>51</v>
       </c>
@@ -4156,7 +4157,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>52</v>
       </c>
@@ -4176,7 +4177,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>53</v>
       </c>
@@ -4196,37 +4197,37 @@
         <v>473</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A63" s="33">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="32">
         <v>54</v>
       </c>
-      <c r="B63" s="33">
+      <c r="B63" s="32">
         <v>102</v>
       </c>
       <c r="E63" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="F63" s="35" t="s">
+      <c r="F63" s="31" t="s">
         <v>470</v>
       </c>
-      <c r="G63" s="36" t="s">
+      <c r="G63" s="33" t="s">
         <v>476</v>
       </c>
       <c r="H63" s="9" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A64" s="33"/>
-      <c r="B64" s="33"/>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="32"/>
+      <c r="B64" s="32"/>
       <c r="E64" s="34"/>
-      <c r="F64" s="35"/>
-      <c r="G64" s="36"/>
+      <c r="F64" s="31"/>
+      <c r="G64" s="33"/>
       <c r="H64" s="10" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>55</v>
       </c>
@@ -4246,7 +4247,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>56</v>
       </c>
@@ -4266,7 +4267,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>57</v>
       </c>
@@ -4286,7 +4287,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>58</v>
       </c>
@@ -4306,7 +4307,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>59</v>
       </c>
@@ -4326,7 +4327,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>60</v>
       </c>
@@ -4346,7 +4347,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>60</v>
       </c>
@@ -4366,7 +4367,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>61</v>
       </c>
@@ -4386,8 +4387,8 @@
         <v>564</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A73" s="33">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="32">
         <v>62</v>
       </c>
       <c r="B73" s="7">
@@ -4406,8 +4407,8 @@
         <v>566</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A74" s="33"/>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="32"/>
       <c r="B74" s="7">
         <v>119</v>
       </c>
@@ -4424,7 +4425,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>63</v>
       </c>
@@ -4444,7 +4445,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>64</v>
       </c>
@@ -4464,7 +4465,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>65</v>
       </c>
@@ -4484,7 +4485,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>66</v>
       </c>
@@ -4504,7 +4505,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>67</v>
       </c>
@@ -4524,7 +4525,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>68</v>
       </c>
@@ -4544,7 +4545,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>69</v>
       </c>
@@ -4564,7 +4565,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>70</v>
       </c>
@@ -4584,7 +4585,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>71</v>
       </c>
@@ -4604,7 +4605,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>72</v>
       </c>
@@ -4624,7 +4625,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>73</v>
       </c>
@@ -4644,37 +4645,37 @@
         <v>597</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A86" s="33">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="32">
         <v>74</v>
       </c>
-      <c r="B86" s="33">
+      <c r="B86" s="32">
         <v>148</v>
       </c>
       <c r="E86" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="F86" s="35" t="s">
+      <c r="F86" s="31" t="s">
         <v>594</v>
       </c>
-      <c r="G86" s="36" t="s">
+      <c r="G86" s="33" t="s">
         <v>601</v>
       </c>
       <c r="H86" s="18" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A87" s="33"/>
-      <c r="B87" s="33"/>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="32"/>
+      <c r="B87" s="32"/>
       <c r="E87" s="34"/>
-      <c r="F87" s="35"/>
-      <c r="G87" s="36"/>
+      <c r="F87" s="31"/>
+      <c r="G87" s="33"/>
       <c r="H87" s="18" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>75</v>
       </c>
@@ -4694,7 +4695,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>76</v>
       </c>
@@ -4714,7 +4715,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>77</v>
       </c>
@@ -4737,7 +4738,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>78</v>
       </c>
@@ -4757,7 +4758,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>79</v>
       </c>
@@ -4777,7 +4778,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>80</v>
       </c>
@@ -4800,7 +4801,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>81</v>
       </c>
@@ -4820,7 +4821,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>82</v>
       </c>
@@ -4840,39 +4841,39 @@
         <v>625</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A96" s="33">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="32">
         <v>83</v>
       </c>
-      <c r="B96" s="33">
+      <c r="B96" s="32">
         <v>179</v>
       </c>
-      <c r="C96" s="32"/>
+      <c r="C96" s="35"/>
       <c r="E96" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="F96" s="35" t="s">
+      <c r="F96" s="31" t="s">
         <v>621</v>
       </c>
-      <c r="G96" s="36" t="s">
+      <c r="G96" s="33" t="s">
         <v>626</v>
       </c>
       <c r="H96" s="18" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A97" s="33"/>
-      <c r="B97" s="33"/>
-      <c r="C97" s="32"/>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="32"/>
+      <c r="B97" s="32"/>
+      <c r="C97" s="35"/>
       <c r="E97" s="34"/>
-      <c r="F97" s="35"/>
-      <c r="G97" s="36"/>
+      <c r="F97" s="31"/>
+      <c r="G97" s="33"/>
       <c r="H97" s="18" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>84</v>
       </c>
@@ -4892,7 +4893,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>85</v>
       </c>
@@ -4912,7 +4913,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>86</v>
       </c>
@@ -4932,7 +4933,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>87</v>
       </c>
@@ -4952,7 +4953,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>88</v>
       </c>
@@ -4972,7 +4973,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>89</v>
       </c>
@@ -4992,7 +4993,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>90</v>
       </c>
@@ -5012,7 +5013,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>91</v>
       </c>
@@ -5032,7 +5033,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>92</v>
       </c>
@@ -5052,7 +5053,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>93</v>
       </c>
@@ -5072,7 +5073,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>94</v>
       </c>
@@ -5092,7 +5093,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>95</v>
       </c>
@@ -5112,7 +5113,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>96</v>
       </c>
@@ -5135,8 +5136,8 @@
         <v>670</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A111" s="33">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="32">
         <v>97</v>
       </c>
       <c r="B111" s="7">
@@ -5155,8 +5156,8 @@
         <v>675</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A112" s="33"/>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="32"/>
       <c r="B112" s="7">
         <v>227</v>
       </c>
@@ -5173,7 +5174,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>98</v>
       </c>
@@ -5196,7 +5197,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>99</v>
       </c>
@@ -5219,7 +5220,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>100</v>
       </c>
@@ -5239,7 +5240,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>101</v>
       </c>
@@ -5262,7 +5263,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>102</v>
       </c>
@@ -5285,7 +5286,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>103</v>
       </c>
@@ -5305,7 +5306,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>104</v>
       </c>
@@ -5319,8 +5320,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A120" s="33">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" s="32">
         <v>105</v>
       </c>
       <c r="B120" s="7">
@@ -5333,8 +5334,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A121" s="33"/>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" s="32"/>
       <c r="B121" s="7">
         <v>240</v>
       </c>
@@ -5345,7 +5346,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>106</v>
       </c>
@@ -5359,7 +5360,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>107</v>
       </c>
@@ -5373,7 +5374,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>108</v>
       </c>
@@ -5387,7 +5388,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>109</v>
       </c>
@@ -5401,7 +5402,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>110</v>
       </c>
@@ -5415,7 +5416,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>111</v>
       </c>
@@ -5429,7 +5430,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>112</v>
       </c>
@@ -5443,7 +5444,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>113</v>
       </c>
@@ -5457,7 +5458,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>114</v>
       </c>
@@ -5471,7 +5472,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>115</v>
       </c>
@@ -5485,7 +5486,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>116</v>
       </c>
@@ -5499,7 +5500,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>117</v>
       </c>
@@ -5513,7 +5514,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>118</v>
       </c>
@@ -5527,8 +5528,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A135" s="33">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="32">
         <v>119</v>
       </c>
       <c r="B135" s="7">
@@ -5541,8 +5542,8 @@
         <v>135</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A136" s="33"/>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="32"/>
       <c r="B136" s="7">
         <v>337</v>
       </c>
@@ -5553,7 +5554,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>120</v>
       </c>
@@ -5567,7 +5568,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>121</v>
       </c>
@@ -5581,7 +5582,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>122</v>
       </c>
@@ -5595,7 +5596,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>123</v>
       </c>
@@ -5609,7 +5610,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>124</v>
       </c>
@@ -5623,7 +5624,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>125</v>
       </c>
@@ -5637,7 +5638,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>126</v>
       </c>
@@ -5651,7 +5652,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>127</v>
       </c>
@@ -5665,7 +5666,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>128</v>
       </c>
@@ -5679,7 +5680,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>129</v>
       </c>
@@ -5693,7 +5694,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>130</v>
       </c>
@@ -5707,7 +5708,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>131</v>
       </c>
@@ -5721,7 +5722,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>132</v>
       </c>
@@ -5735,7 +5736,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>133</v>
       </c>
@@ -5749,7 +5750,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>134</v>
       </c>
@@ -5763,7 +5764,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>135</v>
       </c>
@@ -5777,7 +5778,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>136</v>
       </c>
@@ -5791,7 +5792,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>137</v>
       </c>
@@ -5805,7 +5806,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>138</v>
       </c>
@@ -5819,7 +5820,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>139</v>
       </c>
@@ -5833,7 +5834,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>140</v>
       </c>
@@ -5847,7 +5848,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>141</v>
       </c>
@@ -5861,7 +5862,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>142</v>
       </c>
@@ -5875,7 +5876,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>143</v>
       </c>
@@ -5889,7 +5890,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>144</v>
       </c>
@@ -5903,7 +5904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>145</v>
       </c>
@@ -5917,7 +5918,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>146</v>
       </c>
@@ -5931,7 +5932,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>147</v>
       </c>
@@ -5945,7 +5946,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>148</v>
       </c>
@@ -5959,7 +5960,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>149</v>
       </c>
@@ -5973,7 +5974,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>150</v>
       </c>
@@ -5987,7 +5988,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>151</v>
       </c>
@@ -6001,7 +6002,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>152</v>
       </c>
@@ -6015,7 +6016,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>153</v>
       </c>
@@ -6035,7 +6036,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>154</v>
       </c>
@@ -6049,7 +6050,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>155</v>
       </c>
@@ -6069,7 +6070,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>156</v>
       </c>
@@ -6083,7 +6084,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>157</v>
       </c>
@@ -6097,7 +6098,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>158</v>
       </c>
@@ -6111,7 +6112,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>159</v>
       </c>
@@ -6125,7 +6126,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>160</v>
       </c>
@@ -6139,7 +6140,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>161</v>
       </c>
@@ -6153,7 +6154,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>162</v>
       </c>
@@ -6167,7 +6168,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>163</v>
       </c>
@@ -6181,7 +6182,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>164</v>
       </c>
@@ -6195,7 +6196,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>165</v>
       </c>
@@ -6215,7 +6216,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>166</v>
       </c>
@@ -6229,7 +6230,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>167</v>
       </c>
@@ -6243,7 +6244,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>168</v>
       </c>
@@ -6257,7 +6258,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>169</v>
       </c>
@@ -6271,7 +6272,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>170</v>
       </c>
@@ -6285,7 +6286,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>171</v>
       </c>
@@ -6299,7 +6300,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>172</v>
       </c>
@@ -6313,7 +6314,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>173</v>
       </c>
@@ -6327,7 +6328,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>174</v>
       </c>
@@ -6341,7 +6342,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>175</v>
       </c>
@@ -6355,7 +6356,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>176</v>
       </c>
@@ -6369,7 +6370,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <v>177</v>
       </c>
@@ -6383,7 +6384,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>178</v>
       </c>
@@ -6397,7 +6398,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <v>179</v>
       </c>
@@ -6411,7 +6412,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <v>180</v>
       </c>
@@ -6425,7 +6426,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>181</v>
       </c>
@@ -6439,7 +6440,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>182</v>
       </c>
@@ -6453,7 +6454,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <v>183</v>
       </c>
@@ -6467,7 +6468,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>184</v>
       </c>
@@ -6481,7 +6482,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <v>185</v>
       </c>
@@ -6495,7 +6496,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <v>186</v>
       </c>
@@ -6509,7 +6510,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <v>187</v>
       </c>
@@ -6523,7 +6524,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>188</v>
       </c>
@@ -6537,7 +6538,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
         <v>189</v>
       </c>
@@ -6551,7 +6552,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <v>190</v>
       </c>
@@ -6565,7 +6566,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <v>191</v>
       </c>
@@ -6579,7 +6580,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>192</v>
       </c>
@@ -6593,7 +6594,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>193</v>
       </c>
@@ -6607,7 +6608,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>194</v>
       </c>
@@ -6621,7 +6622,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>195</v>
       </c>
@@ -6635,7 +6636,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>196</v>
       </c>
@@ -6649,7 +6650,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>197</v>
       </c>
@@ -6663,7 +6664,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>198</v>
       </c>
@@ -6677,7 +6678,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>199</v>
       </c>
@@ -6691,7 +6692,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>200</v>
       </c>
@@ -6711,7 +6712,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>201</v>
       </c>
@@ -6731,7 +6732,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>202</v>
       </c>
@@ -6745,7 +6746,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>203</v>
       </c>
@@ -6759,7 +6760,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <v>204</v>
       </c>
@@ -6773,7 +6774,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>205</v>
       </c>
@@ -6787,7 +6788,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>206</v>
       </c>
@@ -6801,7 +6802,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>207</v>
       </c>
@@ -6815,7 +6816,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <v>208</v>
       </c>
@@ -6832,10 +6833,10 @@
   </sheetData>
   <autoFilter ref="A1:I225" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="39">
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="E56:E57"/>
     <mergeCell ref="G56:G57"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="F28:F29"/>
@@ -6848,29 +6849,29 @@
     <mergeCell ref="E63:E64"/>
     <mergeCell ref="A63:A64"/>
     <mergeCell ref="B63:B64"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="G86:G87"/>
+    <mergeCell ref="G96:G97"/>
+    <mergeCell ref="F96:F97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="B86:B87"/>
     <mergeCell ref="A86:A87"/>
     <mergeCell ref="A96:A97"/>
     <mergeCell ref="B56:B57"/>
     <mergeCell ref="B96:B97"/>
     <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="G86:G87"/>
-    <mergeCell ref="G96:G97"/>
-    <mergeCell ref="F96:F97"/>
-    <mergeCell ref="E96:E97"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="E86:E87"/>
-    <mergeCell ref="F86:F87"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A50:A51"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
+ Add 0039 组合总和
</commit_message>
<xml_diff>
--- a/面试高频题.xlsx
+++ b/面试高频题.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C2D7FF-41AB-4AB9-B0E5-A53218CBD49F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACC2F1A-1676-4AA6-8BEE-77934EC37BAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2606,23 +2606,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2971,8 +2971,8 @@
   <dimension ref="A1:I225"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E55" sqref="E55"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -3541,21 +3541,21 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="32">
+      <c r="A28" s="31">
         <v>26</v>
       </c>
-      <c r="B28" s="32">
+      <c r="B28" s="31">
         <v>46</v>
       </c>
-      <c r="C28" s="35"/>
-      <c r="D28" s="36"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="32"/>
       <c r="E28" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="F28" s="31" t="s">
+      <c r="F28" s="36" t="s">
         <v>390</v>
       </c>
-      <c r="G28" s="33" t="s">
+      <c r="G28" s="35" t="s">
         <v>391</v>
       </c>
       <c r="H28" s="29" t="s">
@@ -3563,19 +3563,19 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="36"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="32"/>
       <c r="E29" s="34"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="33"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="35"/>
       <c r="H29" s="29" t="s">
         <v>710</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
+      <c r="A30" s="31"/>
       <c r="B30" s="7">
         <v>47</v>
       </c>
@@ -3750,7 +3750,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="32">
+      <c r="A39" s="31">
         <v>35</v>
       </c>
       <c r="B39" s="7">
@@ -3770,7 +3770,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="32"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="7">
         <v>63</v>
       </c>
@@ -3890,6 +3890,7 @@
       <c r="B46" s="7">
         <v>78</v>
       </c>
+      <c r="D46" s="28"/>
       <c r="E46" s="4" t="s">
         <v>42</v>
       </c>
@@ -3910,6 +3911,7 @@
       <c r="B47" s="7">
         <v>79</v>
       </c>
+      <c r="D47" s="28"/>
       <c r="E47" s="4" t="s">
         <v>43</v>
       </c>
@@ -3924,7 +3926,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="32">
+      <c r="A48" s="31">
         <v>43</v>
       </c>
       <c r="B48" s="7">
@@ -3940,7 +3942,7 @@
       <c r="H48" s="10"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+      <c r="A49" s="31"/>
       <c r="B49" s="7">
         <v>83</v>
       </c>
@@ -3958,7 +3960,7 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="32">
+      <c r="A50" s="31">
         <v>44</v>
       </c>
       <c r="B50" s="7">
@@ -3978,7 +3980,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="32"/>
+      <c r="A51" s="31"/>
       <c r="B51" s="7">
         <v>725</v>
       </c>
@@ -4016,19 +4018,20 @@
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="32">
+      <c r="A53" s="31">
         <v>46</v>
       </c>
-      <c r="B53" s="32">
+      <c r="B53" s="31">
         <v>90</v>
       </c>
+      <c r="D53" s="28"/>
       <c r="E53" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="F53" s="31" t="s">
+      <c r="F53" s="36" t="s">
         <v>448</v>
       </c>
-      <c r="G53" s="33" t="s">
+      <c r="G53" s="35" t="s">
         <v>451</v>
       </c>
       <c r="H53" s="10" t="s">
@@ -4036,11 +4039,12 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="32"/>
-      <c r="B54" s="32"/>
+      <c r="A54" s="31"/>
+      <c r="B54" s="31"/>
+      <c r="D54" s="28"/>
       <c r="E54" s="34"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="33"/>
+      <c r="F54" s="36"/>
+      <c r="G54" s="35"/>
       <c r="H54" s="10" t="s">
         <v>452</v>
       </c>
@@ -4067,16 +4071,16 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
-      <c r="B56" s="32">
+      <c r="B56" s="31">
         <v>92</v>
       </c>
       <c r="E56" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="F56" s="31" t="s">
+      <c r="F56" s="36" t="s">
         <v>450</v>
       </c>
-      <c r="G56" s="33" t="s">
+      <c r="G56" s="35" t="s">
         <v>456</v>
       </c>
       <c r="H56" s="10" t="s">
@@ -4087,10 +4091,10 @@
       <c r="A57" s="2">
         <v>48</v>
       </c>
-      <c r="B57" s="32"/>
+      <c r="B57" s="31"/>
       <c r="E57" s="34"/>
-      <c r="F57" s="31"/>
-      <c r="G57" s="33"/>
+      <c r="F57" s="36"/>
+      <c r="G57" s="35"/>
       <c r="H57" s="10" t="s">
         <v>457</v>
       </c>
@@ -4198,19 +4202,19 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="32">
+      <c r="A63" s="31">
         <v>54</v>
       </c>
-      <c r="B63" s="32">
+      <c r="B63" s="31">
         <v>102</v>
       </c>
       <c r="E63" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="F63" s="31" t="s">
+      <c r="F63" s="36" t="s">
         <v>470</v>
       </c>
-      <c r="G63" s="33" t="s">
+      <c r="G63" s="35" t="s">
         <v>476</v>
       </c>
       <c r="H63" s="9" t="s">
@@ -4218,11 +4222,11 @@
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="32"/>
-      <c r="B64" s="32"/>
+      <c r="A64" s="31"/>
+      <c r="B64" s="31"/>
       <c r="E64" s="34"/>
-      <c r="F64" s="31"/>
-      <c r="G64" s="33"/>
+      <c r="F64" s="36"/>
+      <c r="G64" s="35"/>
       <c r="H64" s="10" t="s">
         <v>475</v>
       </c>
@@ -4388,7 +4392,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="32">
+      <c r="A73" s="31">
         <v>62</v>
       </c>
       <c r="B73" s="7">
@@ -4408,7 +4412,7 @@
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="32"/>
+      <c r="A74" s="31"/>
       <c r="B74" s="7">
         <v>119</v>
       </c>
@@ -4646,19 +4650,19 @@
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="32">
+      <c r="A86" s="31">
         <v>74</v>
       </c>
-      <c r="B86" s="32">
+      <c r="B86" s="31">
         <v>148</v>
       </c>
       <c r="E86" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="F86" s="31" t="s">
+      <c r="F86" s="36" t="s">
         <v>594</v>
       </c>
-      <c r="G86" s="33" t="s">
+      <c r="G86" s="35" t="s">
         <v>601</v>
       </c>
       <c r="H86" s="18" t="s">
@@ -4666,11 +4670,11 @@
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="32"/>
-      <c r="B87" s="32"/>
+      <c r="A87" s="31"/>
+      <c r="B87" s="31"/>
       <c r="E87" s="34"/>
-      <c r="F87" s="31"/>
-      <c r="G87" s="33"/>
+      <c r="F87" s="36"/>
+      <c r="G87" s="35"/>
       <c r="H87" s="18" t="s">
         <v>602</v>
       </c>
@@ -4842,20 +4846,20 @@
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="32">
+      <c r="A96" s="31">
         <v>83</v>
       </c>
-      <c r="B96" s="32">
+      <c r="B96" s="31">
         <v>179</v>
       </c>
-      <c r="C96" s="35"/>
+      <c r="C96" s="33"/>
       <c r="E96" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="F96" s="31" t="s">
+      <c r="F96" s="36" t="s">
         <v>621</v>
       </c>
-      <c r="G96" s="33" t="s">
+      <c r="G96" s="35" t="s">
         <v>626</v>
       </c>
       <c r="H96" s="18" t="s">
@@ -4863,12 +4867,12 @@
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="32"/>
-      <c r="B97" s="32"/>
-      <c r="C97" s="35"/>
+      <c r="A97" s="31"/>
+      <c r="B97" s="31"/>
+      <c r="C97" s="33"/>
       <c r="E97" s="34"/>
-      <c r="F97" s="31"/>
-      <c r="G97" s="33"/>
+      <c r="F97" s="36"/>
+      <c r="G97" s="35"/>
       <c r="H97" s="18" t="s">
         <v>627</v>
       </c>
@@ -5137,7 +5141,7 @@
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="32">
+      <c r="A111" s="31">
         <v>97</v>
       </c>
       <c r="B111" s="7">
@@ -5157,7 +5161,7 @@
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="32"/>
+      <c r="A112" s="31"/>
       <c r="B112" s="7">
         <v>227</v>
       </c>
@@ -5321,7 +5325,7 @@
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="32">
+      <c r="A120" s="31">
         <v>105</v>
       </c>
       <c r="B120" s="7">
@@ -5335,7 +5339,7 @@
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A121" s="32"/>
+      <c r="A121" s="31"/>
       <c r="B121" s="7">
         <v>240</v>
       </c>
@@ -5529,7 +5533,7 @@
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="32">
+      <c r="A135" s="31">
         <v>119</v>
       </c>
       <c r="B135" s="7">
@@ -5543,7 +5547,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="32"/>
+      <c r="A136" s="31"/>
       <c r="B136" s="7">
         <v>337</v>
       </c>
@@ -6833,6 +6837,31 @@
   </sheetData>
   <autoFilter ref="A1:I225" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="39">
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="G86:G87"/>
+    <mergeCell ref="G96:G97"/>
+    <mergeCell ref="F96:F97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:B64"/>
     <mergeCell ref="A53:A54"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="C28:C29"/>
@@ -6844,34 +6873,9 @@
     <mergeCell ref="G53:G54"/>
     <mergeCell ref="E53:E54"/>
     <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="G86:G87"/>
-    <mergeCell ref="G96:G97"/>
-    <mergeCell ref="F96:F97"/>
-    <mergeCell ref="E96:E97"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="E86:E87"/>
-    <mergeCell ref="F86:F87"/>
     <mergeCell ref="F56:F57"/>
     <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A96:A97"/>
     <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A50:A51"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
+ Add 0002 两数相加
</commit_message>
<xml_diff>
--- a/面试高频题.xlsx
+++ b/面试高频题.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A276CE-C291-4555-B8AD-3CA70C41286C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A823AFE-6A09-475A-9231-0592030CC056}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2516,7 +2516,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2609,14 +2609,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2624,10 +2621,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2977,8 +2980,8 @@
   <dimension ref="A1:I225"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -3050,6 +3053,7 @@
       <c r="B3" s="7">
         <v>2</v>
       </c>
+      <c r="D3" s="32"/>
       <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
@@ -3549,21 +3553,21 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="38">
+      <c r="A28" s="33">
         <v>26</v>
       </c>
-      <c r="B28" s="38">
+      <c r="B28" s="33">
         <v>46</v>
       </c>
-      <c r="C28" s="33"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="34" t="s">
+      <c r="C28" s="37"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="F28" s="36" t="s">
+      <c r="F28" s="35" t="s">
         <v>390</v>
       </c>
-      <c r="G28" s="35" t="s">
+      <c r="G28" s="34" t="s">
         <v>391</v>
       </c>
       <c r="H28" s="29" t="s">
@@ -3571,19 +3575,19 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="38"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="35"/>
+      <c r="A29" s="33"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="34"/>
       <c r="H29" s="29" t="s">
         <v>710</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="38"/>
+      <c r="A30" s="33"/>
       <c r="B30" s="7">
         <v>47</v>
       </c>
@@ -3758,7 +3762,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="38">
+      <c r="A39" s="33">
         <v>35</v>
       </c>
       <c r="B39" s="7">
@@ -3778,7 +3782,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="38"/>
+      <c r="A40" s="33"/>
       <c r="B40" s="7">
         <v>63</v>
       </c>
@@ -3934,7 +3938,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="38">
+      <c r="A48" s="33">
         <v>43</v>
       </c>
       <c r="B48" s="7">
@@ -3950,7 +3954,7 @@
       <c r="H48" s="10"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="38"/>
+      <c r="A49" s="33"/>
       <c r="B49" s="7">
         <v>83</v>
       </c>
@@ -3968,7 +3972,7 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="38">
+      <c r="A50" s="33">
         <v>44</v>
       </c>
       <c r="B50" s="7">
@@ -3988,7 +3992,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="38"/>
+      <c r="A51" s="33"/>
       <c r="B51" s="7">
         <v>725</v>
       </c>
@@ -4026,21 +4030,21 @@
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="38">
+      <c r="A53" s="33">
         <v>46</v>
       </c>
-      <c r="B53" s="38">
+      <c r="B53" s="33">
         <v>90</v>
       </c>
-      <c r="C53" s="33"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="34" t="s">
+      <c r="C53" s="37"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="F53" s="36" t="s">
+      <c r="F53" s="35" t="s">
         <v>448</v>
       </c>
-      <c r="G53" s="35" t="s">
+      <c r="G53" s="34" t="s">
         <v>451</v>
       </c>
       <c r="H53" s="10" t="s">
@@ -4048,13 +4052,13 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="38"/>
-      <c r="B54" s="38"/>
-      <c r="C54" s="33"/>
-      <c r="D54" s="37"/>
-      <c r="E54" s="34"/>
-      <c r="F54" s="36"/>
-      <c r="G54" s="35"/>
+      <c r="A54" s="33"/>
+      <c r="B54" s="33"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="39"/>
+      <c r="E54" s="36"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="34"/>
       <c r="H54" s="10" t="s">
         <v>452</v>
       </c>
@@ -4081,16 +4085,16 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
-      <c r="B56" s="38">
+      <c r="B56" s="33">
         <v>92</v>
       </c>
-      <c r="E56" s="34" t="s">
+      <c r="E56" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="F56" s="36" t="s">
+      <c r="F56" s="35" t="s">
         <v>450</v>
       </c>
-      <c r="G56" s="35" t="s">
+      <c r="G56" s="34" t="s">
         <v>456</v>
       </c>
       <c r="H56" s="10" t="s">
@@ -4101,10 +4105,10 @@
       <c r="A57" s="2">
         <v>48</v>
       </c>
-      <c r="B57" s="38"/>
-      <c r="E57" s="34"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="35"/>
+      <c r="B57" s="33"/>
+      <c r="E57" s="36"/>
+      <c r="F57" s="35"/>
+      <c r="G57" s="34"/>
       <c r="H57" s="10" t="s">
         <v>457</v>
       </c>
@@ -4212,19 +4216,19 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="38">
+      <c r="A63" s="33">
         <v>54</v>
       </c>
-      <c r="B63" s="38">
+      <c r="B63" s="33">
         <v>102</v>
       </c>
-      <c r="E63" s="34" t="s">
+      <c r="E63" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="F63" s="36" t="s">
+      <c r="F63" s="35" t="s">
         <v>470</v>
       </c>
-      <c r="G63" s="35" t="s">
+      <c r="G63" s="34" t="s">
         <v>476</v>
       </c>
       <c r="H63" s="9" t="s">
@@ -4232,11 +4236,11 @@
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="38"/>
-      <c r="B64" s="38"/>
-      <c r="E64" s="34"/>
-      <c r="F64" s="36"/>
-      <c r="G64" s="35"/>
+      <c r="A64" s="33"/>
+      <c r="B64" s="33"/>
+      <c r="E64" s="36"/>
+      <c r="F64" s="35"/>
+      <c r="G64" s="34"/>
       <c r="H64" s="10" t="s">
         <v>475</v>
       </c>
@@ -4402,7 +4406,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="38">
+      <c r="A73" s="33">
         <v>62</v>
       </c>
       <c r="B73" s="7">
@@ -4422,7 +4426,7 @@
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="38"/>
+      <c r="A74" s="33"/>
       <c r="B74" s="7">
         <v>119</v>
       </c>
@@ -4660,21 +4664,21 @@
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="38">
+      <c r="A86" s="33">
         <v>74</v>
       </c>
-      <c r="B86" s="38">
+      <c r="B86" s="33">
         <v>148</v>
       </c>
-      <c r="C86" s="33"/>
-      <c r="D86" s="38"/>
-      <c r="E86" s="34" t="s">
+      <c r="C86" s="37"/>
+      <c r="D86" s="33"/>
+      <c r="E86" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="F86" s="36" t="s">
+      <c r="F86" s="35" t="s">
         <v>594</v>
       </c>
-      <c r="G86" s="35" t="s">
+      <c r="G86" s="34" t="s">
         <v>601</v>
       </c>
       <c r="H86" s="18" t="s">
@@ -4682,13 +4686,13 @@
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="38"/>
-      <c r="B87" s="38"/>
-      <c r="C87" s="33"/>
-      <c r="D87" s="38"/>
-      <c r="E87" s="34"/>
-      <c r="F87" s="36"/>
-      <c r="G87" s="35"/>
+      <c r="A87" s="33"/>
+      <c r="B87" s="33"/>
+      <c r="C87" s="37"/>
+      <c r="D87" s="33"/>
+      <c r="E87" s="36"/>
+      <c r="F87" s="35"/>
+      <c r="G87" s="34"/>
       <c r="H87" s="18" t="s">
         <v>602</v>
       </c>
@@ -4860,21 +4864,21 @@
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="38">
+      <c r="A96" s="33">
         <v>83</v>
       </c>
-      <c r="B96" s="38">
+      <c r="B96" s="33">
         <v>179</v>
       </c>
-      <c r="C96" s="33"/>
-      <c r="D96" s="38"/>
-      <c r="E96" s="34" t="s">
+      <c r="C96" s="37"/>
+      <c r="D96" s="33"/>
+      <c r="E96" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="F96" s="36" t="s">
+      <c r="F96" s="35" t="s">
         <v>621</v>
       </c>
-      <c r="G96" s="35" t="s">
+      <c r="G96" s="34" t="s">
         <v>626</v>
       </c>
       <c r="H96" s="18" t="s">
@@ -4882,13 +4886,13 @@
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="38"/>
-      <c r="B97" s="38"/>
-      <c r="C97" s="33"/>
-      <c r="D97" s="38"/>
-      <c r="E97" s="34"/>
-      <c r="F97" s="36"/>
-      <c r="G97" s="35"/>
+      <c r="A97" s="33"/>
+      <c r="B97" s="33"/>
+      <c r="C97" s="37"/>
+      <c r="D97" s="33"/>
+      <c r="E97" s="36"/>
+      <c r="F97" s="35"/>
+      <c r="G97" s="34"/>
       <c r="H97" s="18" t="s">
         <v>627</v>
       </c>
@@ -5157,7 +5161,7 @@
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="38">
+      <c r="A111" s="33">
         <v>97</v>
       </c>
       <c r="B111" s="7">
@@ -5177,7 +5181,7 @@
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="38"/>
+      <c r="A112" s="33"/>
       <c r="B112" s="7">
         <v>227</v>
       </c>
@@ -5341,7 +5345,7 @@
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="38">
+      <c r="A120" s="33">
         <v>105</v>
       </c>
       <c r="B120" s="7">
@@ -5355,7 +5359,7 @@
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A121" s="38"/>
+      <c r="A121" s="33"/>
       <c r="B121" s="7">
         <v>240</v>
       </c>
@@ -5549,7 +5553,7 @@
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="38">
+      <c r="A135" s="33">
         <v>119</v>
       </c>
       <c r="B135" s="7">
@@ -5563,7 +5567,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="38"/>
+      <c r="A136" s="33"/>
       <c r="B136" s="7">
         <v>337</v>
       </c>
@@ -6425,6 +6429,7 @@
       <c r="C196" s="13" t="s">
         <v>522</v>
       </c>
+      <c r="D196" s="32"/>
       <c r="E196" s="5" t="s">
         <v>252</v>
       </c>
@@ -6853,37 +6858,6 @@
   </sheetData>
   <autoFilter ref="A1:I225" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="44">
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="G86:G87"/>
-    <mergeCell ref="G96:G97"/>
-    <mergeCell ref="F96:F97"/>
-    <mergeCell ref="E96:E97"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="E86:E87"/>
-    <mergeCell ref="F86:F87"/>
-    <mergeCell ref="D86:D87"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="B63:B64"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="E56:E57"/>
@@ -6897,6 +6871,37 @@
     <mergeCell ref="F56:F57"/>
     <mergeCell ref="C53:C54"/>
     <mergeCell ref="D53:D54"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="G86:G87"/>
+    <mergeCell ref="G96:G97"/>
+    <mergeCell ref="F96:F97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="D96:D97"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B56:B57"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
+ Add two math problems
</commit_message>
<xml_diff>
--- a/面试高频题.xlsx
+++ b/面试高频题.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A823AFE-6A09-475A-9231-0592030CC056}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034EB361-38E8-43EA-B0C6-6738A6FA08DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2516,7 +2516,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2612,8 +2612,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2621,16 +2636,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2979,25 +2988,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I225"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.36328125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.08984375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="7.26953125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="7.6328125" style="25" customWidth="1"/>
-    <col min="5" max="5" width="37.36328125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="6.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="7.25" style="13" customWidth="1"/>
+    <col min="4" max="4" width="7.625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="37.375" style="5" customWidth="1"/>
     <col min="6" max="6" width="34" style="10" customWidth="1"/>
-    <col min="7" max="7" width="31.90625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="21.90625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="31.875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="21.875" style="3" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>311</v>
       </c>
@@ -3026,7 +3035,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3046,7 +3055,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3067,7 +3076,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3088,7 +3097,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3108,7 +3117,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -3128,13 +3137,14 @@
         <v>330</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="7">
         <v>7</v>
       </c>
+      <c r="D7" s="33"/>
       <c r="E7" s="4" t="s">
         <v>6</v>
       </c>
@@ -3148,13 +3158,14 @@
         <v>333</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="7">
         <v>9</v>
       </c>
+      <c r="D8" s="34"/>
       <c r="E8" s="4" t="s">
         <v>7</v>
       </c>
@@ -3168,7 +3179,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -3189,7 +3200,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -3209,7 +3220,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -3230,7 +3241,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -3250,7 +3261,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -3271,7 +3282,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -3291,7 +3302,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -3311,7 +3322,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -3331,7 +3342,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -3351,7 +3362,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -3372,7 +3383,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -3392,7 +3403,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -3412,7 +3423,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -3432,7 +3443,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -3452,7 +3463,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -3472,7 +3483,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -3492,7 +3503,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -3512,7 +3523,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -3532,7 +3543,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -3552,42 +3563,42 @@
         <v>389</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="33">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A28" s="42">
         <v>26</v>
       </c>
-      <c r="B28" s="33">
+      <c r="B28" s="42">
         <v>46</v>
       </c>
       <c r="C28" s="37"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="36" t="s">
+      <c r="D28" s="36"/>
+      <c r="E28" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="F28" s="35" t="s">
+      <c r="F28" s="40" t="s">
         <v>390</v>
       </c>
-      <c r="G28" s="34" t="s">
+      <c r="G28" s="39" t="s">
         <v>391</v>
       </c>
       <c r="H28" s="29" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="33"/>
-      <c r="B29" s="33"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A29" s="42"/>
+      <c r="B29" s="42"/>
       <c r="C29" s="37"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="34"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="39"/>
       <c r="H29" s="29" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="33"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A30" s="42"/>
       <c r="B30" s="7">
         <v>47</v>
       </c>
@@ -3601,7 +3612,7 @@
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
         <v>27</v>
       </c>
@@ -3621,7 +3632,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <v>28</v>
       </c>
@@ -3641,13 +3652,14 @@
         <v>397</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
         <v>29</v>
       </c>
       <c r="B33" s="7">
         <v>50</v>
       </c>
+      <c r="D33" s="34"/>
       <c r="E33" s="4" t="s">
         <v>30</v>
       </c>
@@ -3661,7 +3673,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A34" s="2">
         <v>30</v>
       </c>
@@ -3681,7 +3693,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A35" s="2">
         <v>31</v>
       </c>
@@ -3701,7 +3713,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A36" s="2">
         <v>32</v>
       </c>
@@ -3721,7 +3733,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
         <v>33</v>
       </c>
@@ -3741,7 +3753,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A38" s="2">
         <v>34</v>
       </c>
@@ -3761,8 +3773,8 @@
         <v>415</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="33">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A39" s="42">
         <v>35</v>
       </c>
       <c r="B39" s="7">
@@ -3781,8 +3793,8 @@
         <v>417</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A40" s="42"/>
       <c r="B40" s="7">
         <v>63</v>
       </c>
@@ -3795,7 +3807,7 @@
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A41" s="2">
         <v>36</v>
       </c>
@@ -3815,7 +3827,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
         <v>37</v>
       </c>
@@ -3835,13 +3847,14 @@
         <v>424</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A43" s="2">
         <v>38</v>
       </c>
       <c r="B43" s="7">
         <v>69</v>
       </c>
+      <c r="D43" s="35"/>
       <c r="E43" s="4" t="s">
         <v>39</v>
       </c>
@@ -3855,7 +3868,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
         <v>39</v>
       </c>
@@ -3875,7 +3888,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A45" s="2">
         <v>40</v>
       </c>
@@ -3895,7 +3908,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A46" s="2">
         <v>41</v>
       </c>
@@ -3916,7 +3929,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A47" s="2">
         <v>42</v>
       </c>
@@ -3937,8 +3950,8 @@
         <v>440</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="33">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A48" s="42">
         <v>43</v>
       </c>
       <c r="B48" s="7">
@@ -3953,8 +3966,8 @@
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="33"/>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A49" s="42"/>
       <c r="B49" s="7">
         <v>83</v>
       </c>
@@ -3971,8 +3984,8 @@
         <v>442</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="33">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A50" s="42">
         <v>44</v>
       </c>
       <c r="B50" s="7">
@@ -3991,8 +4004,8 @@
         <v>444</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="33"/>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A51" s="42"/>
       <c r="B51" s="7">
         <v>725</v>
       </c>
@@ -4009,7 +4022,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A52" s="2">
         <v>45</v>
       </c>
@@ -4029,41 +4042,41 @@
         <v>447</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="33">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A53" s="42">
         <v>46</v>
       </c>
-      <c r="B53" s="33">
+      <c r="B53" s="42">
         <v>90</v>
       </c>
       <c r="C53" s="37"/>
-      <c r="D53" s="39"/>
-      <c r="E53" s="36" t="s">
+      <c r="D53" s="41"/>
+      <c r="E53" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="F53" s="35" t="s">
+      <c r="F53" s="40" t="s">
         <v>448</v>
       </c>
-      <c r="G53" s="34" t="s">
+      <c r="G53" s="39" t="s">
         <v>451</v>
       </c>
       <c r="H53" s="10" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="33"/>
-      <c r="B54" s="33"/>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A54" s="42"/>
+      <c r="B54" s="42"/>
       <c r="C54" s="37"/>
-      <c r="D54" s="39"/>
-      <c r="E54" s="36"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="34"/>
+      <c r="D54" s="41"/>
+      <c r="E54" s="38"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="39"/>
       <c r="H54" s="10" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A55" s="2">
         <v>47</v>
       </c>
@@ -4083,37 +4096,37 @@
         <v>455</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A56" s="7"/>
-      <c r="B56" s="33">
+      <c r="B56" s="42">
         <v>92</v>
       </c>
-      <c r="E56" s="36" t="s">
+      <c r="E56" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="F56" s="35" t="s">
+      <c r="F56" s="40" t="s">
         <v>450</v>
       </c>
-      <c r="G56" s="34" t="s">
+      <c r="G56" s="39" t="s">
         <v>456</v>
       </c>
       <c r="H56" s="10" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A57" s="2">
         <v>48</v>
       </c>
-      <c r="B57" s="33"/>
-      <c r="E57" s="36"/>
-      <c r="F57" s="35"/>
-      <c r="G57" s="34"/>
+      <c r="B57" s="42"/>
+      <c r="E57" s="38"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="39"/>
       <c r="H57" s="10" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A58" s="2">
         <v>49</v>
       </c>
@@ -4133,7 +4146,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A59" s="7">
         <v>50</v>
       </c>
@@ -4155,7 +4168,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A60" s="2">
         <v>51</v>
       </c>
@@ -4175,7 +4188,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A61" s="2">
         <v>52</v>
       </c>
@@ -4195,7 +4208,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A62" s="2">
         <v>53</v>
       </c>
@@ -4215,37 +4228,37 @@
         <v>473</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="33">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A63" s="42">
         <v>54</v>
       </c>
-      <c r="B63" s="33">
+      <c r="B63" s="42">
         <v>102</v>
       </c>
-      <c r="E63" s="36" t="s">
+      <c r="E63" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="F63" s="35" t="s">
+      <c r="F63" s="40" t="s">
         <v>470</v>
       </c>
-      <c r="G63" s="34" t="s">
+      <c r="G63" s="39" t="s">
         <v>476</v>
       </c>
       <c r="H63" s="9" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="33"/>
-      <c r="B64" s="33"/>
-      <c r="E64" s="36"/>
-      <c r="F64" s="35"/>
-      <c r="G64" s="34"/>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A64" s="42"/>
+      <c r="B64" s="42"/>
+      <c r="E64" s="38"/>
+      <c r="F64" s="40"/>
+      <c r="G64" s="39"/>
       <c r="H64" s="10" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A65" s="2">
         <v>55</v>
       </c>
@@ -4265,7 +4278,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A66" s="2">
         <v>56</v>
       </c>
@@ -4285,7 +4298,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A67" s="2">
         <v>57</v>
       </c>
@@ -4305,7 +4318,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A68" s="2">
         <v>58</v>
       </c>
@@ -4325,7 +4338,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A69" s="2">
         <v>59</v>
       </c>
@@ -4345,7 +4358,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A70" s="2">
         <v>60</v>
       </c>
@@ -4365,7 +4378,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A71" s="2">
         <v>60</v>
       </c>
@@ -4385,7 +4398,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A72" s="2">
         <v>61</v>
       </c>
@@ -4405,8 +4418,8 @@
         <v>564</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="33">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A73" s="42">
         <v>62</v>
       </c>
       <c r="B73" s="7">
@@ -4425,8 +4438,8 @@
         <v>566</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="33"/>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A74" s="42"/>
       <c r="B74" s="7">
         <v>119</v>
       </c>
@@ -4443,7 +4456,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A75" s="2">
         <v>63</v>
       </c>
@@ -4463,7 +4476,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A76" s="2">
         <v>64</v>
       </c>
@@ -4483,7 +4496,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A77" s="2">
         <v>65</v>
       </c>
@@ -4503,7 +4516,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A78" s="2">
         <v>66</v>
       </c>
@@ -4523,7 +4536,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A79" s="2">
         <v>67</v>
       </c>
@@ -4543,7 +4556,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A80" s="2">
         <v>68</v>
       </c>
@@ -4563,7 +4576,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A81" s="2">
         <v>69</v>
       </c>
@@ -4583,7 +4596,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A82" s="2">
         <v>70</v>
       </c>
@@ -4603,7 +4616,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A83" s="2">
         <v>71</v>
       </c>
@@ -4623,7 +4636,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A84" s="2">
         <v>72</v>
       </c>
@@ -4643,7 +4656,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A85" s="2">
         <v>73</v>
       </c>
@@ -4663,41 +4676,41 @@
         <v>597</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="33">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A86" s="42">
         <v>74</v>
       </c>
-      <c r="B86" s="33">
+      <c r="B86" s="42">
         <v>148</v>
       </c>
       <c r="C86" s="37"/>
-      <c r="D86" s="33"/>
-      <c r="E86" s="36" t="s">
+      <c r="D86" s="42"/>
+      <c r="E86" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="F86" s="35" t="s">
+      <c r="F86" s="40" t="s">
         <v>594</v>
       </c>
-      <c r="G86" s="34" t="s">
+      <c r="G86" s="39" t="s">
         <v>601</v>
       </c>
       <c r="H86" s="18" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="33"/>
-      <c r="B87" s="33"/>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A87" s="42"/>
+      <c r="B87" s="42"/>
       <c r="C87" s="37"/>
-      <c r="D87" s="33"/>
-      <c r="E87" s="36"/>
-      <c r="F87" s="35"/>
-      <c r="G87" s="34"/>
+      <c r="D87" s="42"/>
+      <c r="E87" s="38"/>
+      <c r="F87" s="40"/>
+      <c r="G87" s="39"/>
       <c r="H87" s="18" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A88" s="2">
         <v>75</v>
       </c>
@@ -4717,7 +4730,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A89" s="2">
         <v>76</v>
       </c>
@@ -4737,7 +4750,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A90" s="2">
         <v>77</v>
       </c>
@@ -4760,7 +4773,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A91" s="2">
         <v>78</v>
       </c>
@@ -4780,7 +4793,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A92" s="2">
         <v>79</v>
       </c>
@@ -4800,7 +4813,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A93" s="2">
         <v>80</v>
       </c>
@@ -4823,7 +4836,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A94" s="2">
         <v>81</v>
       </c>
@@ -4843,7 +4856,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A95" s="2">
         <v>82</v>
       </c>
@@ -4863,41 +4876,41 @@
         <v>625</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="33">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A96" s="42">
         <v>83</v>
       </c>
-      <c r="B96" s="33">
+      <c r="B96" s="42">
         <v>179</v>
       </c>
       <c r="C96" s="37"/>
-      <c r="D96" s="33"/>
-      <c r="E96" s="36" t="s">
+      <c r="D96" s="42"/>
+      <c r="E96" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="F96" s="35" t="s">
+      <c r="F96" s="40" t="s">
         <v>621</v>
       </c>
-      <c r="G96" s="34" t="s">
+      <c r="G96" s="39" t="s">
         <v>626</v>
       </c>
       <c r="H96" s="18" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="33"/>
-      <c r="B97" s="33"/>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A97" s="42"/>
+      <c r="B97" s="42"/>
       <c r="C97" s="37"/>
-      <c r="D97" s="33"/>
-      <c r="E97" s="36"/>
-      <c r="F97" s="35"/>
-      <c r="G97" s="34"/>
+      <c r="D97" s="42"/>
+      <c r="E97" s="38"/>
+      <c r="F97" s="40"/>
+      <c r="G97" s="39"/>
       <c r="H97" s="18" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A98" s="2">
         <v>84</v>
       </c>
@@ -4917,7 +4930,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A99" s="2">
         <v>85</v>
       </c>
@@ -4937,7 +4950,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A100" s="2">
         <v>86</v>
       </c>
@@ -4957,7 +4970,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A101" s="2">
         <v>87</v>
       </c>
@@ -4977,7 +4990,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A102" s="2">
         <v>88</v>
       </c>
@@ -4997,7 +5010,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A103" s="2">
         <v>89</v>
       </c>
@@ -5017,7 +5030,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A104" s="2">
         <v>90</v>
       </c>
@@ -5037,7 +5050,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A105" s="2">
         <v>91</v>
       </c>
@@ -5057,7 +5070,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A106" s="2">
         <v>92</v>
       </c>
@@ -5077,7 +5090,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A107" s="2">
         <v>93</v>
       </c>
@@ -5097,7 +5110,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A108" s="2">
         <v>94</v>
       </c>
@@ -5117,7 +5130,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A109" s="2">
         <v>95</v>
       </c>
@@ -5137,7 +5150,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A110" s="2">
         <v>96</v>
       </c>
@@ -5160,8 +5173,8 @@
         <v>670</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="33">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A111" s="42">
         <v>97</v>
       </c>
       <c r="B111" s="7">
@@ -5180,8 +5193,8 @@
         <v>675</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="33"/>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A112" s="42"/>
       <c r="B112" s="7">
         <v>227</v>
       </c>
@@ -5198,7 +5211,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A113" s="2">
         <v>98</v>
       </c>
@@ -5221,7 +5234,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A114" s="2">
         <v>99</v>
       </c>
@@ -5244,7 +5257,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A115" s="2">
         <v>100</v>
       </c>
@@ -5264,7 +5277,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A116" s="2">
         <v>101</v>
       </c>
@@ -5287,7 +5300,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A117" s="2">
         <v>102</v>
       </c>
@@ -5310,7 +5323,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A118" s="2">
         <v>103</v>
       </c>
@@ -5330,7 +5343,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A119" s="2">
         <v>104</v>
       </c>
@@ -5344,8 +5357,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="33">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A120" s="42">
         <v>105</v>
       </c>
       <c r="B120" s="7">
@@ -5358,8 +5371,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A121" s="33"/>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A121" s="42"/>
       <c r="B121" s="7">
         <v>240</v>
       </c>
@@ -5370,7 +5383,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A122" s="2">
         <v>106</v>
       </c>
@@ -5384,7 +5397,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A123" s="2">
         <v>107</v>
       </c>
@@ -5398,7 +5411,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A124" s="2">
         <v>108</v>
       </c>
@@ -5412,7 +5425,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A125" s="2">
         <v>109</v>
       </c>
@@ -5426,7 +5439,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A126" s="2">
         <v>110</v>
       </c>
@@ -5440,7 +5453,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A127" s="2">
         <v>111</v>
       </c>
@@ -5454,7 +5467,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A128" s="2">
         <v>112</v>
       </c>
@@ -5468,7 +5481,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A129" s="2">
         <v>113</v>
       </c>
@@ -5482,7 +5495,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A130" s="2">
         <v>114</v>
       </c>
@@ -5496,7 +5509,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A131" s="2">
         <v>115</v>
       </c>
@@ -5510,7 +5523,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A132" s="2">
         <v>116</v>
       </c>
@@ -5524,7 +5537,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A133" s="2">
         <v>117</v>
       </c>
@@ -5538,7 +5551,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A134" s="2">
         <v>118</v>
       </c>
@@ -5552,8 +5565,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="33">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A135" s="42">
         <v>119</v>
       </c>
       <c r="B135" s="7">
@@ -5566,8 +5579,8 @@
         <v>135</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="33"/>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A136" s="42"/>
       <c r="B136" s="7">
         <v>337</v>
       </c>
@@ -5578,7 +5591,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A137" s="2">
         <v>120</v>
       </c>
@@ -5592,7 +5605,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A138" s="2">
         <v>121</v>
       </c>
@@ -5606,7 +5619,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A139" s="2">
         <v>122</v>
       </c>
@@ -5620,7 +5633,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A140" s="2">
         <v>123</v>
       </c>
@@ -5634,7 +5647,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A141" s="2">
         <v>124</v>
       </c>
@@ -5648,7 +5661,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A142" s="2">
         <v>125</v>
       </c>
@@ -5662,7 +5675,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A143" s="2">
         <v>126</v>
       </c>
@@ -5676,7 +5689,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A144" s="2">
         <v>127</v>
       </c>
@@ -5690,7 +5703,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A145" s="2">
         <v>128</v>
       </c>
@@ -5704,7 +5717,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A146" s="2">
         <v>129</v>
       </c>
@@ -5718,7 +5731,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A147" s="2">
         <v>130</v>
       </c>
@@ -5732,7 +5745,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A148" s="2">
         <v>131</v>
       </c>
@@ -5746,7 +5759,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A149" s="2">
         <v>132</v>
       </c>
@@ -5760,7 +5773,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A150" s="2">
         <v>133</v>
       </c>
@@ -5774,7 +5787,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A151" s="2">
         <v>134</v>
       </c>
@@ -5788,7 +5801,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A152" s="2">
         <v>135</v>
       </c>
@@ -5802,7 +5815,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A153" s="2">
         <v>136</v>
       </c>
@@ -5816,7 +5829,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A154" s="2">
         <v>137</v>
       </c>
@@ -5830,7 +5843,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A155" s="2">
         <v>138</v>
       </c>
@@ -5844,7 +5857,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A156" s="2">
         <v>139</v>
       </c>
@@ -5858,7 +5871,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A157" s="2">
         <v>140</v>
       </c>
@@ -5872,7 +5885,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A158" s="2">
         <v>141</v>
       </c>
@@ -5886,7 +5899,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A159" s="2">
         <v>142</v>
       </c>
@@ -5900,7 +5913,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A160" s="2">
         <v>143</v>
       </c>
@@ -5914,7 +5927,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A161" s="2">
         <v>144</v>
       </c>
@@ -5928,7 +5941,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A162" s="2">
         <v>145</v>
       </c>
@@ -5942,7 +5955,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A163" s="2">
         <v>146</v>
       </c>
@@ -5956,7 +5969,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A164" s="2">
         <v>147</v>
       </c>
@@ -5970,7 +5983,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A165" s="2">
         <v>148</v>
       </c>
@@ -5984,7 +5997,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A166" s="2">
         <v>149</v>
       </c>
@@ -5998,7 +6011,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A167" s="2">
         <v>150</v>
       </c>
@@ -6012,7 +6025,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A168" s="2">
         <v>151</v>
       </c>
@@ -6026,7 +6039,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A169" s="2">
         <v>152</v>
       </c>
@@ -6040,7 +6053,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A170" s="2">
         <v>153</v>
       </c>
@@ -6060,7 +6073,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A171" s="2">
         <v>154</v>
       </c>
@@ -6074,7 +6087,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A172" s="2">
         <v>155</v>
       </c>
@@ -6094,7 +6107,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A173" s="2">
         <v>156</v>
       </c>
@@ -6108,7 +6121,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A174" s="2">
         <v>157</v>
       </c>
@@ -6122,7 +6135,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A175" s="2">
         <v>158</v>
       </c>
@@ -6136,7 +6149,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A176" s="2">
         <v>159</v>
       </c>
@@ -6150,7 +6163,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A177" s="2">
         <v>160</v>
       </c>
@@ -6164,7 +6177,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A178" s="2">
         <v>161</v>
       </c>
@@ -6178,7 +6191,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A179" s="2">
         <v>162</v>
       </c>
@@ -6192,7 +6205,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A180" s="2">
         <v>163</v>
       </c>
@@ -6206,7 +6219,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A181" s="2">
         <v>164</v>
       </c>
@@ -6220,7 +6233,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A182" s="2">
         <v>165</v>
       </c>
@@ -6240,7 +6253,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A183" s="2">
         <v>166</v>
       </c>
@@ -6254,7 +6267,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A184" s="2">
         <v>167</v>
       </c>
@@ -6268,7 +6281,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A185" s="2">
         <v>168</v>
       </c>
@@ -6282,7 +6295,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A186" s="2">
         <v>169</v>
       </c>
@@ -6296,7 +6309,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A187" s="2">
         <v>170</v>
       </c>
@@ -6310,7 +6323,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A188" s="2">
         <v>171</v>
       </c>
@@ -6324,7 +6337,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A189" s="2">
         <v>172</v>
       </c>
@@ -6338,7 +6351,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A190" s="2">
         <v>173</v>
       </c>
@@ -6352,7 +6365,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A191" s="2">
         <v>174</v>
       </c>
@@ -6366,7 +6379,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A192" s="2">
         <v>175</v>
       </c>
@@ -6380,7 +6393,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A193" s="2">
         <v>176</v>
       </c>
@@ -6394,7 +6407,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A194" s="2">
         <v>177</v>
       </c>
@@ -6408,7 +6421,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A195" s="2">
         <v>178</v>
       </c>
@@ -6422,7 +6435,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A196" s="2">
         <v>179</v>
       </c>
@@ -6437,7 +6450,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A197" s="2">
         <v>180</v>
       </c>
@@ -6451,7 +6464,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A198" s="2">
         <v>181</v>
       </c>
@@ -6465,7 +6478,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A199" s="2">
         <v>182</v>
       </c>
@@ -6479,7 +6492,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A200" s="2">
         <v>183</v>
       </c>
@@ -6493,7 +6506,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A201" s="2">
         <v>184</v>
       </c>
@@ -6507,7 +6520,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A202" s="2">
         <v>185</v>
       </c>
@@ -6521,7 +6534,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A203" s="2">
         <v>186</v>
       </c>
@@ -6535,7 +6548,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A204" s="2">
         <v>187</v>
       </c>
@@ -6549,7 +6562,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A205" s="2">
         <v>188</v>
       </c>
@@ -6563,7 +6576,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A206" s="2">
         <v>189</v>
       </c>
@@ -6577,7 +6590,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A207" s="2">
         <v>190</v>
       </c>
@@ -6591,7 +6604,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A208" s="2">
         <v>191</v>
       </c>
@@ -6605,7 +6618,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A209" s="2">
         <v>192</v>
       </c>
@@ -6619,7 +6632,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A210" s="2">
         <v>193</v>
       </c>
@@ -6633,7 +6646,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A211" s="2">
         <v>194</v>
       </c>
@@ -6647,7 +6660,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A212" s="2">
         <v>195</v>
       </c>
@@ -6661,7 +6674,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A213" s="2">
         <v>196</v>
       </c>
@@ -6675,7 +6688,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A214" s="2">
         <v>197</v>
       </c>
@@ -6689,7 +6702,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A215" s="2">
         <v>198</v>
       </c>
@@ -6703,7 +6716,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A216" s="2">
         <v>199</v>
       </c>
@@ -6717,7 +6730,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A217" s="2">
         <v>200</v>
       </c>
@@ -6737,7 +6750,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A218" s="2">
         <v>201</v>
       </c>
@@ -6757,7 +6770,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A219" s="2">
         <v>202</v>
       </c>
@@ -6771,7 +6784,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A220" s="2">
         <v>203</v>
       </c>
@@ -6785,7 +6798,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A221" s="2">
         <v>204</v>
       </c>
@@ -6799,7 +6812,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A222" s="2">
         <v>205</v>
       </c>
@@ -6813,7 +6826,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A223" s="2">
         <v>206</v>
       </c>
@@ -6827,7 +6840,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A224" s="2">
         <v>207</v>
       </c>
@@ -6841,7 +6854,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A225" s="2">
         <v>208</v>
       </c>
@@ -6858,6 +6871,37 @@
   </sheetData>
   <autoFilter ref="A1:I225" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="44">
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="G86:G87"/>
+    <mergeCell ref="G96:G97"/>
+    <mergeCell ref="F96:F97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="D96:D97"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:B64"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="E56:E57"/>
@@ -6871,37 +6915,6 @@
     <mergeCell ref="F56:F57"/>
     <mergeCell ref="C53:C54"/>
     <mergeCell ref="D53:D54"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="G86:G87"/>
-    <mergeCell ref="G96:G97"/>
-    <mergeCell ref="F96:F97"/>
-    <mergeCell ref="E96:E97"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="E86:E87"/>
-    <mergeCell ref="F86:F87"/>
-    <mergeCell ref="D86:D87"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B56:B57"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
+ Add 0227 and 0224
</commit_message>
<xml_diff>
--- a/面试高频题.xlsx
+++ b/面试高频题.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D116073-E299-476B-B4FC-2ACA55FC105E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5ADD93-7458-4EF2-B647-9DED7A528E76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2516,7 +2516,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2624,8 +2624,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2633,16 +2642,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2992,24 +2995,24 @@
   <dimension ref="A1:I225"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E101" sqref="E101"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="7.25" style="13" customWidth="1"/>
-    <col min="4" max="4" width="7.625" style="25" customWidth="1"/>
-    <col min="5" max="5" width="27.125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="6.36328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.08984375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="7.26953125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="7.6328125" style="25" customWidth="1"/>
+    <col min="5" max="5" width="27.08984375" style="5" customWidth="1"/>
     <col min="6" max="6" width="34" style="10" customWidth="1"/>
-    <col min="7" max="7" width="31.875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="21.875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="31.90625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="21.90625" style="3" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>311</v>
       </c>
@@ -3038,7 +3041,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3058,7 +3061,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3079,7 +3082,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3100,7 +3103,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3120,7 +3123,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -3140,7 +3143,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -3161,7 +3164,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -3182,7 +3185,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -3203,7 +3206,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -3223,7 +3226,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -3244,7 +3247,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -3264,7 +3267,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -3285,7 +3288,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -3305,7 +3308,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -3325,7 +3328,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -3345,7 +3348,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -3365,7 +3368,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -3386,7 +3389,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -3406,7 +3409,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -3426,7 +3429,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -3446,7 +3449,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -3466,7 +3469,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -3486,7 +3489,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -3506,7 +3509,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -3526,7 +3529,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -3546,7 +3549,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -3566,42 +3569,42 @@
         <v>389</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A28" s="37">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="44">
         <v>26</v>
       </c>
-      <c r="B28" s="37">
+      <c r="B28" s="44">
         <v>46</v>
       </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="42"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="38"/>
       <c r="E28" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="F28" s="39" t="s">
+      <c r="F28" s="42" t="s">
         <v>390</v>
       </c>
-      <c r="G28" s="38" t="s">
+      <c r="G28" s="41" t="s">
         <v>391</v>
       </c>
       <c r="H28" s="29" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A29" s="37"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="42"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="44"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="38"/>
       <c r="E29" s="40"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="38"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="41"/>
       <c r="H29" s="29" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A30" s="37"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="44"/>
       <c r="B30" s="7">
         <v>47</v>
       </c>
@@ -3615,7 +3618,7 @@
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>27</v>
       </c>
@@ -3635,7 +3638,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>28</v>
       </c>
@@ -3655,7 +3658,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>29</v>
       </c>
@@ -3676,7 +3679,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>30</v>
       </c>
@@ -3696,7 +3699,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>31</v>
       </c>
@@ -3716,7 +3719,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>32</v>
       </c>
@@ -3736,7 +3739,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>33</v>
       </c>
@@ -3756,7 +3759,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>34</v>
       </c>
@@ -3776,8 +3779,8 @@
         <v>415</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A39" s="37">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="44">
         <v>35</v>
       </c>
       <c r="B39" s="7">
@@ -3796,8 +3799,8 @@
         <v>417</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A40" s="37"/>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="44"/>
       <c r="B40" s="7">
         <v>63</v>
       </c>
@@ -3810,7 +3813,7 @@
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>36</v>
       </c>
@@ -3830,7 +3833,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>37</v>
       </c>
@@ -3850,7 +3853,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>38</v>
       </c>
@@ -3871,7 +3874,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>39</v>
       </c>
@@ -3891,7 +3894,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>40</v>
       </c>
@@ -3911,7 +3914,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>41</v>
       </c>
@@ -3932,7 +3935,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>42</v>
       </c>
@@ -3953,8 +3956,8 @@
         <v>440</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A48" s="37">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="44">
         <v>43</v>
       </c>
       <c r="B48" s="7">
@@ -3969,8 +3972,8 @@
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A49" s="37"/>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="44"/>
       <c r="B49" s="7">
         <v>83</v>
       </c>
@@ -3987,8 +3990,8 @@
         <v>442</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A50" s="37">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="44">
         <v>44</v>
       </c>
       <c r="B50" s="7">
@@ -4007,8 +4010,8 @@
         <v>444</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A51" s="37"/>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="44"/>
       <c r="B51" s="7">
         <v>725</v>
       </c>
@@ -4025,7 +4028,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>45</v>
       </c>
@@ -4045,41 +4048,41 @@
         <v>447</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A53" s="37">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="44">
         <v>46</v>
       </c>
-      <c r="B53" s="37">
+      <c r="B53" s="44">
         <v>90</v>
       </c>
-      <c r="C53" s="41"/>
+      <c r="C53" s="39"/>
       <c r="D53" s="43"/>
       <c r="E53" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="F53" s="39" t="s">
+      <c r="F53" s="42" t="s">
         <v>448</v>
       </c>
-      <c r="G53" s="38" t="s">
+      <c r="G53" s="41" t="s">
         <v>451</v>
       </c>
       <c r="H53" s="10" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A54" s="37"/>
-      <c r="B54" s="37"/>
-      <c r="C54" s="41"/>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="44"/>
+      <c r="B54" s="44"/>
+      <c r="C54" s="39"/>
       <c r="D54" s="43"/>
       <c r="E54" s="40"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="38"/>
+      <c r="F54" s="42"/>
+      <c r="G54" s="41"/>
       <c r="H54" s="10" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>47</v>
       </c>
@@ -4099,37 +4102,37 @@
         <v>455</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
-      <c r="B56" s="37">
+      <c r="B56" s="44">
         <v>92</v>
       </c>
       <c r="E56" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="F56" s="39" t="s">
+      <c r="F56" s="42" t="s">
         <v>450</v>
       </c>
-      <c r="G56" s="38" t="s">
+      <c r="G56" s="41" t="s">
         <v>456</v>
       </c>
       <c r="H56" s="10" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>48</v>
       </c>
-      <c r="B57" s="37"/>
+      <c r="B57" s="44"/>
       <c r="E57" s="40"/>
-      <c r="F57" s="39"/>
-      <c r="G57" s="38"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="41"/>
       <c r="H57" s="10" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>49</v>
       </c>
@@ -4149,7 +4152,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>50</v>
       </c>
@@ -4171,7 +4174,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>51</v>
       </c>
@@ -4191,7 +4194,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>52</v>
       </c>
@@ -4211,7 +4214,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>53</v>
       </c>
@@ -4231,37 +4234,37 @@
         <v>473</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A63" s="37">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="44">
         <v>54</v>
       </c>
-      <c r="B63" s="37">
+      <c r="B63" s="44">
         <v>102</v>
       </c>
       <c r="E63" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="F63" s="39" t="s">
+      <c r="F63" s="42" t="s">
         <v>470</v>
       </c>
-      <c r="G63" s="38" t="s">
+      <c r="G63" s="41" t="s">
         <v>476</v>
       </c>
       <c r="H63" s="9" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A64" s="37"/>
-      <c r="B64" s="37"/>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="44"/>
+      <c r="B64" s="44"/>
       <c r="E64" s="40"/>
-      <c r="F64" s="39"/>
-      <c r="G64" s="38"/>
+      <c r="F64" s="42"/>
+      <c r="G64" s="41"/>
       <c r="H64" s="10" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>55</v>
       </c>
@@ -4281,7 +4284,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>56</v>
       </c>
@@ -4301,7 +4304,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>57</v>
       </c>
@@ -4321,7 +4324,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>58</v>
       </c>
@@ -4341,7 +4344,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>59</v>
       </c>
@@ -4361,7 +4364,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>60</v>
       </c>
@@ -4381,7 +4384,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>60</v>
       </c>
@@ -4401,7 +4404,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>61</v>
       </c>
@@ -4421,8 +4424,8 @@
         <v>564</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A73" s="37">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="44">
         <v>62</v>
       </c>
       <c r="B73" s="7">
@@ -4441,8 +4444,8 @@
         <v>566</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A74" s="37"/>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="44"/>
       <c r="B74" s="7">
         <v>119</v>
       </c>
@@ -4459,7 +4462,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>63</v>
       </c>
@@ -4479,7 +4482,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>64</v>
       </c>
@@ -4499,7 +4502,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>65</v>
       </c>
@@ -4519,7 +4522,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>66</v>
       </c>
@@ -4539,7 +4542,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>67</v>
       </c>
@@ -4559,7 +4562,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>68</v>
       </c>
@@ -4579,7 +4582,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>69</v>
       </c>
@@ -4599,7 +4602,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>70</v>
       </c>
@@ -4619,7 +4622,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>71</v>
       </c>
@@ -4639,7 +4642,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>72</v>
       </c>
@@ -4659,7 +4662,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>73</v>
       </c>
@@ -4679,41 +4682,41 @@
         <v>597</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A86" s="37">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="44">
         <v>74</v>
       </c>
-      <c r="B86" s="37">
+      <c r="B86" s="44">
         <v>148</v>
       </c>
-      <c r="C86" s="41"/>
-      <c r="D86" s="37"/>
+      <c r="C86" s="39"/>
+      <c r="D86" s="44"/>
       <c r="E86" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="F86" s="39" t="s">
+      <c r="F86" s="42" t="s">
         <v>594</v>
       </c>
-      <c r="G86" s="38" t="s">
+      <c r="G86" s="41" t="s">
         <v>601</v>
       </c>
       <c r="H86" s="18" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A87" s="37"/>
-      <c r="B87" s="37"/>
-      <c r="C87" s="41"/>
-      <c r="D87" s="37"/>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="44"/>
+      <c r="B87" s="44"/>
+      <c r="C87" s="39"/>
+      <c r="D87" s="44"/>
       <c r="E87" s="40"/>
-      <c r="F87" s="39"/>
-      <c r="G87" s="38"/>
+      <c r="F87" s="42"/>
+      <c r="G87" s="41"/>
       <c r="H87" s="18" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>75</v>
       </c>
@@ -4733,7 +4736,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>76</v>
       </c>
@@ -4753,7 +4756,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>77</v>
       </c>
@@ -4776,7 +4779,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>78</v>
       </c>
@@ -4796,7 +4799,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>79</v>
       </c>
@@ -4816,7 +4819,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>80</v>
       </c>
@@ -4839,7 +4842,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>81</v>
       </c>
@@ -4860,7 +4863,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>82</v>
       </c>
@@ -4881,41 +4884,41 @@
         <v>625</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A96" s="37">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="44">
         <v>83</v>
       </c>
-      <c r="B96" s="37">
+      <c r="B96" s="44">
         <v>179</v>
       </c>
-      <c r="C96" s="41"/>
-      <c r="D96" s="37"/>
+      <c r="C96" s="39"/>
+      <c r="D96" s="44"/>
       <c r="E96" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="F96" s="39" t="s">
+      <c r="F96" s="42" t="s">
         <v>621</v>
       </c>
-      <c r="G96" s="38" t="s">
+      <c r="G96" s="41" t="s">
         <v>626</v>
       </c>
       <c r="H96" s="18" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A97" s="37"/>
-      <c r="B97" s="37"/>
-      <c r="C97" s="41"/>
-      <c r="D97" s="37"/>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="44"/>
+      <c r="B97" s="44"/>
+      <c r="C97" s="39"/>
+      <c r="D97" s="44"/>
       <c r="E97" s="40"/>
-      <c r="F97" s="39"/>
-      <c r="G97" s="38"/>
+      <c r="F97" s="42"/>
+      <c r="G97" s="41"/>
       <c r="H97" s="18" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>84</v>
       </c>
@@ -4935,7 +4938,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>85</v>
       </c>
@@ -4955,7 +4958,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>86</v>
       </c>
@@ -4975,7 +4978,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>87</v>
       </c>
@@ -4995,7 +4998,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>88</v>
       </c>
@@ -5015,7 +5018,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>89</v>
       </c>
@@ -5036,7 +5039,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>90</v>
       </c>
@@ -5056,7 +5059,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>91</v>
       </c>
@@ -5076,7 +5079,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>92</v>
       </c>
@@ -5096,7 +5099,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>93</v>
       </c>
@@ -5116,7 +5119,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>94</v>
       </c>
@@ -5136,7 +5139,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>95</v>
       </c>
@@ -5156,7 +5159,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>96</v>
       </c>
@@ -5179,13 +5182,14 @@
         <v>670</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A111" s="37">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="44">
         <v>97</v>
       </c>
       <c r="B111" s="7">
-        <v>224</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="D111" s="37"/>
       <c r="E111" s="4" t="s">
         <v>673</v>
       </c>
@@ -5199,11 +5203,12 @@
         <v>675</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A112" s="37"/>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="44"/>
       <c r="B112" s="7">
-        <v>227</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="D112" s="37"/>
       <c r="E112" s="4" t="s">
         <v>674</v>
       </c>
@@ -5217,7 +5222,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>98</v>
       </c>
@@ -5240,7 +5245,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>99</v>
       </c>
@@ -5263,7 +5268,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>100</v>
       </c>
@@ -5283,7 +5288,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>101</v>
       </c>
@@ -5306,7 +5311,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>102</v>
       </c>
@@ -5329,7 +5334,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>103</v>
       </c>
@@ -5349,7 +5354,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>104</v>
       </c>
@@ -5363,8 +5368,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A120" s="37">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" s="44">
         <v>105</v>
       </c>
       <c r="B120" s="7">
@@ -5377,8 +5382,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A121" s="37"/>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" s="44"/>
       <c r="B121" s="7">
         <v>240</v>
       </c>
@@ -5389,7 +5394,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>106</v>
       </c>
@@ -5403,7 +5408,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>107</v>
       </c>
@@ -5417,7 +5422,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>108</v>
       </c>
@@ -5431,7 +5436,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>109</v>
       </c>
@@ -5445,7 +5450,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>110</v>
       </c>
@@ -5459,7 +5464,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>111</v>
       </c>
@@ -5473,7 +5478,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>112</v>
       </c>
@@ -5487,7 +5492,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>113</v>
       </c>
@@ -5501,7 +5506,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>114</v>
       </c>
@@ -5515,7 +5520,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>115</v>
       </c>
@@ -5529,7 +5534,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>116</v>
       </c>
@@ -5543,7 +5548,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>117</v>
       </c>
@@ -5557,7 +5562,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>118</v>
       </c>
@@ -5571,8 +5576,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A135" s="37">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="44">
         <v>119</v>
       </c>
       <c r="B135" s="7">
@@ -5585,8 +5590,8 @@
         <v>135</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A136" s="37"/>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="44"/>
       <c r="B136" s="7">
         <v>337</v>
       </c>
@@ -5597,7 +5602,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>120</v>
       </c>
@@ -5611,7 +5616,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>121</v>
       </c>
@@ -5625,7 +5630,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>122</v>
       </c>
@@ -5639,7 +5644,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>123</v>
       </c>
@@ -5653,7 +5658,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>124</v>
       </c>
@@ -5667,7 +5672,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>125</v>
       </c>
@@ -5681,7 +5686,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>126</v>
       </c>
@@ -5695,7 +5700,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>127</v>
       </c>
@@ -5709,7 +5714,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>128</v>
       </c>
@@ -5723,7 +5728,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>129</v>
       </c>
@@ -5737,7 +5742,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>130</v>
       </c>
@@ -5751,7 +5756,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>131</v>
       </c>
@@ -5765,7 +5770,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>132</v>
       </c>
@@ -5779,7 +5784,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>133</v>
       </c>
@@ -5793,7 +5798,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>134</v>
       </c>
@@ -5807,7 +5812,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>135</v>
       </c>
@@ -5821,7 +5826,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>136</v>
       </c>
@@ -5835,7 +5840,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>137</v>
       </c>
@@ -5849,7 +5854,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>138</v>
       </c>
@@ -5863,7 +5868,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>139</v>
       </c>
@@ -5877,7 +5882,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>140</v>
       </c>
@@ -5891,7 +5896,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>141</v>
       </c>
@@ -5905,7 +5910,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>142</v>
       </c>
@@ -5919,7 +5924,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>143</v>
       </c>
@@ -5933,7 +5938,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>144</v>
       </c>
@@ -5947,7 +5952,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>145</v>
       </c>
@@ -5961,7 +5966,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>146</v>
       </c>
@@ -5975,7 +5980,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>147</v>
       </c>
@@ -5989,7 +5994,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>148</v>
       </c>
@@ -6003,7 +6008,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>149</v>
       </c>
@@ -6017,7 +6022,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>150</v>
       </c>
@@ -6031,7 +6036,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>151</v>
       </c>
@@ -6045,7 +6050,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>152</v>
       </c>
@@ -6059,7 +6064,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>153</v>
       </c>
@@ -6079,7 +6084,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>154</v>
       </c>
@@ -6093,7 +6098,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>155</v>
       </c>
@@ -6113,7 +6118,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>156</v>
       </c>
@@ -6127,7 +6132,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>157</v>
       </c>
@@ -6141,7 +6146,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>158</v>
       </c>
@@ -6155,7 +6160,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>159</v>
       </c>
@@ -6169,7 +6174,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>160</v>
       </c>
@@ -6183,7 +6188,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>161</v>
       </c>
@@ -6197,7 +6202,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>162</v>
       </c>
@@ -6211,7 +6216,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>163</v>
       </c>
@@ -6225,7 +6230,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>164</v>
       </c>
@@ -6239,7 +6244,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>165</v>
       </c>
@@ -6259,7 +6264,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>166</v>
       </c>
@@ -6273,7 +6278,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>167</v>
       </c>
@@ -6287,7 +6292,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>168</v>
       </c>
@@ -6301,7 +6306,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>169</v>
       </c>
@@ -6315,7 +6320,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>170</v>
       </c>
@@ -6329,7 +6334,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>171</v>
       </c>
@@ -6343,7 +6348,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>172</v>
       </c>
@@ -6357,7 +6362,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>173</v>
       </c>
@@ -6371,7 +6376,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>174</v>
       </c>
@@ -6385,7 +6390,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>175</v>
       </c>
@@ -6399,7 +6404,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>176</v>
       </c>
@@ -6413,7 +6418,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <v>177</v>
       </c>
@@ -6427,7 +6432,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>178</v>
       </c>
@@ -6441,7 +6446,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <v>179</v>
       </c>
@@ -6456,7 +6461,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <v>180</v>
       </c>
@@ -6470,7 +6475,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>181</v>
       </c>
@@ -6484,7 +6489,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>182</v>
       </c>
@@ -6498,7 +6503,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <v>183</v>
       </c>
@@ -6512,7 +6517,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>184</v>
       </c>
@@ -6526,7 +6531,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <v>185</v>
       </c>
@@ -6540,7 +6545,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <v>186</v>
       </c>
@@ -6554,7 +6559,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <v>187</v>
       </c>
@@ -6568,7 +6573,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>188</v>
       </c>
@@ -6582,7 +6587,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
         <v>189</v>
       </c>
@@ -6596,7 +6601,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <v>190</v>
       </c>
@@ -6610,7 +6615,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <v>191</v>
       </c>
@@ -6624,7 +6629,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>192</v>
       </c>
@@ -6638,7 +6643,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>193</v>
       </c>
@@ -6652,7 +6657,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>194</v>
       </c>
@@ -6666,7 +6671,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>195</v>
       </c>
@@ -6680,7 +6685,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>196</v>
       </c>
@@ -6694,7 +6699,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>197</v>
       </c>
@@ -6708,7 +6713,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>198</v>
       </c>
@@ -6722,7 +6727,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>199</v>
       </c>
@@ -6736,7 +6741,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>200</v>
       </c>
@@ -6756,7 +6761,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>201</v>
       </c>
@@ -6776,7 +6781,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>202</v>
       </c>
@@ -6790,7 +6795,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>203</v>
       </c>
@@ -6804,7 +6809,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <v>204</v>
       </c>
@@ -6818,7 +6823,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>205</v>
       </c>
@@ -6832,7 +6837,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>206</v>
       </c>
@@ -6846,7 +6851,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>207</v>
       </c>
@@ -6860,7 +6865,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <v>208</v>
       </c>
@@ -6877,6 +6882,37 @@
   </sheetData>
   <autoFilter ref="A1:I225" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="44">
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="G86:G87"/>
+    <mergeCell ref="G96:G97"/>
+    <mergeCell ref="F96:F97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="D96:D97"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:B64"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="E56:E57"/>
@@ -6890,37 +6926,6 @@
     <mergeCell ref="F56:F57"/>
     <mergeCell ref="C53:C54"/>
     <mergeCell ref="D53:D54"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="G86:G87"/>
-    <mergeCell ref="G96:G97"/>
-    <mergeCell ref="F96:F97"/>
-    <mergeCell ref="E96:E97"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="E86:E87"/>
-    <mergeCell ref="F86:F87"/>
-    <mergeCell ref="D86:D87"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B56:B57"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
+ Add a dp problem
</commit_message>
<xml_diff>
--- a/面试高频题.xlsx
+++ b/面试高频题.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5ADD93-7458-4EF2-B647-9DED7A528E76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A19EB8-3CDE-446D-8234-C90D5C519C78}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -908,9 +908,6 @@
     <t>https://leetcode-cn.com/problems/er-cha-sou-suo-shu-de-di-kda-jie-dian-lcof</t>
   </si>
   <si>
-    <t>丑数</t>
-  </si>
-  <si>
     <t>不用加减乘除做加法</t>
   </si>
   <si>
@@ -2443,6 +2440,10 @@
   </si>
   <si>
     <t>https://leetcode-cn.com/problems/permutations-ii</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>丑数 II</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2516,7 +2517,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2627,14 +2628,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2642,10 +2643,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2995,8 +3002,8 @@
   <dimension ref="A1:I225"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E105" sqref="E105"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -3014,31 +3021,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>552</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>553</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>703</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>315</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3052,13 +3059,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>318</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3073,13 +3080,13 @@
         <v>1</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3094,13 +3101,13 @@
         <v>2</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3114,13 +3121,13 @@
         <v>3</v>
       </c>
       <c r="F5" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -3134,13 +3141,13 @@
         <v>5</v>
       </c>
       <c r="F6" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>329</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3155,13 +3162,13 @@
         <v>6</v>
       </c>
       <c r="F7" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>332</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3176,13 +3183,13 @@
         <v>7</v>
       </c>
       <c r="F8" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>335</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -3197,13 +3204,13 @@
         <v>8</v>
       </c>
       <c r="F9" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>338</v>
-      </c>
       <c r="H9" s="26" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3217,13 +3224,13 @@
         <v>9</v>
       </c>
       <c r="F10" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>340</v>
-      </c>
       <c r="H10" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -3238,13 +3245,13 @@
         <v>10</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H11" s="26" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3258,13 +3265,13 @@
         <v>11</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G12" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>345</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -3279,13 +3286,13 @@
         <v>12</v>
       </c>
       <c r="F13" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>347</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3299,13 +3306,13 @@
         <v>13</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G14" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>351</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3319,13 +3326,13 @@
         <v>14</v>
       </c>
       <c r="F15" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>354</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -3339,13 +3346,13 @@
         <v>15</v>
       </c>
       <c r="F16" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>357</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -3359,13 +3366,13 @@
         <v>16</v>
       </c>
       <c r="F17" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>360</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -3380,13 +3387,13 @@
         <v>17</v>
       </c>
       <c r="F18" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>363</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -3400,13 +3407,13 @@
         <v>18</v>
       </c>
       <c r="F19" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>366</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -3420,13 +3427,13 @@
         <v>19</v>
       </c>
       <c r="F20" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>368</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -3440,13 +3447,13 @@
         <v>20</v>
       </c>
       <c r="F21" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="H21" s="3" t="s">
         <v>370</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -3460,13 +3467,13 @@
         <v>21</v>
       </c>
       <c r="F22" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="H22" s="3" t="s">
         <v>373</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -3480,13 +3487,13 @@
         <v>22</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -3500,13 +3507,13 @@
         <v>23</v>
       </c>
       <c r="F24" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>378</v>
-      </c>
       <c r="H24" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -3520,13 +3527,13 @@
         <v>24</v>
       </c>
       <c r="F25" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="H25" s="3" t="s">
         <v>382</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -3540,13 +3547,13 @@
         <v>25</v>
       </c>
       <c r="F26" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>385</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -3560,60 +3567,60 @@
         <v>26</v>
       </c>
       <c r="F27" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="H27" s="3" t="s">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="40">
+        <v>26</v>
+      </c>
+      <c r="B28" s="40">
+        <v>46</v>
+      </c>
+      <c r="C28" s="44"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="42" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="44">
-        <v>26</v>
-      </c>
-      <c r="B28" s="44">
-        <v>46</v>
-      </c>
-      <c r="C28" s="39"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="F28" s="42" t="s">
+      <c r="G28" s="41" t="s">
         <v>390</v>
       </c>
-      <c r="G28" s="41" t="s">
-        <v>391</v>
-      </c>
       <c r="H28" s="29" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
-      <c r="B29" s="44"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="40"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="43"/>
       <c r="F29" s="42"/>
       <c r="G29" s="41"/>
       <c r="H29" s="29" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="7">
         <v>47</v>
       </c>
       <c r="D30" s="28"/>
       <c r="E30" s="8" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
@@ -3629,13 +3636,13 @@
         <v>28</v>
       </c>
       <c r="F31" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="H31" s="3" t="s">
         <v>392</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3649,13 +3656,13 @@
         <v>29</v>
       </c>
       <c r="F32" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="H32" s="3" t="s">
         <v>396</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3670,13 +3677,13 @@
         <v>30</v>
       </c>
       <c r="F33" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="G33" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="H33" s="3" t="s">
         <v>399</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3690,13 +3697,13 @@
         <v>31</v>
       </c>
       <c r="F34" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="H34" s="3" t="s">
         <v>401</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3710,13 +3717,13 @@
         <v>32</v>
       </c>
       <c r="F35" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="H35" s="3" t="s">
         <v>404</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3730,13 +3737,13 @@
         <v>33</v>
       </c>
       <c r="F36" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>408</v>
-      </c>
       <c r="H36" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3750,13 +3757,13 @@
         <v>34</v>
       </c>
       <c r="F37" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="H37" s="3" t="s">
         <v>410</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3770,17 +3777,17 @@
         <v>35</v>
       </c>
       <c r="F38" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="G38" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="H38" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="H38" s="3" t="s">
-        <v>415</v>
-      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="44">
+      <c r="A39" s="40">
         <v>35</v>
       </c>
       <c r="B39" s="7">
@@ -3790,25 +3797,25 @@
         <v>36</v>
       </c>
       <c r="F39" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="H39" s="3" t="s">
         <v>416</v>
       </c>
-      <c r="G39" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>417</v>
-      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="44"/>
+      <c r="A40" s="40"/>
       <c r="B40" s="7">
         <v>63</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
@@ -3824,13 +3831,13 @@
         <v>37</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3844,13 +3851,13 @@
         <v>38</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G42" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="H42" s="3" t="s">
         <v>423</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -3865,13 +3872,13 @@
         <v>39</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G43" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="H43" s="3" t="s">
         <v>425</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -3885,13 +3892,13 @@
         <v>40</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3905,13 +3912,13 @@
         <v>41</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3926,13 +3933,13 @@
         <v>42</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3947,33 +3954,33 @@
         <v>43</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="44">
+      <c r="A48" s="40">
         <v>43</v>
       </c>
       <c r="B48" s="7">
         <v>82</v>
       </c>
       <c r="E48" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="F48" s="9" t="s">
         <v>493</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>494</v>
       </c>
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="44"/>
+      <c r="A49" s="40"/>
       <c r="B49" s="7">
         <v>83</v>
       </c>
@@ -3981,17 +3988,17 @@
         <v>44</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="44">
+      <c r="A50" s="40">
         <v>44</v>
       </c>
       <c r="B50" s="7">
@@ -4001,17 +4008,17 @@
         <v>45</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H50" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="44"/>
+      <c r="A51" s="40"/>
       <c r="B51" s="7">
         <v>725</v>
       </c>
@@ -4019,13 +4026,13 @@
         <v>45</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H51" s="10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -4039,47 +4046,47 @@
         <v>46</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G52" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="H52" s="10" t="s">
         <v>446</v>
       </c>
-      <c r="H52" s="10" t="s">
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="40">
+        <v>46</v>
+      </c>
+      <c r="B53" s="40">
+        <v>90</v>
+      </c>
+      <c r="C53" s="44"/>
+      <c r="D53" s="46"/>
+      <c r="E53" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="F53" s="42" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="44">
-        <v>46</v>
-      </c>
-      <c r="B53" s="44">
-        <v>90</v>
-      </c>
-      <c r="C53" s="39"/>
-      <c r="D53" s="43"/>
-      <c r="E53" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="F53" s="42" t="s">
-        <v>448</v>
-      </c>
       <c r="G53" s="41" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="H53" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="44"/>
-      <c r="B54" s="44"/>
-      <c r="C54" s="39"/>
-      <c r="D54" s="43"/>
-      <c r="E54" s="40"/>
+      <c r="A54" s="40"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="44"/>
+      <c r="D54" s="46"/>
+      <c r="E54" s="43"/>
       <c r="F54" s="42"/>
       <c r="G54" s="41"/>
       <c r="H54" s="10" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -4093,43 +4100,43 @@
         <v>48</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G55" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="H55" s="10" t="s">
         <v>454</v>
-      </c>
-      <c r="H55" s="10" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
-      <c r="B56" s="44">
+      <c r="B56" s="40">
         <v>92</v>
       </c>
-      <c r="E56" s="40" t="s">
+      <c r="E56" s="43" t="s">
         <v>49</v>
       </c>
       <c r="F56" s="42" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G56" s="41" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>48</v>
       </c>
-      <c r="B57" s="44"/>
-      <c r="E57" s="40"/>
+      <c r="B57" s="40"/>
+      <c r="E57" s="43"/>
       <c r="F57" s="42"/>
       <c r="G57" s="41"/>
       <c r="H57" s="10" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -4143,13 +4150,13 @@
         <v>50</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G58" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="H58" s="10" t="s">
         <v>462</v>
-      </c>
-      <c r="H58" s="10" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -4165,13 +4172,13 @@
         <v>51</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G59" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="H59" s="10" t="s">
         <v>464</v>
-      </c>
-      <c r="H59" s="10" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -4185,13 +4192,13 @@
         <v>52</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -4205,13 +4212,13 @@
         <v>53</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H61" s="10" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -4225,43 +4232,43 @@
         <v>54</v>
       </c>
       <c r="F62" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="H62" s="9" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="40">
+        <v>54</v>
+      </c>
+      <c r="B63" s="40">
+        <v>102</v>
+      </c>
+      <c r="E63" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="F63" s="42" t="s">
         <v>469</v>
       </c>
-      <c r="G62" s="3" t="s">
-        <v>474</v>
-      </c>
-      <c r="H62" s="9" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="44">
-        <v>54</v>
-      </c>
-      <c r="B63" s="44">
-        <v>102</v>
-      </c>
-      <c r="E63" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="F63" s="42" t="s">
-        <v>470</v>
-      </c>
       <c r="G63" s="41" t="s">
+        <v>475</v>
+      </c>
+      <c r="H63" s="9" t="s">
         <v>476</v>
       </c>
-      <c r="H63" s="9" t="s">
-        <v>477</v>
-      </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="44"/>
-      <c r="B64" s="44"/>
-      <c r="E64" s="40"/>
+      <c r="A64" s="40"/>
+      <c r="B64" s="40"/>
+      <c r="E64" s="43"/>
       <c r="F64" s="42"/>
       <c r="G64" s="41"/>
       <c r="H64" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -4275,13 +4282,13 @@
         <v>56</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H65" s="10" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -4295,13 +4302,13 @@
         <v>57</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H66" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -4315,13 +4322,13 @@
         <v>58</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H67" s="10" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -4335,13 +4342,13 @@
         <v>59</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H68" s="10" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -4355,13 +4362,13 @@
         <v>60</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H69" s="12" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -4375,13 +4382,13 @@
         <v>61</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H70" s="27" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -4395,13 +4402,13 @@
         <v>62</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="H71" s="27" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -4415,17 +4422,17 @@
         <v>63</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="G72" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="H72" s="12" t="s">
         <v>563</v>
       </c>
-      <c r="H72" s="12" t="s">
-        <v>564</v>
-      </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="44">
+      <c r="A73" s="40">
         <v>62</v>
       </c>
       <c r="B73" s="7">
@@ -4435,31 +4442,31 @@
         <v>64</v>
       </c>
       <c r="F73" s="11" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G73" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="H73" s="12" t="s">
         <v>565</v>
       </c>
-      <c r="H73" s="12" t="s">
-        <v>566</v>
-      </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="44"/>
+      <c r="A74" s="40"/>
       <c r="B74" s="7">
         <v>119</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H74" s="12" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -4473,13 +4480,13 @@
         <v>65</v>
       </c>
       <c r="F75" s="11" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H75" s="12" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -4493,13 +4500,13 @@
         <v>66</v>
       </c>
       <c r="F76" s="11" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H76" s="12" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -4513,13 +4520,13 @@
         <v>67</v>
       </c>
       <c r="F77" s="11" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="G77" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="H77" s="12" t="s">
         <v>574</v>
-      </c>
-      <c r="H77" s="12" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -4533,13 +4540,13 @@
         <v>68</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="H78" s="12" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -4553,13 +4560,13 @@
         <v>69</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="H79" s="16" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -4573,13 +4580,13 @@
         <v>70</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="G80" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="H80" s="16" t="s">
         <v>583</v>
-      </c>
-      <c r="H80" s="16" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -4593,13 +4600,13 @@
         <v>71</v>
       </c>
       <c r="F81" s="17" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H81" s="16" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -4613,13 +4620,13 @@
         <v>72</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H82" s="16" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -4633,13 +4640,13 @@
         <v>73</v>
       </c>
       <c r="F83" s="17" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="H83" s="16" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -4653,13 +4660,13 @@
         <v>74</v>
       </c>
       <c r="F84" s="17" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="G84" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="H84" s="16" t="s">
         <v>595</v>
-      </c>
-      <c r="H84" s="16" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -4673,47 +4680,47 @@
         <v>75</v>
       </c>
       <c r="F85" s="17" t="s">
+        <v>592</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="H85" s="16" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="40">
+        <v>74</v>
+      </c>
+      <c r="B86" s="40">
+        <v>148</v>
+      </c>
+      <c r="C86" s="44"/>
+      <c r="D86" s="40"/>
+      <c r="E86" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="F86" s="42" t="s">
         <v>593</v>
       </c>
-      <c r="G85" s="3" t="s">
-        <v>598</v>
-      </c>
-      <c r="H85" s="16" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="44">
-        <v>74</v>
-      </c>
-      <c r="B86" s="44">
-        <v>148</v>
-      </c>
-      <c r="C86" s="39"/>
-      <c r="D86" s="44"/>
-      <c r="E86" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="F86" s="42" t="s">
-        <v>594</v>
-      </c>
       <c r="G86" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H86" s="18" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="44"/>
-      <c r="B87" s="44"/>
-      <c r="C87" s="39"/>
-      <c r="D87" s="44"/>
-      <c r="E87" s="40"/>
+      <c r="A87" s="40"/>
+      <c r="B87" s="40"/>
+      <c r="C87" s="44"/>
+      <c r="D87" s="40"/>
+      <c r="E87" s="43"/>
       <c r="F87" s="42"/>
       <c r="G87" s="41"/>
       <c r="H87" s="18" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -4727,13 +4734,13 @@
         <v>77</v>
       </c>
       <c r="F88" s="19" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G88" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="H88" s="18" t="s">
         <v>604</v>
-      </c>
-      <c r="H88" s="18" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -4747,13 +4754,13 @@
         <v>78</v>
       </c>
       <c r="F89" s="19" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="G89" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="H89" s="18" t="s">
         <v>606</v>
-      </c>
-      <c r="H89" s="18" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -4764,19 +4771,19 @@
         <v>155</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>79</v>
       </c>
       <c r="F90" s="19" t="s">
+        <v>607</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="H90" s="18" t="s">
         <v>608</v>
-      </c>
-      <c r="G90" s="3" t="s">
-        <v>613</v>
-      </c>
-      <c r="H90" s="18" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -4790,13 +4797,13 @@
         <v>80</v>
       </c>
       <c r="F91" s="19" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H91" s="18" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -4810,13 +4817,13 @@
         <v>81</v>
       </c>
       <c r="F92" s="19" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G92" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="H92" s="18" t="s">
         <v>615</v>
-      </c>
-      <c r="H92" s="18" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -4827,19 +4834,19 @@
         <v>169</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E93" s="4" t="s">
         <v>82</v>
       </c>
       <c r="F93" s="19" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="H93" s="18" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -4854,13 +4861,13 @@
         <v>83</v>
       </c>
       <c r="F94" s="19" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G94" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="H94" s="18" t="s">
         <v>623</v>
-      </c>
-      <c r="H94" s="18" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -4875,47 +4882,47 @@
         <v>84</v>
       </c>
       <c r="F95" s="19" t="s">
+        <v>619</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="H95" s="18" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="40">
+        <v>83</v>
+      </c>
+      <c r="B96" s="40">
+        <v>179</v>
+      </c>
+      <c r="C96" s="44"/>
+      <c r="D96" s="40"/>
+      <c r="E96" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="F96" s="42" t="s">
         <v>620</v>
       </c>
-      <c r="G95" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="H95" s="18" t="s">
+      <c r="G96" s="41" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="44">
-        <v>83</v>
-      </c>
-      <c r="B96" s="44">
-        <v>179</v>
-      </c>
-      <c r="C96" s="39"/>
-      <c r="D96" s="44"/>
-      <c r="E96" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="F96" s="42" t="s">
-        <v>621</v>
-      </c>
-      <c r="G96" s="41" t="s">
-        <v>626</v>
-      </c>
       <c r="H96" s="18" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="44"/>
-      <c r="B97" s="44"/>
-      <c r="C97" s="39"/>
-      <c r="D97" s="44"/>
-      <c r="E97" s="40"/>
+      <c r="A97" s="40"/>
+      <c r="B97" s="40"/>
+      <c r="C97" s="44"/>
+      <c r="D97" s="40"/>
+      <c r="E97" s="43"/>
       <c r="F97" s="42"/>
       <c r="G97" s="41"/>
       <c r="H97" s="18" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -4929,13 +4936,13 @@
         <v>86</v>
       </c>
       <c r="F98" s="19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="G98" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="H98" s="18" t="s">
         <v>632</v>
-      </c>
-      <c r="H98" s="18" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -4949,13 +4956,13 @@
         <v>87</v>
       </c>
       <c r="F99" s="19" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H99" s="18" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -4969,13 +4976,13 @@
         <v>88</v>
       </c>
       <c r="F100" s="19" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="H100" s="18" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -4989,13 +4996,13 @@
         <v>89</v>
       </c>
       <c r="F101" s="19" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="H101" s="18" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -5006,16 +5013,16 @@
         <v>200</v>
       </c>
       <c r="E102" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="F102" s="19" t="s">
+        <v>636</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="H102" s="22" t="s">
         <v>701</v>
-      </c>
-      <c r="F102" s="19" t="s">
-        <v>637</v>
-      </c>
-      <c r="G102" s="3" t="s">
-        <v>640</v>
-      </c>
-      <c r="H102" s="22" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -5030,13 +5037,13 @@
         <v>90</v>
       </c>
       <c r="F103" s="19" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="H103" s="18" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -5050,13 +5057,13 @@
         <v>91</v>
       </c>
       <c r="F104" s="19" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H104" s="18" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -5070,13 +5077,13 @@
         <v>92</v>
       </c>
       <c r="F105" s="19" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="H105" s="18" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -5090,13 +5097,13 @@
         <v>93</v>
       </c>
       <c r="F106" s="19" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="H106" s="18" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -5110,13 +5117,13 @@
         <v>94</v>
       </c>
       <c r="F107" s="19" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H107" s="18" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -5130,13 +5137,13 @@
         <v>95</v>
       </c>
       <c r="F108" s="19" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="H108" s="18" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -5150,13 +5157,13 @@
         <v>96</v>
       </c>
       <c r="F109" s="19" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G109" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="H109" s="18" t="s">
         <v>660</v>
-      </c>
-      <c r="H109" s="18" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -5167,23 +5174,23 @@
         <v>226</v>
       </c>
       <c r="C110" s="13" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E110" s="4" t="s">
         <v>97</v>
       </c>
       <c r="F110" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="G110" s="3" t="s">
+        <v>668</v>
+      </c>
+      <c r="H110" s="18" t="s">
         <v>669</v>
       </c>
-      <c r="H110" s="18" t="s">
-        <v>670</v>
-      </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="44">
+      <c r="A111" s="40">
         <v>97</v>
       </c>
       <c r="B111" s="7">
@@ -5191,35 +5198,35 @@
       </c>
       <c r="D111" s="37"/>
       <c r="E111" s="4" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="F111" s="19" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="H111" s="21" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="44"/>
+      <c r="A112" s="40"/>
       <c r="B112" s="7">
         <v>224</v>
       </c>
       <c r="D112" s="37"/>
       <c r="E112" s="4" t="s">
+        <v>673</v>
+      </c>
+      <c r="F112" s="19" t="s">
+        <v>662</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="H112" s="21" t="s">
         <v>674</v>
-      </c>
-      <c r="F112" s="19" t="s">
-        <v>663</v>
-      </c>
-      <c r="G112" s="3" t="s">
-        <v>696</v>
-      </c>
-      <c r="H112" s="21" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -5230,19 +5237,19 @@
         <v>230</v>
       </c>
       <c r="C113" s="13" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E113" s="4" t="s">
         <v>98</v>
       </c>
       <c r="F113" s="19" t="s">
+        <v>665</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="H113" s="18" t="s">
         <v>666</v>
-      </c>
-      <c r="G113" s="3" t="s">
-        <v>668</v>
-      </c>
-      <c r="H113" s="18" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -5253,19 +5260,19 @@
         <v>232</v>
       </c>
       <c r="C114" s="13" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E114" s="4" t="s">
         <v>99</v>
       </c>
       <c r="F114" s="20" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H114" s="21" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -5279,13 +5286,13 @@
         <v>100</v>
       </c>
       <c r="F115" s="6" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H115" s="21" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -5296,19 +5303,19 @@
         <v>235</v>
       </c>
       <c r="C116" s="13" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E116" s="5" t="s">
         <v>101</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="H116" s="21" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -5319,19 +5326,19 @@
         <v>236</v>
       </c>
       <c r="C117" s="13" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E117" s="5" t="s">
         <v>102</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G117" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="H117" s="21" t="s">
         <v>691</v>
-      </c>
-      <c r="H117" s="21" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -5345,13 +5352,13 @@
         <v>103</v>
       </c>
       <c r="F118" s="6" t="s">
+        <v>697</v>
+      </c>
+      <c r="G118" s="3" t="s">
         <v>698</v>
       </c>
-      <c r="G118" s="3" t="s">
+      <c r="H118" s="23" t="s">
         <v>699</v>
-      </c>
-      <c r="H118" s="23" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -5369,7 +5376,7 @@
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="44">
+      <c r="A120" s="40">
         <v>105</v>
       </c>
       <c r="B120" s="7">
@@ -5383,7 +5390,7 @@
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A121" s="44"/>
+      <c r="A121" s="40"/>
       <c r="B121" s="7">
         <v>240</v>
       </c>
@@ -5405,7 +5412,7 @@
         <v>110</v>
       </c>
       <c r="F122" s="6" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -5415,6 +5422,7 @@
       <c r="B123" s="7">
         <v>258</v>
       </c>
+      <c r="D123" s="38"/>
       <c r="E123" s="5" t="s">
         <v>111</v>
       </c>
@@ -5429,6 +5437,7 @@
       <c r="B124" s="7">
         <v>268</v>
       </c>
+      <c r="D124" s="39"/>
       <c r="E124" s="5" t="s">
         <v>113</v>
       </c>
@@ -5545,7 +5554,7 @@
         <v>129</v>
       </c>
       <c r="F132" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -5577,7 +5586,7 @@
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="44">
+      <c r="A135" s="40">
         <v>119</v>
       </c>
       <c r="B135" s="7">
@@ -5591,7 +5600,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="44"/>
+      <c r="A136" s="40"/>
       <c r="B136" s="7">
         <v>337</v>
       </c>
@@ -6078,10 +6087,10 @@
         <v>203</v>
       </c>
       <c r="G170" s="3" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="H170" s="24" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
@@ -6089,7 +6098,7 @@
         <v>154</v>
       </c>
       <c r="C171" s="13" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E171" s="5" t="s">
         <v>204</v>
@@ -6103,7 +6112,7 @@
         <v>155</v>
       </c>
       <c r="C172" s="13" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E172" s="5" t="s">
         <v>206</v>
@@ -6112,10 +6121,10 @@
         <v>207</v>
       </c>
       <c r="G172" s="3" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="H172" s="18" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
@@ -6123,7 +6132,7 @@
         <v>156</v>
       </c>
       <c r="C173" s="13" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E173" s="5" t="s">
         <v>208</v>
@@ -6137,7 +6146,7 @@
         <v>157</v>
       </c>
       <c r="C174" s="13" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E174" s="5" t="s">
         <v>210</v>
@@ -6151,7 +6160,7 @@
         <v>158</v>
       </c>
       <c r="C175" s="13" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E175" s="5" t="s">
         <v>212</v>
@@ -6165,7 +6174,7 @@
         <v>159</v>
       </c>
       <c r="C176" s="13" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E176" s="5" t="s">
         <v>214</v>
@@ -6179,7 +6188,7 @@
         <v>160</v>
       </c>
       <c r="C177" s="13" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E177" s="5" t="s">
         <v>216</v>
@@ -6193,7 +6202,7 @@
         <v>161</v>
       </c>
       <c r="C178" s="13" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E178" s="5" t="s">
         <v>218</v>
@@ -6207,7 +6216,7 @@
         <v>162</v>
       </c>
       <c r="C179" s="13" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E179" s="5" t="s">
         <v>220</v>
@@ -6221,7 +6230,7 @@
         <v>163</v>
       </c>
       <c r="C180" s="13" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E180" s="5" t="s">
         <v>222</v>
@@ -6235,7 +6244,7 @@
         <v>164</v>
       </c>
       <c r="C181" s="13" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E181" s="5" t="s">
         <v>224</v>
@@ -6249,19 +6258,19 @@
         <v>165</v>
       </c>
       <c r="C182" s="13" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E182" s="5" t="s">
         <v>226</v>
       </c>
       <c r="F182" s="6" t="s">
+        <v>670</v>
+      </c>
+      <c r="G182" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="H182" s="18" t="s">
         <v>671</v>
-      </c>
-      <c r="G182" s="3" t="s">
-        <v>595</v>
-      </c>
-      <c r="H182" s="18" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
@@ -6269,7 +6278,7 @@
         <v>166</v>
       </c>
       <c r="C183" s="13" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E183" s="5" t="s">
         <v>227</v>
@@ -6283,7 +6292,7 @@
         <v>167</v>
       </c>
       <c r="C184" s="13" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E184" s="5" t="s">
         <v>229</v>
@@ -6297,7 +6306,7 @@
         <v>168</v>
       </c>
       <c r="C185" s="13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E185" s="5" t="s">
         <v>231</v>
@@ -6311,7 +6320,7 @@
         <v>169</v>
       </c>
       <c r="C186" s="13" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E186" s="5" t="s">
         <v>233</v>
@@ -6325,7 +6334,7 @@
         <v>170</v>
       </c>
       <c r="C187" s="13" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E187" s="5" t="s">
         <v>235</v>
@@ -6339,7 +6348,7 @@
         <v>171</v>
       </c>
       <c r="C188" s="13" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E188" s="5" t="s">
         <v>237</v>
@@ -6353,7 +6362,7 @@
         <v>172</v>
       </c>
       <c r="C189" s="13" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E189" s="5" t="s">
         <v>92</v>
@@ -6367,7 +6376,7 @@
         <v>173</v>
       </c>
       <c r="C190" s="13" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E190" s="5" t="s">
         <v>240</v>
@@ -6381,7 +6390,7 @@
         <v>174</v>
       </c>
       <c r="C191" s="13" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E191" s="5" t="s">
         <v>242</v>
@@ -6395,7 +6404,7 @@
         <v>175</v>
       </c>
       <c r="C192" s="13" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E192" s="5" t="s">
         <v>244</v>
@@ -6409,7 +6418,7 @@
         <v>176</v>
       </c>
       <c r="C193" s="13" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E193" s="5" t="s">
         <v>246</v>
@@ -6423,7 +6432,7 @@
         <v>177</v>
       </c>
       <c r="C194" s="13" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E194" s="5" t="s">
         <v>248</v>
@@ -6437,7 +6446,7 @@
         <v>178</v>
       </c>
       <c r="C195" s="13" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E195" s="5" t="s">
         <v>250</v>
@@ -6451,7 +6460,7 @@
         <v>179</v>
       </c>
       <c r="C196" s="13" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D196" s="32"/>
       <c r="E196" s="5" t="s">
@@ -6466,7 +6475,7 @@
         <v>180</v>
       </c>
       <c r="C197" s="13" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E197" s="5" t="s">
         <v>254</v>
@@ -6480,7 +6489,7 @@
         <v>181</v>
       </c>
       <c r="C198" s="13" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E198" s="5" t="s">
         <v>256</v>
@@ -6494,7 +6503,7 @@
         <v>182</v>
       </c>
       <c r="C199" s="13" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E199" s="5" t="s">
         <v>258</v>
@@ -6508,7 +6517,7 @@
         <v>183</v>
       </c>
       <c r="C200" s="13" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E200" s="5" t="s">
         <v>260</v>
@@ -6522,7 +6531,7 @@
         <v>184</v>
       </c>
       <c r="C201" s="13" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E201" s="5" t="s">
         <v>262</v>
@@ -6536,7 +6545,7 @@
         <v>185</v>
       </c>
       <c r="C202" s="13" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E202" s="5" t="s">
         <v>264</v>
@@ -6550,7 +6559,7 @@
         <v>186</v>
       </c>
       <c r="C203" s="13" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E203" s="5" t="s">
         <v>266</v>
@@ -6564,7 +6573,7 @@
         <v>187</v>
       </c>
       <c r="C204" s="13" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E204" s="5" t="s">
         <v>268</v>
@@ -6578,7 +6587,7 @@
         <v>188</v>
       </c>
       <c r="C205" s="13" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E205" s="5" t="s">
         <v>270</v>
@@ -6592,7 +6601,7 @@
         <v>189</v>
       </c>
       <c r="C206" s="13" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E206" s="5" t="s">
         <v>272</v>
@@ -6606,7 +6615,7 @@
         <v>190</v>
       </c>
       <c r="C207" s="13" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E207" s="5" t="s">
         <v>274</v>
@@ -6620,7 +6629,7 @@
         <v>191</v>
       </c>
       <c r="C208" s="13" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E208" s="5" t="s">
         <v>276</v>
@@ -6634,7 +6643,7 @@
         <v>192</v>
       </c>
       <c r="C209" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E209" s="5" t="s">
         <v>278</v>
@@ -6648,7 +6657,7 @@
         <v>193</v>
       </c>
       <c r="C210" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E210" s="5" t="s">
         <v>280</v>
@@ -6662,7 +6671,7 @@
         <v>194</v>
       </c>
       <c r="C211" s="13" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E211" s="5" t="s">
         <v>282</v>
@@ -6676,7 +6685,7 @@
         <v>195</v>
       </c>
       <c r="C212" s="13" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E212" s="5" t="s">
         <v>284</v>
@@ -6690,7 +6699,7 @@
         <v>196</v>
       </c>
       <c r="C213" s="13" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E213" s="5" t="s">
         <v>286</v>
@@ -6704,7 +6713,7 @@
         <v>197</v>
       </c>
       <c r="C214" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E214" s="5" t="s">
         <v>288</v>
@@ -6718,7 +6727,7 @@
         <v>198</v>
       </c>
       <c r="C215" s="13" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E215" s="5" t="s">
         <v>290</v>
@@ -6732,7 +6741,7 @@
         <v>199</v>
       </c>
       <c r="C216" s="13" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E216" s="5" t="s">
         <v>292</v>
@@ -6746,7 +6755,7 @@
         <v>200</v>
       </c>
       <c r="C217" s="13" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E217" s="5" t="s">
         <v>294</v>
@@ -6755,30 +6764,34 @@
         <v>295</v>
       </c>
       <c r="G217" s="3" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="H217" s="18" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>201</v>
       </c>
+      <c r="B218" s="7">
+        <v>264</v>
+      </c>
       <c r="C218" s="13" t="s">
-        <v>544</v>
-      </c>
+        <v>543</v>
+      </c>
+      <c r="D218" s="39"/>
       <c r="E218" s="5" t="s">
-        <v>296</v>
+        <v>711</v>
       </c>
       <c r="F218" s="6" t="s">
+        <v>692</v>
+      </c>
+      <c r="G218" s="3" t="s">
         <v>693</v>
       </c>
-      <c r="G218" s="3" t="s">
+      <c r="H218" s="23" t="s">
         <v>694</v>
-      </c>
-      <c r="H218" s="23" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
@@ -6786,13 +6799,13 @@
         <v>202</v>
       </c>
       <c r="C219" s="13" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E219" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="F219" s="8" t="s">
         <v>297</v>
-      </c>
-      <c r="F219" s="8" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
@@ -6800,13 +6813,13 @@
         <v>203</v>
       </c>
       <c r="C220" s="13" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E220" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="F220" s="8" t="s">
         <v>299</v>
-      </c>
-      <c r="F220" s="8" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
@@ -6814,13 +6827,13 @@
         <v>204</v>
       </c>
       <c r="C221" s="13" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E221" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="F221" s="8" t="s">
         <v>301</v>
-      </c>
-      <c r="F221" s="8" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
@@ -6828,13 +6841,13 @@
         <v>205</v>
       </c>
       <c r="C222" s="13" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E222" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="F222" s="8" t="s">
         <v>303</v>
-      </c>
-      <c r="F222" s="8" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
@@ -6842,13 +6855,13 @@
         <v>206</v>
       </c>
       <c r="C223" s="13" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E223" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="F223" s="8" t="s">
         <v>305</v>
-      </c>
-      <c r="F223" s="8" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
@@ -6856,13 +6869,13 @@
         <v>207</v>
       </c>
       <c r="C224" s="13" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E224" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="F224" s="8" t="s">
         <v>307</v>
-      </c>
-      <c r="F224" s="8" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
@@ -6870,49 +6883,18 @@
         <v>208</v>
       </c>
       <c r="C225" s="13" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E225" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="F225" s="8" t="s">
         <v>309</v>
-      </c>
-      <c r="F225" s="8" t="s">
-        <v>310</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I225" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="44">
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="G86:G87"/>
-    <mergeCell ref="G96:G97"/>
-    <mergeCell ref="F96:F97"/>
-    <mergeCell ref="E96:E97"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="E86:E87"/>
-    <mergeCell ref="F86:F87"/>
-    <mergeCell ref="D86:D87"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="B63:B64"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="E56:E57"/>
@@ -6926,6 +6908,37 @@
     <mergeCell ref="F56:F57"/>
     <mergeCell ref="C53:C54"/>
     <mergeCell ref="D53:D54"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="G86:G87"/>
+    <mergeCell ref="G96:G97"/>
+    <mergeCell ref="F96:F97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="D96:D97"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B56:B57"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
+ Add several problems
</commit_message>
<xml_diff>
--- a/面试高频题.xlsx
+++ b/面试高频题.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30930F5-B3C4-40ED-9457-C96E51B2B9F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EA2F8B-2749-40E0-9C57-1A88EF0F194E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$225</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$226</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
@@ -2530,7 +2530,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2656,8 +2656,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2665,16 +2674,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3024,8 +3027,8 @@
   <dimension ref="A1:I226"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D226" sqref="D226"/>
+      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E205" sqref="E205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -3034,7 +3037,7 @@
     <col min="2" max="2" width="7.08984375" style="7" customWidth="1"/>
     <col min="3" max="3" width="7.26953125" style="13" customWidth="1"/>
     <col min="4" max="4" width="7.6328125" style="25" customWidth="1"/>
-    <col min="5" max="5" width="27.08984375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="34.453125" style="5" customWidth="1"/>
     <col min="6" max="6" width="34" style="10" customWidth="1"/>
     <col min="7" max="7" width="31.90625" style="3" customWidth="1"/>
     <col min="8" max="8" width="21.90625" style="3" customWidth="1"/>
@@ -3601,21 +3604,21 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="43">
+      <c r="A28" s="50">
         <v>26</v>
       </c>
-      <c r="B28" s="43">
+      <c r="B28" s="50">
         <v>46</v>
       </c>
-      <c r="C28" s="47"/>
-      <c r="D28" s="48"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="44"/>
       <c r="E28" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="F28" s="45" t="s">
+      <c r="F28" s="48" t="s">
         <v>388</v>
       </c>
-      <c r="G28" s="44" t="s">
+      <c r="G28" s="47" t="s">
         <v>389</v>
       </c>
       <c r="H28" s="29" t="s">
@@ -3623,19 +3626,19 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="43"/>
-      <c r="B29" s="43"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="48"/>
+      <c r="A29" s="50"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="44"/>
       <c r="E29" s="46"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="44"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="47"/>
       <c r="H29" s="29" t="s">
         <v>708</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="43"/>
+      <c r="A30" s="50"/>
       <c r="B30" s="7">
         <v>47</v>
       </c>
@@ -3811,7 +3814,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="43">
+      <c r="A39" s="50">
         <v>35</v>
       </c>
       <c r="B39" s="7">
@@ -3831,7 +3834,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="43"/>
+      <c r="A40" s="50"/>
       <c r="B40" s="7">
         <v>63</v>
       </c>
@@ -3991,7 +3994,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="43">
+      <c r="A48" s="50">
         <v>43</v>
       </c>
       <c r="B48" s="7">
@@ -4007,7 +4010,7 @@
       <c r="H48" s="10"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="43"/>
+      <c r="A49" s="50"/>
       <c r="B49" s="7">
         <v>83</v>
       </c>
@@ -4025,7 +4028,7 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="43">
+      <c r="A50" s="50">
         <v>44</v>
       </c>
       <c r="B50" s="7">
@@ -4045,7 +4048,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="43"/>
+      <c r="A51" s="50"/>
       <c r="B51" s="7">
         <v>725</v>
       </c>
@@ -4083,21 +4086,21 @@
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="43">
+      <c r="A53" s="50">
         <v>46</v>
       </c>
-      <c r="B53" s="43">
+      <c r="B53" s="50">
         <v>90</v>
       </c>
-      <c r="C53" s="47"/>
+      <c r="C53" s="45"/>
       <c r="D53" s="49"/>
       <c r="E53" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="F53" s="45" t="s">
+      <c r="F53" s="48" t="s">
         <v>446</v>
       </c>
-      <c r="G53" s="44" t="s">
+      <c r="G53" s="47" t="s">
         <v>449</v>
       </c>
       <c r="H53" s="10" t="s">
@@ -4105,13 +4108,13 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="43"/>
-      <c r="B54" s="43"/>
-      <c r="C54" s="47"/>
+      <c r="A54" s="50"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="45"/>
       <c r="D54" s="49"/>
       <c r="E54" s="46"/>
-      <c r="F54" s="45"/>
-      <c r="G54" s="44"/>
+      <c r="F54" s="48"/>
+      <c r="G54" s="47"/>
       <c r="H54" s="10" t="s">
         <v>450</v>
       </c>
@@ -4138,16 +4141,16 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
-      <c r="B56" s="43">
+      <c r="B56" s="50">
         <v>92</v>
       </c>
       <c r="E56" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="F56" s="45" t="s">
+      <c r="F56" s="48" t="s">
         <v>448</v>
       </c>
-      <c r="G56" s="44" t="s">
+      <c r="G56" s="47" t="s">
         <v>454</v>
       </c>
       <c r="H56" s="10" t="s">
@@ -4158,10 +4161,10 @@
       <c r="A57" s="2">
         <v>48</v>
       </c>
-      <c r="B57" s="43"/>
+      <c r="B57" s="50"/>
       <c r="E57" s="46"/>
-      <c r="F57" s="45"/>
-      <c r="G57" s="44"/>
+      <c r="F57" s="48"/>
+      <c r="G57" s="47"/>
       <c r="H57" s="10" t="s">
         <v>455</v>
       </c>
@@ -4269,19 +4272,19 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="43">
+      <c r="A63" s="50">
         <v>54</v>
       </c>
-      <c r="B63" s="43">
+      <c r="B63" s="50">
         <v>102</v>
       </c>
       <c r="E63" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="F63" s="45" t="s">
+      <c r="F63" s="48" t="s">
         <v>468</v>
       </c>
-      <c r="G63" s="44" t="s">
+      <c r="G63" s="47" t="s">
         <v>474</v>
       </c>
       <c r="H63" s="9" t="s">
@@ -4289,11 +4292,11 @@
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="43"/>
-      <c r="B64" s="43"/>
+      <c r="A64" s="50"/>
+      <c r="B64" s="50"/>
       <c r="E64" s="46"/>
-      <c r="F64" s="45"/>
-      <c r="G64" s="44"/>
+      <c r="F64" s="48"/>
+      <c r="G64" s="47"/>
       <c r="H64" s="10" t="s">
         <v>473</v>
       </c>
@@ -4459,7 +4462,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="43">
+      <c r="A73" s="50">
         <v>62</v>
       </c>
       <c r="B73" s="7">
@@ -4479,7 +4482,7 @@
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="43"/>
+      <c r="A74" s="50"/>
       <c r="B74" s="7">
         <v>119</v>
       </c>
@@ -4717,21 +4720,21 @@
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="43">
+      <c r="A86" s="50">
         <v>74</v>
       </c>
-      <c r="B86" s="43">
+      <c r="B86" s="50">
         <v>148</v>
       </c>
-      <c r="C86" s="47"/>
-      <c r="D86" s="43"/>
+      <c r="C86" s="45"/>
+      <c r="D86" s="50"/>
       <c r="E86" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="F86" s="45" t="s">
+      <c r="F86" s="48" t="s">
         <v>592</v>
       </c>
-      <c r="G86" s="44" t="s">
+      <c r="G86" s="47" t="s">
         <v>599</v>
       </c>
       <c r="H86" s="18" t="s">
@@ -4739,13 +4742,13 @@
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="43"/>
-      <c r="B87" s="43"/>
-      <c r="C87" s="47"/>
-      <c r="D87" s="43"/>
+      <c r="A87" s="50"/>
+      <c r="B87" s="50"/>
+      <c r="C87" s="45"/>
+      <c r="D87" s="50"/>
       <c r="E87" s="46"/>
-      <c r="F87" s="45"/>
-      <c r="G87" s="44"/>
+      <c r="F87" s="48"/>
+      <c r="G87" s="47"/>
       <c r="H87" s="18" t="s">
         <v>600</v>
       </c>
@@ -4919,21 +4922,21 @@
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="43">
+      <c r="A96" s="50">
         <v>83</v>
       </c>
-      <c r="B96" s="43">
+      <c r="B96" s="50">
         <v>179</v>
       </c>
-      <c r="C96" s="47"/>
-      <c r="D96" s="43"/>
+      <c r="C96" s="45"/>
+      <c r="D96" s="50"/>
       <c r="E96" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="F96" s="45" t="s">
+      <c r="F96" s="48" t="s">
         <v>619</v>
       </c>
-      <c r="G96" s="44" t="s">
+      <c r="G96" s="47" t="s">
         <v>624</v>
       </c>
       <c r="H96" s="18" t="s">
@@ -4941,13 +4944,13 @@
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="43"/>
-      <c r="B97" s="43"/>
-      <c r="C97" s="47"/>
-      <c r="D97" s="43"/>
+      <c r="A97" s="50"/>
+      <c r="B97" s="50"/>
+      <c r="C97" s="45"/>
+      <c r="D97" s="50"/>
       <c r="E97" s="46"/>
-      <c r="F97" s="45"/>
-      <c r="G97" s="44"/>
+      <c r="F97" s="48"/>
+      <c r="G97" s="47"/>
       <c r="H97" s="18" t="s">
         <v>625</v>
       </c>
@@ -5217,7 +5220,7 @@
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="43">
+      <c r="A111" s="50">
         <v>97</v>
       </c>
       <c r="B111" s="7">
@@ -5238,7 +5241,7 @@
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="43"/>
+      <c r="A112" s="50"/>
       <c r="B112" s="7">
         <v>224</v>
       </c>
@@ -5403,7 +5406,7 @@
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="43">
+      <c r="A120" s="50">
         <v>105</v>
       </c>
       <c r="B120" s="7">
@@ -5417,7 +5420,7 @@
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A121" s="43"/>
+      <c r="A121" s="50"/>
       <c r="B121" s="7">
         <v>240</v>
       </c>
@@ -5615,7 +5618,7 @@
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="43">
+      <c r="A135" s="50">
         <v>119</v>
       </c>
       <c r="B135" s="7">
@@ -5629,7 +5632,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="43"/>
+      <c r="A136" s="50"/>
       <c r="B136" s="7">
         <v>337</v>
       </c>
@@ -6475,9 +6478,13 @@
       <c r="A195" s="2">
         <v>178</v>
       </c>
+      <c r="B195" s="7">
+        <v>946</v>
+      </c>
       <c r="C195" s="13" t="s">
         <v>519</v>
       </c>
+      <c r="D195" s="43"/>
       <c r="E195" s="5" t="s">
         <v>250</v>
       </c>
@@ -6935,8 +6942,39 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I225" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I226" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="44">
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="G86:G87"/>
+    <mergeCell ref="G96:G97"/>
+    <mergeCell ref="F96:F97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="D96:D97"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:B64"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="E56:E57"/>
@@ -6950,37 +6988,6 @@
     <mergeCell ref="F56:F57"/>
     <mergeCell ref="C53:C54"/>
     <mergeCell ref="D53:D54"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="G86:G87"/>
-    <mergeCell ref="G96:G97"/>
-    <mergeCell ref="F96:F97"/>
-    <mergeCell ref="E96:E97"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="E86:E87"/>
-    <mergeCell ref="F86:F87"/>
-    <mergeCell ref="D86:D87"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B56:B57"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
+ Add two hard problems
</commit_message>
<xml_diff>
--- a/面试高频题.xlsx
+++ b/面试高频题.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EA2F8B-2749-40E0-9C57-1A88EF0F194E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EC10DE-1A15-4F1F-B0C9-D45C723816BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2530,7 +2530,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2659,14 +2659,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2674,10 +2671,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3027,8 +3030,8 @@
   <dimension ref="A1:I226"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E205" sqref="E205"/>
+      <pane ySplit="1" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E201" sqref="E201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -3604,21 +3607,21 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="50">
+      <c r="A28" s="45">
         <v>26</v>
       </c>
-      <c r="B28" s="50">
+      <c r="B28" s="45">
         <v>46</v>
       </c>
-      <c r="C28" s="45"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="46" t="s">
+      <c r="C28" s="49"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="F28" s="48" t="s">
+      <c r="F28" s="47" t="s">
         <v>388</v>
       </c>
-      <c r="G28" s="47" t="s">
+      <c r="G28" s="46" t="s">
         <v>389</v>
       </c>
       <c r="H28" s="29" t="s">
@@ -3626,19 +3629,19 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="47"/>
+      <c r="A29" s="45"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="46"/>
       <c r="H29" s="29" t="s">
         <v>708</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="50"/>
+      <c r="A30" s="45"/>
       <c r="B30" s="7">
         <v>47</v>
       </c>
@@ -3814,7 +3817,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="50">
+      <c r="A39" s="45">
         <v>35</v>
       </c>
       <c r="B39" s="7">
@@ -3834,7 +3837,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="50"/>
+      <c r="A40" s="45"/>
       <c r="B40" s="7">
         <v>63</v>
       </c>
@@ -3994,7 +3997,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="50">
+      <c r="A48" s="45">
         <v>43</v>
       </c>
       <c r="B48" s="7">
@@ -4010,7 +4013,7 @@
       <c r="H48" s="10"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="50"/>
+      <c r="A49" s="45"/>
       <c r="B49" s="7">
         <v>83</v>
       </c>
@@ -4028,7 +4031,7 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="50">
+      <c r="A50" s="45">
         <v>44</v>
       </c>
       <c r="B50" s="7">
@@ -4048,7 +4051,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="50"/>
+      <c r="A51" s="45"/>
       <c r="B51" s="7">
         <v>725</v>
       </c>
@@ -4086,21 +4089,21 @@
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="50">
+      <c r="A53" s="45">
         <v>46</v>
       </c>
-      <c r="B53" s="50">
+      <c r="B53" s="45">
         <v>90</v>
       </c>
-      <c r="C53" s="45"/>
-      <c r="D53" s="49"/>
-      <c r="E53" s="46" t="s">
+      <c r="C53" s="49"/>
+      <c r="D53" s="51"/>
+      <c r="E53" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="F53" s="48" t="s">
+      <c r="F53" s="47" t="s">
         <v>446</v>
       </c>
-      <c r="G53" s="47" t="s">
+      <c r="G53" s="46" t="s">
         <v>449</v>
       </c>
       <c r="H53" s="10" t="s">
@@ -4108,13 +4111,13 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="50"/>
-      <c r="B54" s="50"/>
-      <c r="C54" s="45"/>
-      <c r="D54" s="49"/>
-      <c r="E54" s="46"/>
-      <c r="F54" s="48"/>
-      <c r="G54" s="47"/>
+      <c r="A54" s="45"/>
+      <c r="B54" s="45"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="51"/>
+      <c r="E54" s="48"/>
+      <c r="F54" s="47"/>
+      <c r="G54" s="46"/>
       <c r="H54" s="10" t="s">
         <v>450</v>
       </c>
@@ -4141,16 +4144,16 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
-      <c r="B56" s="50">
+      <c r="B56" s="45">
         <v>92</v>
       </c>
-      <c r="E56" s="46" t="s">
+      <c r="E56" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="F56" s="48" t="s">
+      <c r="F56" s="47" t="s">
         <v>448</v>
       </c>
-      <c r="G56" s="47" t="s">
+      <c r="G56" s="46" t="s">
         <v>454</v>
       </c>
       <c r="H56" s="10" t="s">
@@ -4161,10 +4164,10 @@
       <c r="A57" s="2">
         <v>48</v>
       </c>
-      <c r="B57" s="50"/>
-      <c r="E57" s="46"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="47"/>
+      <c r="B57" s="45"/>
+      <c r="E57" s="48"/>
+      <c r="F57" s="47"/>
+      <c r="G57" s="46"/>
       <c r="H57" s="10" t="s">
         <v>455</v>
       </c>
@@ -4272,19 +4275,19 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="50">
+      <c r="A63" s="45">
         <v>54</v>
       </c>
-      <c r="B63" s="50">
+      <c r="B63" s="45">
         <v>102</v>
       </c>
-      <c r="E63" s="46" t="s">
+      <c r="E63" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="F63" s="48" t="s">
+      <c r="F63" s="47" t="s">
         <v>468</v>
       </c>
-      <c r="G63" s="47" t="s">
+      <c r="G63" s="46" t="s">
         <v>474</v>
       </c>
       <c r="H63" s="9" t="s">
@@ -4292,11 +4295,11 @@
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="50"/>
-      <c r="B64" s="50"/>
-      <c r="E64" s="46"/>
-      <c r="F64" s="48"/>
-      <c r="G64" s="47"/>
+      <c r="A64" s="45"/>
+      <c r="B64" s="45"/>
+      <c r="E64" s="48"/>
+      <c r="F64" s="47"/>
+      <c r="G64" s="46"/>
       <c r="H64" s="10" t="s">
         <v>473</v>
       </c>
@@ -4462,7 +4465,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="50">
+      <c r="A73" s="45">
         <v>62</v>
       </c>
       <c r="B73" s="7">
@@ -4482,7 +4485,7 @@
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="50"/>
+      <c r="A74" s="45"/>
       <c r="B74" s="7">
         <v>119</v>
       </c>
@@ -4720,21 +4723,21 @@
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="50">
+      <c r="A86" s="45">
         <v>74</v>
       </c>
-      <c r="B86" s="50">
+      <c r="B86" s="45">
         <v>148</v>
       </c>
-      <c r="C86" s="45"/>
-      <c r="D86" s="50"/>
-      <c r="E86" s="46" t="s">
+      <c r="C86" s="49"/>
+      <c r="D86" s="45"/>
+      <c r="E86" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="F86" s="48" t="s">
+      <c r="F86" s="47" t="s">
         <v>592</v>
       </c>
-      <c r="G86" s="47" t="s">
+      <c r="G86" s="46" t="s">
         <v>599</v>
       </c>
       <c r="H86" s="18" t="s">
@@ -4742,13 +4745,13 @@
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="50"/>
-      <c r="B87" s="50"/>
-      <c r="C87" s="45"/>
-      <c r="D87" s="50"/>
-      <c r="E87" s="46"/>
-      <c r="F87" s="48"/>
-      <c r="G87" s="47"/>
+      <c r="A87" s="45"/>
+      <c r="B87" s="45"/>
+      <c r="C87" s="49"/>
+      <c r="D87" s="45"/>
+      <c r="E87" s="48"/>
+      <c r="F87" s="47"/>
+      <c r="G87" s="46"/>
       <c r="H87" s="18" t="s">
         <v>600</v>
       </c>
@@ -4922,21 +4925,21 @@
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="50">
+      <c r="A96" s="45">
         <v>83</v>
       </c>
-      <c r="B96" s="50">
+      <c r="B96" s="45">
         <v>179</v>
       </c>
-      <c r="C96" s="45"/>
-      <c r="D96" s="50"/>
-      <c r="E96" s="46" t="s">
+      <c r="C96" s="49"/>
+      <c r="D96" s="45"/>
+      <c r="E96" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="F96" s="48" t="s">
+      <c r="F96" s="47" t="s">
         <v>619</v>
       </c>
-      <c r="G96" s="47" t="s">
+      <c r="G96" s="46" t="s">
         <v>624</v>
       </c>
       <c r="H96" s="18" t="s">
@@ -4944,13 +4947,13 @@
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="50"/>
-      <c r="B97" s="50"/>
-      <c r="C97" s="45"/>
-      <c r="D97" s="50"/>
-      <c r="E97" s="46"/>
-      <c r="F97" s="48"/>
-      <c r="G97" s="47"/>
+      <c r="A97" s="45"/>
+      <c r="B97" s="45"/>
+      <c r="C97" s="49"/>
+      <c r="D97" s="45"/>
+      <c r="E97" s="48"/>
+      <c r="F97" s="47"/>
+      <c r="G97" s="46"/>
       <c r="H97" s="18" t="s">
         <v>625</v>
       </c>
@@ -5220,7 +5223,7 @@
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="50">
+      <c r="A111" s="45">
         <v>97</v>
       </c>
       <c r="B111" s="7">
@@ -5241,7 +5244,7 @@
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="50"/>
+      <c r="A112" s="45"/>
       <c r="B112" s="7">
         <v>224</v>
       </c>
@@ -5406,7 +5409,7 @@
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="50">
+      <c r="A120" s="45">
         <v>105</v>
       </c>
       <c r="B120" s="7">
@@ -5420,7 +5423,7 @@
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A121" s="50"/>
+      <c r="A121" s="45"/>
       <c r="B121" s="7">
         <v>240</v>
       </c>
@@ -5618,7 +5621,7 @@
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="50">
+      <c r="A135" s="45">
         <v>119</v>
       </c>
       <c r="B135" s="7">
@@ -5632,7 +5635,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="50"/>
+      <c r="A136" s="45"/>
       <c r="B136" s="7">
         <v>337</v>
       </c>
@@ -6570,6 +6573,7 @@
       <c r="C201" s="13" t="s">
         <v>525</v>
       </c>
+      <c r="D201" s="44"/>
       <c r="E201" s="5" t="s">
         <v>261</v>
       </c>
@@ -6944,37 +6948,6 @@
   </sheetData>
   <autoFilter ref="A1:I226" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="44">
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="G86:G87"/>
-    <mergeCell ref="G96:G97"/>
-    <mergeCell ref="F96:F97"/>
-    <mergeCell ref="E96:E97"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="E86:E87"/>
-    <mergeCell ref="F86:F87"/>
-    <mergeCell ref="D86:D87"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="B63:B64"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="E56:E57"/>
@@ -6988,6 +6961,37 @@
     <mergeCell ref="F56:F57"/>
     <mergeCell ref="C53:C54"/>
     <mergeCell ref="D53:D54"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="G86:G87"/>
+    <mergeCell ref="G96:G97"/>
+    <mergeCell ref="F96:F97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="D96:D97"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B56:B57"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
+ Add some cpp implementations
</commit_message>
<xml_diff>
--- a/面试高频题.xlsx
+++ b/面试高频题.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE8BB02-4971-4E44-8837-ED6B01292A11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9E41A5-7893-45BA-AED2-DC51CFF1F0E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2520,7 +2520,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2530,6 +2530,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF4FF329"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2547,7 +2553,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2697,14 +2703,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2712,10 +2715,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3065,8 +3077,8 @@
   <dimension ref="A1:I228"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E210" sqref="E210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -3642,21 +3654,21 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="57">
+      <c r="A28" s="52">
         <v>26</v>
       </c>
-      <c r="B28" s="57">
+      <c r="B28" s="52">
         <v>46</v>
       </c>
-      <c r="C28" s="52"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="53" t="s">
+      <c r="C28" s="56"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="F28" s="55" t="s">
+      <c r="F28" s="54" t="s">
         <v>387</v>
       </c>
-      <c r="G28" s="54" t="s">
+      <c r="G28" s="53" t="s">
         <v>388</v>
       </c>
       <c r="H28" s="29" t="s">
@@ -3664,19 +3676,19 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="57"/>
-      <c r="B29" s="57"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="54"/>
+      <c r="A29" s="52"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="54"/>
+      <c r="G29" s="53"/>
       <c r="H29" s="29" t="s">
         <v>706</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="57"/>
+      <c r="A30" s="52"/>
       <c r="B30" s="7">
         <v>47</v>
       </c>
@@ -3852,7 +3864,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="57">
+      <c r="A39" s="52">
         <v>35</v>
       </c>
       <c r="B39" s="7">
@@ -3872,7 +3884,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="57"/>
+      <c r="A40" s="52"/>
       <c r="B40" s="7">
         <v>63</v>
       </c>
@@ -4032,7 +4044,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="57">
+      <c r="A48" s="52">
         <v>43</v>
       </c>
       <c r="B48" s="7">
@@ -4048,7 +4060,7 @@
       <c r="H48" s="10"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="57"/>
+      <c r="A49" s="52"/>
       <c r="B49" s="7">
         <v>83</v>
       </c>
@@ -4066,7 +4078,7 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="57">
+      <c r="A50" s="52">
         <v>44</v>
       </c>
       <c r="B50" s="7">
@@ -4086,7 +4098,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="57"/>
+      <c r="A51" s="52"/>
       <c r="B51" s="7">
         <v>725</v>
       </c>
@@ -4124,21 +4136,21 @@
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="57">
+      <c r="A53" s="52">
         <v>46</v>
       </c>
-      <c r="B53" s="57">
+      <c r="B53" s="52">
         <v>90</v>
       </c>
-      <c r="C53" s="52"/>
-      <c r="D53" s="56"/>
-      <c r="E53" s="53" t="s">
+      <c r="C53" s="56"/>
+      <c r="D53" s="58"/>
+      <c r="E53" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="F53" s="55" t="s">
+      <c r="F53" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="G53" s="54" t="s">
+      <c r="G53" s="53" t="s">
         <v>448</v>
       </c>
       <c r="H53" s="10" t="s">
@@ -4146,13 +4158,13 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="57"/>
-      <c r="B54" s="57"/>
-      <c r="C54" s="52"/>
-      <c r="D54" s="56"/>
-      <c r="E54" s="53"/>
-      <c r="F54" s="55"/>
-      <c r="G54" s="54"/>
+      <c r="A54" s="52"/>
+      <c r="B54" s="52"/>
+      <c r="C54" s="56"/>
+      <c r="D54" s="58"/>
+      <c r="E54" s="55"/>
+      <c r="F54" s="54"/>
+      <c r="G54" s="53"/>
       <c r="H54" s="10" t="s">
         <v>449</v>
       </c>
@@ -4179,16 +4191,16 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
-      <c r="B56" s="57">
+      <c r="B56" s="52">
         <v>92</v>
       </c>
-      <c r="E56" s="53" t="s">
+      <c r="E56" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="F56" s="55" t="s">
+      <c r="F56" s="54" t="s">
         <v>447</v>
       </c>
-      <c r="G56" s="54" t="s">
+      <c r="G56" s="53" t="s">
         <v>453</v>
       </c>
       <c r="H56" s="10" t="s">
@@ -4199,10 +4211,10 @@
       <c r="A57" s="2">
         <v>48</v>
       </c>
-      <c r="B57" s="57"/>
-      <c r="E57" s="53"/>
-      <c r="F57" s="55"/>
-      <c r="G57" s="54"/>
+      <c r="B57" s="52"/>
+      <c r="E57" s="55"/>
+      <c r="F57" s="54"/>
+      <c r="G57" s="53"/>
       <c r="H57" s="10" t="s">
         <v>454</v>
       </c>
@@ -4310,19 +4322,19 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="57">
+      <c r="A63" s="52">
         <v>54</v>
       </c>
-      <c r="B63" s="57">
+      <c r="B63" s="52">
         <v>102</v>
       </c>
-      <c r="E63" s="53" t="s">
+      <c r="E63" s="55" t="s">
         <v>713</v>
       </c>
-      <c r="F63" s="55" t="s">
+      <c r="F63" s="54" t="s">
         <v>467</v>
       </c>
-      <c r="G63" s="54" t="s">
+      <c r="G63" s="53" t="s">
         <v>473</v>
       </c>
       <c r="H63" s="9" t="s">
@@ -4330,11 +4342,11 @@
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="57"/>
-      <c r="B64" s="57"/>
-      <c r="E64" s="53"/>
-      <c r="F64" s="55"/>
-      <c r="G64" s="54"/>
+      <c r="A64" s="52"/>
+      <c r="B64" s="52"/>
+      <c r="E64" s="55"/>
+      <c r="F64" s="54"/>
+      <c r="G64" s="53"/>
       <c r="H64" s="10" t="s">
         <v>472</v>
       </c>
@@ -4500,7 +4512,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="57">
+      <c r="A73" s="52">
         <v>62</v>
       </c>
       <c r="B73" s="7">
@@ -4520,7 +4532,7 @@
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="57"/>
+      <c r="A74" s="52"/>
       <c r="B74" s="7">
         <v>119</v>
       </c>
@@ -4760,21 +4772,21 @@
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="57">
+      <c r="A86" s="52">
         <v>74</v>
       </c>
-      <c r="B86" s="57">
+      <c r="B86" s="52">
         <v>148</v>
       </c>
-      <c r="C86" s="52"/>
-      <c r="D86" s="57"/>
-      <c r="E86" s="53" t="s">
+      <c r="C86" s="56"/>
+      <c r="D86" s="52"/>
+      <c r="E86" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="F86" s="55" t="s">
+      <c r="F86" s="54" t="s">
         <v>590</v>
       </c>
-      <c r="G86" s="54" t="s">
+      <c r="G86" s="53" t="s">
         <v>597</v>
       </c>
       <c r="H86" s="18" t="s">
@@ -4782,13 +4794,13 @@
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="57"/>
-      <c r="B87" s="57"/>
-      <c r="C87" s="52"/>
-      <c r="D87" s="57"/>
-      <c r="E87" s="53"/>
-      <c r="F87" s="55"/>
-      <c r="G87" s="54"/>
+      <c r="A87" s="52"/>
+      <c r="B87" s="52"/>
+      <c r="C87" s="56"/>
+      <c r="D87" s="52"/>
+      <c r="E87" s="55"/>
+      <c r="F87" s="54"/>
+      <c r="G87" s="53"/>
       <c r="H87" s="18" t="s">
         <v>598</v>
       </c>
@@ -4962,21 +4974,21 @@
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="57">
+      <c r="A96" s="52">
         <v>83</v>
       </c>
-      <c r="B96" s="57">
+      <c r="B96" s="52">
         <v>179</v>
       </c>
-      <c r="C96" s="52"/>
-      <c r="D96" s="57"/>
-      <c r="E96" s="53" t="s">
+      <c r="C96" s="56"/>
+      <c r="D96" s="52"/>
+      <c r="E96" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="F96" s="55" t="s">
+      <c r="F96" s="54" t="s">
         <v>617</v>
       </c>
-      <c r="G96" s="54" t="s">
+      <c r="G96" s="53" t="s">
         <v>622</v>
       </c>
       <c r="H96" s="18" t="s">
@@ -4984,13 +4996,13 @@
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="57"/>
-      <c r="B97" s="57"/>
-      <c r="C97" s="52"/>
-      <c r="D97" s="57"/>
-      <c r="E97" s="53"/>
-      <c r="F97" s="55"/>
-      <c r="G97" s="54"/>
+      <c r="A97" s="52"/>
+      <c r="B97" s="52"/>
+      <c r="C97" s="56"/>
+      <c r="D97" s="52"/>
+      <c r="E97" s="55"/>
+      <c r="F97" s="54"/>
+      <c r="G97" s="53"/>
       <c r="H97" s="18" t="s">
         <v>623</v>
       </c>
@@ -5260,7 +5272,7 @@
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="57">
+      <c r="A111" s="52">
         <v>97</v>
       </c>
       <c r="B111" s="7">
@@ -5281,7 +5293,7 @@
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="57"/>
+      <c r="A112" s="52"/>
       <c r="B112" s="7">
         <v>224</v>
       </c>
@@ -5446,7 +5458,7 @@
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="57">
+      <c r="A120" s="52">
         <v>105</v>
       </c>
       <c r="B120" s="7">
@@ -5460,7 +5472,7 @@
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A121" s="57"/>
+      <c r="A121" s="52"/>
       <c r="B121" s="7">
         <v>240</v>
       </c>
@@ -5658,7 +5670,7 @@
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="57">
+      <c r="A135" s="52">
         <v>119</v>
       </c>
       <c r="B135" s="7">
@@ -5672,7 +5684,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="57"/>
+      <c r="A136" s="52"/>
       <c r="B136" s="7">
         <v>337</v>
       </c>
@@ -6776,6 +6788,7 @@
       <c r="C212" s="13" t="s">
         <v>534</v>
       </c>
+      <c r="D212" s="51"/>
       <c r="E212" s="5" t="s">
         <v>282</v>
       </c>
@@ -6804,6 +6817,7 @@
       <c r="C214" s="13" t="s">
         <v>536</v>
       </c>
+      <c r="D214" s="59"/>
       <c r="E214" s="5" t="s">
         <v>286</v>
       </c>
@@ -7017,37 +7031,6 @@
   </sheetData>
   <autoFilter ref="A1:I228" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="44">
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="G86:G87"/>
-    <mergeCell ref="G96:G97"/>
-    <mergeCell ref="F96:F97"/>
-    <mergeCell ref="E96:E97"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="E86:E87"/>
-    <mergeCell ref="F86:F87"/>
-    <mergeCell ref="D86:D87"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="B63:B64"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="E56:E57"/>
@@ -7061,6 +7044,37 @@
     <mergeCell ref="F56:F57"/>
     <mergeCell ref="C53:C54"/>
     <mergeCell ref="D53:D54"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="G86:G87"/>
+    <mergeCell ref="G96:G97"/>
+    <mergeCell ref="F96:F97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="D96:D97"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B56:B57"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
+ Add two jz problem
</commit_message>
<xml_diff>
--- a/面试高频题.xlsx
+++ b/面试高频题.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E05E380-1A39-4B2E-A7F2-FA8523A69196}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E01D56-AD4B-4836-8439-88B8AD21BC3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="723">
   <si>
     <t>两数之和</t>
   </si>
@@ -2482,6 +2482,14 @@
   </si>
   <si>
     <t>n个骰子的点数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>62</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>圆圈中最后剩下的数字</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2555,7 +2563,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2714,8 +2722,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2723,16 +2740,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3079,27 +3090,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I229"/>
+  <dimension ref="A1:I230"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E230" sqref="E230"/>
+      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D221" sqref="D221"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="7.25" style="13" customWidth="1"/>
-    <col min="4" max="4" width="7.625" style="25" customWidth="1"/>
-    <col min="5" max="5" width="34.5" style="5" customWidth="1"/>
+    <col min="1" max="1" width="6.36328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.08984375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="7.26953125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="7.6328125" style="25" customWidth="1"/>
+    <col min="5" max="5" width="34.453125" style="5" customWidth="1"/>
     <col min="6" max="6" width="34" style="10" customWidth="1"/>
-    <col min="7" max="7" width="31.875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="21.875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="31.90625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="21.90625" style="3" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>308</v>
       </c>
@@ -3128,7 +3139,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3148,7 +3159,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3169,7 +3180,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3190,7 +3201,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3210,7 +3221,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -3230,7 +3241,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -3251,7 +3262,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -3272,7 +3283,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -3293,7 +3304,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -3313,7 +3324,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -3334,7 +3345,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -3354,7 +3365,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -3375,7 +3386,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -3395,7 +3406,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -3415,7 +3426,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -3435,7 +3446,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -3455,7 +3466,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -3476,7 +3487,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -3496,7 +3507,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -3516,7 +3527,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -3536,7 +3547,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -3556,7 +3567,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -3576,7 +3587,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -3596,7 +3607,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -3616,7 +3627,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -3637,7 +3648,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -3658,42 +3669,42 @@
         <v>386</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A28" s="54">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="61">
         <v>26</v>
       </c>
-      <c r="B28" s="54">
+      <c r="B28" s="61">
         <v>46</v>
       </c>
-      <c r="C28" s="58"/>
-      <c r="D28" s="59"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="55"/>
       <c r="E28" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="F28" s="56" t="s">
+      <c r="F28" s="59" t="s">
         <v>387</v>
       </c>
-      <c r="G28" s="55" t="s">
+      <c r="G28" s="58" t="s">
         <v>388</v>
       </c>
       <c r="H28" s="29" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A29" s="54"/>
-      <c r="B29" s="54"/>
-      <c r="C29" s="58"/>
-      <c r="D29" s="59"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="61"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="55"/>
       <c r="E29" s="57"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="55"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="58"/>
       <c r="H29" s="29" t="s">
         <v>706</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A30" s="54"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="61"/>
       <c r="B30" s="7">
         <v>47</v>
       </c>
@@ -3707,7 +3718,7 @@
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>27</v>
       </c>
@@ -3727,7 +3738,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>28</v>
       </c>
@@ -3747,7 +3758,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>29</v>
       </c>
@@ -3768,7 +3779,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>30</v>
       </c>
@@ -3788,7 +3799,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>31</v>
       </c>
@@ -3808,7 +3819,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>32</v>
       </c>
@@ -3828,7 +3839,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>33</v>
       </c>
@@ -3848,7 +3859,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>34</v>
       </c>
@@ -3868,8 +3879,8 @@
         <v>412</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A39" s="54">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="61">
         <v>35</v>
       </c>
       <c r="B39" s="7">
@@ -3888,8 +3899,8 @@
         <v>414</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A40" s="54"/>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="61"/>
       <c r="B40" s="7">
         <v>63</v>
       </c>
@@ -3902,7 +3913,7 @@
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>36</v>
       </c>
@@ -3922,7 +3933,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>37</v>
       </c>
@@ -3942,7 +3953,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>38</v>
       </c>
@@ -3963,7 +3974,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>39</v>
       </c>
@@ -3983,7 +3994,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>40</v>
       </c>
@@ -4003,7 +4014,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>41</v>
       </c>
@@ -4024,7 +4035,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>42</v>
       </c>
@@ -4048,8 +4059,8 @@
         <v>437</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A48" s="54">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="61">
         <v>43</v>
       </c>
       <c r="B48" s="7">
@@ -4064,8 +4075,8 @@
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A49" s="54"/>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="61"/>
       <c r="B49" s="7">
         <v>83</v>
       </c>
@@ -4082,8 +4093,8 @@
         <v>439</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A50" s="54">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="61">
         <v>44</v>
       </c>
       <c r="B50" s="7">
@@ -4102,8 +4113,8 @@
         <v>441</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A51" s="54"/>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="61"/>
       <c r="B51" s="7">
         <v>725</v>
       </c>
@@ -4120,7 +4131,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>45</v>
       </c>
@@ -4140,41 +4151,41 @@
         <v>444</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A53" s="54">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="61">
         <v>46</v>
       </c>
-      <c r="B53" s="54">
+      <c r="B53" s="61">
         <v>90</v>
       </c>
-      <c r="C53" s="58"/>
+      <c r="C53" s="56"/>
       <c r="D53" s="60"/>
       <c r="E53" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="F53" s="56" t="s">
+      <c r="F53" s="59" t="s">
         <v>445</v>
       </c>
-      <c r="G53" s="55" t="s">
+      <c r="G53" s="58" t="s">
         <v>448</v>
       </c>
       <c r="H53" s="10" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A54" s="54"/>
-      <c r="B54" s="54"/>
-      <c r="C54" s="58"/>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="61"/>
+      <c r="B54" s="61"/>
+      <c r="C54" s="56"/>
       <c r="D54" s="60"/>
       <c r="E54" s="57"/>
-      <c r="F54" s="56"/>
-      <c r="G54" s="55"/>
+      <c r="F54" s="59"/>
+      <c r="G54" s="58"/>
       <c r="H54" s="10" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>47</v>
       </c>
@@ -4194,37 +4205,37 @@
         <v>452</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
-      <c r="B56" s="54">
+      <c r="B56" s="61">
         <v>92</v>
       </c>
       <c r="E56" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="F56" s="56" t="s">
+      <c r="F56" s="59" t="s">
         <v>447</v>
       </c>
-      <c r="G56" s="55" t="s">
+      <c r="G56" s="58" t="s">
         <v>453</v>
       </c>
       <c r="H56" s="10" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>48</v>
       </c>
-      <c r="B57" s="54"/>
+      <c r="B57" s="61"/>
       <c r="E57" s="57"/>
-      <c r="F57" s="56"/>
-      <c r="G57" s="55"/>
+      <c r="F57" s="59"/>
+      <c r="G57" s="58"/>
       <c r="H57" s="10" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>49</v>
       </c>
@@ -4244,7 +4255,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>50</v>
       </c>
@@ -4266,7 +4277,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>51</v>
       </c>
@@ -4286,7 +4297,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>52</v>
       </c>
@@ -4306,7 +4317,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>53</v>
       </c>
@@ -4326,37 +4337,37 @@
         <v>470</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A63" s="54">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="61">
         <v>54</v>
       </c>
-      <c r="B63" s="54">
+      <c r="B63" s="61">
         <v>102</v>
       </c>
       <c r="E63" s="57" t="s">
         <v>713</v>
       </c>
-      <c r="F63" s="56" t="s">
+      <c r="F63" s="59" t="s">
         <v>467</v>
       </c>
-      <c r="G63" s="55" t="s">
+      <c r="G63" s="58" t="s">
         <v>473</v>
       </c>
       <c r="H63" s="9" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A64" s="54"/>
-      <c r="B64" s="54"/>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="61"/>
+      <c r="B64" s="61"/>
       <c r="E64" s="57"/>
-      <c r="F64" s="56"/>
-      <c r="G64" s="55"/>
+      <c r="F64" s="59"/>
+      <c r="G64" s="58"/>
       <c r="H64" s="10" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>55</v>
       </c>
@@ -4376,7 +4387,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>56</v>
       </c>
@@ -4396,7 +4407,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>57</v>
       </c>
@@ -4416,7 +4427,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>58</v>
       </c>
@@ -4436,7 +4447,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>59</v>
       </c>
@@ -4456,7 +4467,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>60</v>
       </c>
@@ -4476,7 +4487,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>60</v>
       </c>
@@ -4496,7 +4507,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>61</v>
       </c>
@@ -4516,8 +4527,8 @@
         <v>560</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A73" s="54">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="61">
         <v>62</v>
       </c>
       <c r="B73" s="7">
@@ -4536,8 +4547,8 @@
         <v>562</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A74" s="54"/>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="61"/>
       <c r="B74" s="7">
         <v>119</v>
       </c>
@@ -4554,7 +4565,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>63</v>
       </c>
@@ -4574,7 +4585,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>64</v>
       </c>
@@ -4594,7 +4605,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>65</v>
       </c>
@@ -4614,7 +4625,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>66</v>
       </c>
@@ -4635,7 +4646,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>67</v>
       </c>
@@ -4656,7 +4667,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>68</v>
       </c>
@@ -4676,7 +4687,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>69</v>
       </c>
@@ -4696,7 +4707,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>70</v>
       </c>
@@ -4716,7 +4727,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>71</v>
       </c>
@@ -4736,7 +4747,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>72</v>
       </c>
@@ -4756,7 +4767,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>73</v>
       </c>
@@ -4776,41 +4787,41 @@
         <v>593</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A86" s="54">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="61">
         <v>74</v>
       </c>
-      <c r="B86" s="54">
+      <c r="B86" s="61">
         <v>148</v>
       </c>
-      <c r="C86" s="58"/>
-      <c r="D86" s="54"/>
+      <c r="C86" s="56"/>
+      <c r="D86" s="61"/>
       <c r="E86" s="57" t="s">
         <v>75</v>
       </c>
-      <c r="F86" s="56" t="s">
+      <c r="F86" s="59" t="s">
         <v>590</v>
       </c>
-      <c r="G86" s="55" t="s">
+      <c r="G86" s="58" t="s">
         <v>597</v>
       </c>
       <c r="H86" s="18" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A87" s="54"/>
-      <c r="B87" s="54"/>
-      <c r="C87" s="58"/>
-      <c r="D87" s="54"/>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="61"/>
+      <c r="B87" s="61"/>
+      <c r="C87" s="56"/>
+      <c r="D87" s="61"/>
       <c r="E87" s="57"/>
-      <c r="F87" s="56"/>
-      <c r="G87" s="55"/>
+      <c r="F87" s="59"/>
+      <c r="G87" s="58"/>
       <c r="H87" s="18" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>75</v>
       </c>
@@ -4830,7 +4841,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>76</v>
       </c>
@@ -4850,7 +4861,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>77</v>
       </c>
@@ -4873,7 +4884,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>78</v>
       </c>
@@ -4893,7 +4904,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>79</v>
       </c>
@@ -4913,7 +4924,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>80</v>
       </c>
@@ -4936,7 +4947,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>81</v>
       </c>
@@ -4957,7 +4968,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>82</v>
       </c>
@@ -4978,41 +4989,41 @@
         <v>621</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A96" s="54">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="61">
         <v>83</v>
       </c>
-      <c r="B96" s="54">
+      <c r="B96" s="61">
         <v>179</v>
       </c>
-      <c r="C96" s="58"/>
-      <c r="D96" s="54"/>
+      <c r="C96" s="56"/>
+      <c r="D96" s="61"/>
       <c r="E96" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="F96" s="56" t="s">
+      <c r="F96" s="59" t="s">
         <v>617</v>
       </c>
-      <c r="G96" s="55" t="s">
+      <c r="G96" s="58" t="s">
         <v>622</v>
       </c>
       <c r="H96" s="18" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A97" s="54"/>
-      <c r="B97" s="54"/>
-      <c r="C97" s="58"/>
-      <c r="D97" s="54"/>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="61"/>
+      <c r="B97" s="61"/>
+      <c r="C97" s="56"/>
+      <c r="D97" s="61"/>
       <c r="E97" s="57"/>
-      <c r="F97" s="56"/>
-      <c r="G97" s="55"/>
+      <c r="F97" s="59"/>
+      <c r="G97" s="58"/>
       <c r="H97" s="18" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>84</v>
       </c>
@@ -5032,7 +5043,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>85</v>
       </c>
@@ -5052,7 +5063,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>86</v>
       </c>
@@ -5072,7 +5083,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>87</v>
       </c>
@@ -5092,7 +5103,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>88</v>
       </c>
@@ -5112,7 +5123,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>89</v>
       </c>
@@ -5133,7 +5144,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>90</v>
       </c>
@@ -5153,7 +5164,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>91</v>
       </c>
@@ -5173,7 +5184,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>92</v>
       </c>
@@ -5193,7 +5204,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>93</v>
       </c>
@@ -5213,7 +5224,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>94</v>
       </c>
@@ -5233,7 +5244,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>95</v>
       </c>
@@ -5253,7 +5264,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>96</v>
       </c>
@@ -5276,8 +5287,8 @@
         <v>666</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A111" s="54">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="61">
         <v>97</v>
       </c>
       <c r="B111" s="7">
@@ -5297,8 +5308,8 @@
         <v>671</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A112" s="54"/>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="61"/>
       <c r="B112" s="7">
         <v>224</v>
       </c>
@@ -5316,7 +5327,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>98</v>
       </c>
@@ -5339,7 +5350,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>99</v>
       </c>
@@ -5362,7 +5373,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>100</v>
       </c>
@@ -5382,7 +5393,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>101</v>
       </c>
@@ -5405,7 +5416,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>102</v>
       </c>
@@ -5428,7 +5439,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>103</v>
       </c>
@@ -5448,7 +5459,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>104</v>
       </c>
@@ -5462,8 +5473,8 @@
         <v>104</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A120" s="54">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" s="61">
         <v>105</v>
       </c>
       <c r="B120" s="7">
@@ -5476,8 +5487,8 @@
         <v>106</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A121" s="54"/>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" s="61"/>
       <c r="B121" s="7">
         <v>240</v>
       </c>
@@ -5488,7 +5499,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>106</v>
       </c>
@@ -5502,7 +5513,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>107</v>
       </c>
@@ -5517,7 +5528,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>108</v>
       </c>
@@ -5532,7 +5543,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>109</v>
       </c>
@@ -5546,7 +5557,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>110</v>
       </c>
@@ -5560,7 +5571,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>111</v>
       </c>
@@ -5574,7 +5585,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>112</v>
       </c>
@@ -5588,7 +5599,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>113</v>
       </c>
@@ -5602,7 +5613,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>114</v>
       </c>
@@ -5617,7 +5628,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>115</v>
       </c>
@@ -5631,7 +5642,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>116</v>
       </c>
@@ -5646,7 +5657,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>117</v>
       </c>
@@ -5660,7 +5671,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>118</v>
       </c>
@@ -5674,8 +5685,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A135" s="54">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="61">
         <v>119</v>
       </c>
       <c r="B135" s="7">
@@ -5688,8 +5699,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A136" s="54"/>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="61"/>
       <c r="B136" s="7">
         <v>337</v>
       </c>
@@ -5700,7 +5711,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>120</v>
       </c>
@@ -5714,7 +5725,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>121</v>
       </c>
@@ -5728,7 +5739,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>122</v>
       </c>
@@ -5742,7 +5753,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>123</v>
       </c>
@@ -5756,7 +5767,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>124</v>
       </c>
@@ -5770,7 +5781,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>125</v>
       </c>
@@ -5784,7 +5795,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>126</v>
       </c>
@@ -5798,7 +5809,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>127</v>
       </c>
@@ -5812,7 +5823,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>128</v>
       </c>
@@ -5826,7 +5837,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>129</v>
       </c>
@@ -5840,7 +5851,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>130</v>
       </c>
@@ -5854,7 +5865,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>131</v>
       </c>
@@ -5868,7 +5879,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>132</v>
       </c>
@@ -5882,7 +5893,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>133</v>
       </c>
@@ -5896,7 +5907,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>134</v>
       </c>
@@ -5910,7 +5921,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>135</v>
       </c>
@@ -5924,7 +5935,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>136</v>
       </c>
@@ -5938,7 +5949,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>137</v>
       </c>
@@ -5952,7 +5963,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>138</v>
       </c>
@@ -5966,7 +5977,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>139</v>
       </c>
@@ -5980,7 +5991,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>140</v>
       </c>
@@ -5994,7 +6005,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>141</v>
       </c>
@@ -6008,7 +6019,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>142</v>
       </c>
@@ -6022,7 +6033,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>143</v>
       </c>
@@ -6036,7 +6047,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>144</v>
       </c>
@@ -6050,7 +6061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>145</v>
       </c>
@@ -6064,7 +6075,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>146</v>
       </c>
@@ -6078,7 +6089,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>147</v>
       </c>
@@ -6092,7 +6103,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>148</v>
       </c>
@@ -6107,7 +6118,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>149</v>
       </c>
@@ -6121,7 +6132,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>150</v>
       </c>
@@ -6135,7 +6146,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>151</v>
       </c>
@@ -6149,7 +6160,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>152</v>
       </c>
@@ -6163,7 +6174,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>153</v>
       </c>
@@ -6183,7 +6194,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>154</v>
       </c>
@@ -6197,7 +6208,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>155</v>
       </c>
@@ -6217,7 +6228,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>156</v>
       </c>
@@ -6231,7 +6242,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>157</v>
       </c>
@@ -6245,7 +6256,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>158</v>
       </c>
@@ -6259,7 +6270,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>159</v>
       </c>
@@ -6273,7 +6284,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>160</v>
       </c>
@@ -6287,7 +6298,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>161</v>
       </c>
@@ -6301,7 +6312,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>162</v>
       </c>
@@ -6315,7 +6326,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>163</v>
       </c>
@@ -6329,7 +6340,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>164</v>
       </c>
@@ -6343,7 +6354,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>165</v>
       </c>
@@ -6363,7 +6374,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>166</v>
       </c>
@@ -6377,7 +6388,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>167</v>
       </c>
@@ -6391,7 +6402,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>168</v>
       </c>
@@ -6405,7 +6416,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>169</v>
       </c>
@@ -6419,7 +6430,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>170</v>
       </c>
@@ -6433,7 +6444,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>171</v>
       </c>
@@ -6447,7 +6458,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>172</v>
       </c>
@@ -6461,7 +6472,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>173</v>
       </c>
@@ -6475,7 +6486,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>174</v>
       </c>
@@ -6489,7 +6500,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>175</v>
       </c>
@@ -6503,7 +6514,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>176</v>
       </c>
@@ -6517,7 +6528,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <v>177</v>
       </c>
@@ -6531,7 +6542,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>178</v>
       </c>
@@ -6549,7 +6560,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <v>179</v>
       </c>
@@ -6564,7 +6575,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <v>180</v>
       </c>
@@ -6578,7 +6589,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>181</v>
       </c>
@@ -6592,7 +6603,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>182</v>
       </c>
@@ -6606,7 +6617,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <v>183</v>
       </c>
@@ -6620,7 +6631,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>184</v>
       </c>
@@ -6635,7 +6646,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <v>185</v>
       </c>
@@ -6649,7 +6660,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <v>186</v>
       </c>
@@ -6663,7 +6674,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <v>187</v>
       </c>
@@ -6677,7 +6688,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>188</v>
       </c>
@@ -6692,7 +6703,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
         <v>189</v>
       </c>
@@ -6710,7 +6721,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <v>190</v>
       </c>
@@ -6725,7 +6736,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <v>191</v>
       </c>
@@ -6740,7 +6751,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>192</v>
       </c>
@@ -6755,7 +6766,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>193</v>
       </c>
@@ -6769,7 +6780,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>194</v>
       </c>
@@ -6783,7 +6794,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>195</v>
       </c>
@@ -6801,7 +6812,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>196</v>
       </c>
@@ -6815,7 +6826,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>197</v>
       </c>
@@ -6830,7 +6841,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>198</v>
       </c>
@@ -6844,7 +6855,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>199</v>
       </c>
@@ -6858,7 +6869,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>200</v>
       </c>
@@ -6878,7 +6889,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>201</v>
       </c>
@@ -6902,7 +6913,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>202</v>
       </c>
@@ -6916,7 +6927,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>203</v>
       </c>
@@ -6930,7 +6941,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <v>204</v>
       </c>
@@ -6944,13 +6955,14 @@
         <v>299</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>205</v>
       </c>
       <c r="C222" s="13" t="s">
         <v>544</v>
       </c>
+      <c r="D222" s="54"/>
       <c r="E222" s="5" t="s">
         <v>300</v>
       </c>
@@ -6958,7 +6970,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>206</v>
       </c>
@@ -6972,7 +6984,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>207</v>
       </c>
@@ -6986,7 +6998,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <v>208</v>
       </c>
@@ -7000,7 +7012,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="42">
         <v>209</v>
       </c>
@@ -7012,7 +7024,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="46">
         <v>210</v>
       </c>
@@ -7024,7 +7036,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C228" s="13" t="s">
         <v>717</v>
       </c>
@@ -7033,7 +7045,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C229" s="13" t="s">
         <v>719</v>
       </c>
@@ -7042,9 +7054,49 @@
         <v>720</v>
       </c>
     </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C230" s="13" t="s">
+        <v>721</v>
+      </c>
+      <c r="D230" s="54"/>
+      <c r="E230" s="5" t="s">
+        <v>722</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I228" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="44">
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="G86:G87"/>
+    <mergeCell ref="G96:G97"/>
+    <mergeCell ref="F96:F97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="D96:D97"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:B64"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="E56:E57"/>
@@ -7058,37 +7110,6 @@
     <mergeCell ref="F56:F57"/>
     <mergeCell ref="C53:C54"/>
     <mergeCell ref="D53:D54"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="G86:G87"/>
-    <mergeCell ref="G96:G97"/>
-    <mergeCell ref="F96:F97"/>
-    <mergeCell ref="E96:E97"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="E86:E87"/>
-    <mergeCell ref="F86:F87"/>
-    <mergeCell ref="D86:D87"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B56:B57"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>